<commit_message>
Site updated: 2022-05-05 13:39:00
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -34,6 +34,75 @@
     <t>Url</t>
   </si>
   <si>
+    <t>2022-04-26</t>
+  </si>
+  <si>
+    <t>习近平总书记在人大考察调研时发表的重要讲话在同济青年中引发热烈反响</t>
+  </si>
+  <si>
+    <t>JI团委</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5f1erKcqsibl7UsQSFUqNvKdMrRBfmcTuAAsuGBxLkxGPjibhwplt64w3F8Hszj6OoCMfrWjcDC7Ltlcx6mZlcZg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018701&amp;idx=1&amp;sn=71488e5e4e4ec2c3e4495673a8732419&amp;chksm=bd179a148a601302af9ab4c475a3bc82a6ed687fa9c55b199c91f3fa5c706250d4be02c59afd#rd</t>
+  </si>
+  <si>
+    <t>同读团史，寻迹百年 | 争当新长征突击手活动</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_png/5f1erKcqsibkrvCY0S51icF0ENPBGNLdGaoNbibaJmbY7B8z31th0G41x7pw8cYUIgo3rVlmmErPMEcjcccHDaRRg/0?wx_fmt=png</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018701&amp;idx=2&amp;sn=5c383b7fbf8b67c521273d0ebc1b9fa2&amp;chksm=bd179a148a601302acebdc7f9c3c98d7decc6fd457e87d3d83fd67748bce5a1c321bbf400140#rd</t>
+  </si>
+  <si>
+    <t>青年大学习 | 2022年第十期：把青春献给祖国</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5f1erKcqsibnUgnFuheHbcHbjq77E8Ux3dnEtwrhd7mDMHKzz46UJdhmzrX6z9v6byjSbS0WFqd8JPuwvmrYxug/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018701&amp;idx=3&amp;sn=39f35287fa30c2ba2001960f5e93d579&amp;chksm=bd179a148a60130286564f9dbced3800e849e6b24d29086eaf0992c22a4dcea8cce3410a75a6#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018692&amp;idx=1&amp;sn=9a2976ff85b46d962400f45c3e7ac4f2&amp;chksm=bd179a1d8a60130b5edba763ae44a3119a8ac329dc40613a1b07d0935c6ec0e99ababfcd0f3a#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018692&amp;idx=2&amp;sn=cd6b23c0d19a145e188d0562c2af00ad&amp;chksm=bd179a1d8a60130b5b8fc53fa63f22049d6affffe5fecbbc3e3dbadc8132d2f728e8217188c9#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018692&amp;idx=3&amp;sn=74bb4072240771fce9061a7f1910d5f3&amp;chksm=bd179a1d8a60130b5b2cc844a890535dfd182388689129dbf974786adf0eadf5efda3309c526#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018690&amp;idx=1&amp;sn=b0f1c07d154445dfc7ffe43e2a7176ff&amp;chksm=bd179a1b8a60130d2fa07ac241a8c6b1c18ef51f7da81e6cfab3b0995f5c7178ceace6035395#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018690&amp;idx=2&amp;sn=c6d03a5c9ef948a93e515798568c5554&amp;chksm=bd179a1b8a60130de2722b61d032af18161e050e4080b4da7f66471a576b04694d56146259f1#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018690&amp;idx=3&amp;sn=e0f61b0a588ed1f33539507eb59376c0&amp;chksm=bd179a1b8a60130dd87dcbadba8a43b7e3076d7bf0294f049c54d56fd344c19097c9a9d89e31#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018688&amp;idx=1&amp;sn=482e4609640cd943bb4b79ea112be3e2&amp;chksm=bd179a198a60130f83cf6d2257042c4e119667ca464ba12acf1855d8167857fd0a044860203b#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018688&amp;idx=2&amp;sn=221dce6dd496fac8b3a39aae2be6a3d0&amp;chksm=bd179a198a60130f1a180d30b60b957134eb2b65eb52571d1823d56cfd42e8408e4236fae89c#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018688&amp;idx=3&amp;sn=a92104c4ef121b777b5271ee656fc2ab&amp;chksm=bd179a198a60130f3f48210027649e7fcc98a6e28408bf67183ce9dbf9428311548c5b4ffe07#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018686&amp;idx=1&amp;sn=26dcb9b800f249acd36b64dc5bb131ad&amp;chksm=bd179be78a6012f1c4493f504302cb8b88a4aaba0a69e3fc9c5c606fa1b7815638d7c11377d7#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018686&amp;idx=2&amp;sn=8f21c8cc4423543c2a9e6774d048fe77&amp;chksm=bd179be78a6012f1b839aa5a1e260a7ff9122f407e80616cfcdc0a011c20353114007051941c#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018686&amp;idx=3&amp;sn=0e61b61c2895b59746c2a61e3b926cf6&amp;chksm=bd179be78a6012f1c325d0965cfb224c7d4e69fcfd2e11b4dd4c3892239a39af34e412f66269#rd</t>
+  </si>
+  <si>
     <t>2022-04-25</t>
   </si>
   <si>
@@ -119,75 +188,6 @@
   </si>
   <si>
     <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185525&amp;idx=2&amp;sn=f650c5383b8c2407618fc447beeca6cd&amp;chksm=8bfc274dbc8bae5b06e2f695913f8d7f219e11c669541dc01d5bb26e38f3379ad5b933e5929b#rd</t>
-  </si>
-  <si>
-    <t>2022-04-26</t>
-  </si>
-  <si>
-    <t>习近平总书记在人大考察调研时发表的重要讲话在同济青年中引发热烈反响</t>
-  </si>
-  <si>
-    <t>JI团委</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5f1erKcqsibl7UsQSFUqNvKdMrRBfmcTuAAsuGBxLkxGPjibhwplt64w3F8Hszj6OoCMfrWjcDC7Ltlcx6mZlcZg/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018701&amp;idx=1&amp;sn=71488e5e4e4ec2c3e4495673a8732419&amp;chksm=bd179a148a601302af9ab4c475a3bc82a6ed687fa9c55b199c91f3fa5c706250d4be02c59afd#rd</t>
-  </si>
-  <si>
-    <t>同读团史，寻迹百年 | 争当新长征突击手活动</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_png/5f1erKcqsibkrvCY0S51icF0ENPBGNLdGaoNbibaJmbY7B8z31th0G41x7pw8cYUIgo3rVlmmErPMEcjcccHDaRRg/0?wx_fmt=png</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018701&amp;idx=2&amp;sn=5c383b7fbf8b67c521273d0ebc1b9fa2&amp;chksm=bd179a148a601302acebdc7f9c3c98d7decc6fd457e87d3d83fd67748bce5a1c321bbf400140#rd</t>
-  </si>
-  <si>
-    <t>青年大学习 | 2022年第十期：把青春献给祖国</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5f1erKcqsibnUgnFuheHbcHbjq77E8Ux3dnEtwrhd7mDMHKzz46UJdhmzrX6z9v6byjSbS0WFqd8JPuwvmrYxug/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018701&amp;idx=3&amp;sn=39f35287fa30c2ba2001960f5e93d579&amp;chksm=bd179a148a60130286564f9dbced3800e849e6b24d29086eaf0992c22a4dcea8cce3410a75a6#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018692&amp;idx=1&amp;sn=9a2976ff85b46d962400f45c3e7ac4f2&amp;chksm=bd179a1d8a60130b5edba763ae44a3119a8ac329dc40613a1b07d0935c6ec0e99ababfcd0f3a#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018692&amp;idx=2&amp;sn=cd6b23c0d19a145e188d0562c2af00ad&amp;chksm=bd179a1d8a60130b5b8fc53fa63f22049d6affffe5fecbbc3e3dbadc8132d2f728e8217188c9#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018692&amp;idx=3&amp;sn=74bb4072240771fce9061a7f1910d5f3&amp;chksm=bd179a1d8a60130b5b2cc844a890535dfd182388689129dbf974786adf0eadf5efda3309c526#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018690&amp;idx=1&amp;sn=b0f1c07d154445dfc7ffe43e2a7176ff&amp;chksm=bd179a1b8a60130d2fa07ac241a8c6b1c18ef51f7da81e6cfab3b0995f5c7178ceace6035395#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018690&amp;idx=2&amp;sn=c6d03a5c9ef948a93e515798568c5554&amp;chksm=bd179a1b8a60130de2722b61d032af18161e050e4080b4da7f66471a576b04694d56146259f1#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018690&amp;idx=3&amp;sn=e0f61b0a588ed1f33539507eb59376c0&amp;chksm=bd179a1b8a60130dd87dcbadba8a43b7e3076d7bf0294f049c54d56fd344c19097c9a9d89e31#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018688&amp;idx=1&amp;sn=482e4609640cd943bb4b79ea112be3e2&amp;chksm=bd179a198a60130f83cf6d2257042c4e119667ca464ba12acf1855d8167857fd0a044860203b#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018688&amp;idx=2&amp;sn=221dce6dd496fac8b3a39aae2be6a3d0&amp;chksm=bd179a198a60130f1a180d30b60b957134eb2b65eb52571d1823d56cfd42e8408e4236fae89c#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018688&amp;idx=3&amp;sn=a92104c4ef121b777b5271ee656fc2ab&amp;chksm=bd179a198a60130f3f48210027649e7fcc98a6e28408bf67183ce9dbf9428311548c5b4ffe07#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018686&amp;idx=1&amp;sn=26dcb9b800f249acd36b64dc5bb131ad&amp;chksm=bd179be78a6012f1c4493f504302cb8b88a4aaba0a69e3fc9c5c606fa1b7815638d7c11377d7#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018686&amp;idx=2&amp;sn=8f21c8cc4423543c2a9e6774d048fe77&amp;chksm=bd179be78a6012f1b839aa5a1e260a7ff9122f407e80616cfcdc0a011c20353114007051941c#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MjM5MjAyNjIzMA==&amp;mid=2656018686&amp;idx=3&amp;sn=0e61b61c2895b59746c2a61e3b926cf6&amp;chksm=bd179be78a6012f1c325d0965cfb224c7d4e69fcfd2e11b4dd4c3892239a39af34e412f66269#rd</t>
   </si>
 </sst>
 </file>
@@ -197,8 +197,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -224,6 +224,80 @@
       <charset val="0"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -233,7 +307,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,16 +346,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -268,105 +367,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -377,31 +377,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,19 +479,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,127 +557,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,11 +571,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -591,6 +597,35 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -612,29 +647,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -653,168 +668,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1154,7 +1154,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3">
-        <v>1650877867</v>
+        <v>1650988342</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -1206,40 +1206,40 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3">
-        <v>1650271571</v>
+        <v>1650988342</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3">
-        <v>1650271571</v>
+        <v>1650988342</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>16</v>
@@ -1248,418 +1248,418 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3">
-        <v>1650179444</v>
+        <v>1650987645</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3">
-        <v>1650179444</v>
+        <v>1650987645</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3">
-        <v>1650084362</v>
+        <v>1650987645</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3">
-        <v>1650017558</v>
+        <v>1650986793</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3">
-        <v>1650017558</v>
+        <v>1650986793</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3">
-        <v>1650988342</v>
+        <v>1650986793</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3">
-        <v>1650988342</v>
+        <v>1650986147</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3">
-        <v>1650988342</v>
+        <v>1650986147</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3">
-        <v>1650987645</v>
+        <v>1650986147</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3">
-        <v>1650987645</v>
+        <v>1650984490</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3">
-        <v>1650987645</v>
+        <v>1650984490</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="3">
-        <v>1650986793</v>
+        <v>1650984490</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3">
-        <v>1650986793</v>
+        <v>1650877867</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3">
-        <v>1650986793</v>
+        <v>1650271571</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="D18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="3">
-        <v>1650986147</v>
+        <v>1650271571</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="F19" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3">
-        <v>1650986147</v>
+        <v>1650179444</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="3">
-        <v>1650986147</v>
+        <v>1650179444</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="3">
-        <v>1650984490</v>
+        <v>1650084362</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="3">
-        <v>1650984490</v>
+        <v>1650017558</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3">
-        <v>1650984490</v>
+        <v>1650017558</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>57</v>
@@ -1667,6 +1667,9 @@
       <c r="G24" s="4"/>
     </row>
   </sheetData>
+  <sortState ref="A2:F24">
+    <sortCondition ref="B2" descending="1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Site updated: 2022-05-13 21:23:46
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148">
   <si>
     <t>发布编号</t>
   </si>
@@ -34,6 +34,21 @@
     <t>公众号链接</t>
   </si>
   <si>
+    <t>2022-05-13</t>
+  </si>
+  <si>
+    <t>Advising Center 2022夏季值班开始啦！</t>
+  </si>
+  <si>
+    <t>JIAdvisingCenter</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMjWgCnzBljYto7icrPEnHXQC4cy7rNjSd6GKiaD656icFHp9AnswEvkxLjQTNU8xvsYfm9dsCUI1AoeQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484386&amp;idx=1&amp;sn=53e4f39fe1667d350e45971054f395dd&amp;chksm=fbeb945fcc9c1d49c73e66f4c902bda11550bebd2b8c3aa208a47049880bc118d0bbc0958645#rd</t>
+  </si>
+  <si>
     <t>2022-05-10</t>
   </si>
   <si>
@@ -49,6 +64,15 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486223&amp;idx=1&amp;sn=db36fb765b9db906aa0f94614b6d7b8b&amp;chksm=fa3f12b1cd489ba7afd5a19b68e5ea2131296c3ce7475ab1d736aa4f65d65489f02d902af2f4#rd</t>
   </si>
   <si>
+    <t>回顾 | 2022 SU 夏季学期高阶课Workshop</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMh1meUTqmoUql10eOsXhGLdITGosqLDvdhSbiaJ1J3yJbQlBult9LMvZJNiboWabhv5sbcUeCDA6nqQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484363&amp;idx=1&amp;sn=078f19bc982e4d2364b59183cbda6bc2&amp;chksm=fbeb9476cc9c1d6088b799541e50d11c78b5909fb1dce5f6a563385e690a52b8e5dadb85eedd#rd</t>
+  </si>
+  <si>
     <t>2022-05-09</t>
   </si>
   <si>
@@ -61,9 +85,33 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486202&amp;idx=1&amp;sn=15f8515fdd5eb4e37e92ac0c472ab9ea&amp;chksm=fa3f1344cd489a528a1327d07214775677408fe41a33b39ec489e87ec61011c8cc68254e96fe#rd</t>
   </si>
   <si>
+    <t>JI Science｜浅谈卷积神经网络剪枝</t>
+  </si>
+  <si>
+    <t>密院科协</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWnZ7vX7YChza3GmCdIpXKj27x4O0woo44ib6icNmmn0mkDXTpUcAzlL1tuJibNF1mYJT1tQicVcaYRc9Q/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488220&amp;idx=1&amp;sn=9e8b911d5e8c63dcdddc83406e0f9e32&amp;chksm=97d0fc6ba0a7757d9a7af76790df233439763819589492f842798e21e6f119870826e0f641f6#rd</t>
+  </si>
+  <si>
     <t>2022-05-08</t>
   </si>
   <si>
+    <t>GDP × 保研workshop预告+预热系列之GDP项目专访</t>
+  </si>
+  <si>
+    <t>JIcareer</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moQ2PH5YeuJPgYpFv3BTia9hadiaicr4Vg38fj1lwKob4zuicY5qENleTMCiakoRaibvgl6UkN5yE9HOtbMA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491670&amp;idx=1&amp;sn=c1323727d8529c2e627a9130165052c3&amp;chksm=ec0e0947db7980518ce7fb1e26e3ac06f636d3cfe2e7997ef7abf032b47ea586f2b25dcca847#rd</t>
+  </si>
+  <si>
     <t>上海交通大学密西根学院学生会第十七届主席团候选团队公示</t>
   </si>
   <si>
@@ -76,21 +124,18 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185652&amp;idx=1&amp;sn=46e290b80311a189bf74761a80dd671f&amp;chksm=8bfc27ccbc8baedaeece4553f1e6c995cf9fb7dcbc51762dd9bb449091fe0ace68ba4e189cff#rd</t>
   </si>
   <si>
-    <t>GDP × 保研workshop预告+预热系列之GDP项目专访</t>
-  </si>
-  <si>
-    <t>JIcareer</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moQ2PH5YeuJPgYpFv3BTia9hadiaicr4Vg38fj1lwKob4zuicY5qENleTMCiakoRaibvgl6UkN5yE9HOtbMA/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491670&amp;idx=1&amp;sn=c1323727d8529c2e627a9130165052c3&amp;chksm=ec0e0947db7980518ce7fb1e26e3ac06f636d3cfe2e7997ef7abf032b47ea586f2b25dcca847#rd</t>
-  </si>
-  <si>
     <t>2022-05-07</t>
   </si>
   <si>
+    <t>学术招聘 | Multiple Ph.D. and Research Internship Openings</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moRe9EsZQXWBFwwU14TXxQmxHicjHCM7NaVibYkEnGWM1vUzNYicadmjHYgOjCnmXEh8sOMW72CAajXOg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491638&amp;idx=1&amp;sn=ca7d0f32349e0b6970c2c9d2ce14d863&amp;chksm=ec0e0927db798031c8174d64f850c457cf8aa8854795845d896a2366c36ba4cd2fb8fc2e4223#rd</t>
+  </si>
+  <si>
     <t>社体部 | 2022 密院杯英雄联盟圆满结束啦！</t>
   </si>
   <si>
@@ -100,18 +145,18 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185649&amp;idx=1&amp;sn=a782a9ada7f18a729007a59c756a4344&amp;chksm=8bfc27c9bc8baedf4138fcf0930f900eec2e1799dd803db91e844a49316af517d3cda8b80e21#rd</t>
   </si>
   <si>
-    <t>学术招聘 | Multiple Ph.D. and Research Internship Openings</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moRe9EsZQXWBFwwU14TXxQmxHicjHCM7NaVibYkEnGWM1vUzNYicadmjHYgOjCnmXEh8sOMW72CAajXOg/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491638&amp;idx=1&amp;sn=ca7d0f32349e0b6970c2c9d2ce14d863&amp;chksm=ec0e0927db798031c8174d64f850c457cf8aa8854795845d896a2366c36ba4cd2fb8fc2e4223#rd</t>
-  </si>
-  <si>
     <t>2022-05-06</t>
   </si>
   <si>
+    <t>2022 SU 夏季学期高阶课Workshop</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMiaOw0xZPvwT9sNvxmzSr6Pwv7HM5oGZM9hib0Dc5EuGzicIxfH6kKHxk5OQO0uNKY0D4aqQIkyNKzPw/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484343&amp;idx=1&amp;sn=5d6a9c8d05bd283af59317f9d51f450b&amp;chksm=fbeb940acc9c1d1cd6924f088a6b38cfed82ac1b7ac2cdc407c2a956fe33e65338f8ce26443f#rd</t>
+  </si>
+  <si>
     <t>文艺部 | Echoism 线上歌会倒计时</t>
   </si>
   <si>
@@ -130,6 +175,21 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486185&amp;idx=1&amp;sn=c64eeec3346165d5829cde1f61f4adca&amp;chksm=fa3f1357cd489a41ec0c01b809e0a927a2c0f5dada0dc88b1047f82f6f2fc35fc7f33bde445b#rd</t>
   </si>
   <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486182&amp;idx=1&amp;sn=72e51b4720009f9afef0c7d51fb692ff&amp;chksm=fa3f1358cd489a4e0a6f6e2aa1443c3a2be49eacb75df3bc656cafa6afc75bd79b1e2e236716#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486173&amp;idx=1&amp;sn=6ecdbacb97830fad0b757ce3b426e3c3&amp;chksm=fa3f1363cd489a7572205cb63ed1f80c34081f6fe7e49085756f9cd02555a09218933a6ad3b6#rd</t>
+  </si>
+  <si>
+    <t>赛事相关 | E创 | 咱就是说，极客派对x创意工坊一整个爱住了</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWmXibAdwXQ75yr5DCxiaVkfxD8ia9ZthibXT2uLQ2PaX7xHldBuDMpjHwMPdXqDTHgmO4cAxXkVZibmgFg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488207&amp;idx=1&amp;sn=1953baf8cc4aad31e0d8a79a8105e3df&amp;chksm=97d0fc78a0a7756ee8e506311d88f0361953267b91db390e44655440abf5d2b5502cd4850ef6#rd</t>
+  </si>
+  <si>
     <t>2022-05-05</t>
   </si>
   <si>
@@ -145,6 +205,24 @@
     <t>2022-05-04</t>
   </si>
   <si>
+    <t>百年风雨路，青春勇担当！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWnj8zwbJgnCyIS573w0WOreDvzkmrCOcHNZmDj9sFBVp5CyHyHJqjE8gNgCYYOAWIaDuMmxaZlB1Q/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488188&amp;idx=1&amp;sn=7bdb958cacbe58eef2a86d3951977b3c&amp;chksm=97d0fc0ba0a7751d5fb928108bea1a2b6a11a19112a12c582c04fb46e0c554034dce037efe1a#rd</t>
+  </si>
+  <si>
+    <t>事业部Piazza | 期待你的加入！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moTpusu5p5xibiaddAlkR3IVyyEQA6kRK9I6UaUS5Bh4W76qicBQ42ibUAGIMjcDWzU3hfeia0e3hKYN7YA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491595&amp;idx=1&amp;sn=f69986ee829561de050049d016718a05&amp;chksm=ec0e091adb79800c6376087fb6e78975c64c4c4bb7dca96d6adb9b7e1e5347ed959259424738#rd</t>
+  </si>
+  <si>
     <t>庆祝中国共产主义青年团成立100周年！</t>
   </si>
   <si>
@@ -154,15 +232,6 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185625&amp;idx=1&amp;sn=d8383126344a73d70f669fdf402cc980&amp;chksm=8bfc27e1bc8baef7c57a15e9ce96a6dc6b19c1a6add98af6eb0d5c89ddefed115e1155e112e5#rd</t>
   </si>
   <si>
-    <t>事业部Piazza | 期待你的加入！</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moTpusu5p5xibiaddAlkR3IVyyEQA6kRK9I6UaUS5Bh4W76qicBQ42ibUAGIMjcDWzU3hfeia0e3hKYN7YA/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491595&amp;idx=1&amp;sn=f69986ee829561de050049d016718a05&amp;chksm=ec0e091adb79800c6376087fb6e78975c64c4c4bb7dca96d6adb9b7e1e5347ed959259424738#rd</t>
-  </si>
-  <si>
     <t>分享图片</t>
   </si>
   <si>
@@ -184,6 +253,15 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486150&amp;idx=1&amp;sn=b3073dee8e7be246e703dd7d56e47d2f&amp;chksm=fa3f1378cd489a6ef3c9f4cbd1358175fe3cc881abb3b4855b78608d10fc786e927d4ef6fbba#rd</t>
   </si>
   <si>
+    <t>回顾 | 2022 SU TA Workshop</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMgKSTr4zstBNBAFr1gMAYtMbuKiahRyEcIW4RT5qtReo10wiczrXDr4zyia255FEovgutgQDXiaaSqZ8Q/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484329&amp;idx=1&amp;sn=086b74915dd33d34ede2cef1f4adf534&amp;chksm=fbeb9414cc9c1d024b5cb0455b4ba3d568223d3de7ce1d6f7974c75e8ad0c32aebea745f33f3#rd</t>
+  </si>
+  <si>
     <t>2022-05-02</t>
   </si>
   <si>
@@ -196,9 +274,27 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486142&amp;idx=1&amp;sn=ed082adade2cdf25de03ccae4b803cf1&amp;chksm=fa3f1300cd489a161734868acb63db53aee2a3f4eeb346a1ffd75423b4c82b5fa9dff2af3d97#rd</t>
   </si>
   <si>
+    <t>赛事相关 | 2022年度上海交通大学“数学建模培训营”国赛招生通知</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWnKzHPNfCK5SXsZUJR24vicm38H5shbxicaB2l8CaeuAC0eOOkib0cVcuic9licP14Yq0eejJDITwlx1ug/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488176&amp;idx=1&amp;sn=e5ac653e3bb798e01e7808af0c448c91&amp;chksm=97d0fc07a0a77511c146ac371336b4676e6f16c6004a5427da0629b64a131df9c82fd5dbddd7#rd</t>
+  </si>
+  <si>
     <t>2022-04-30</t>
   </si>
   <si>
+    <t>觅源青志队部长团换届通知</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5RXNeQ7icPqEAeaG8jVkjicInqsxw39TslNB2B5aEsh7QJZQtgVZVicv9vaWXC8BC30jh4eaWZwJArmA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzAwNTYxNzk3Mw==&amp;mid=2648011540&amp;idx=1&amp;sn=f1bd1d93df35cc1f5bd1a3b24d254904&amp;chksm=8338334eb44fba58f1b21c0608de25aaef4dcf110b9d74f410b867eeed2291e04851791f534f#rd</t>
+  </si>
+  <si>
     <t>聚焦 | 做好斗图准备了吗？密院“顶流”蓝虎表情包第二期上线，赶紧收藏起来吧！</t>
   </si>
   <si>
@@ -208,13 +304,13 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185612&amp;idx=1&amp;sn=e423fafa1c7d1f3f71996e26df150d7e&amp;chksm=8bfc27f4bc8baee2bae234df36b435792d4f9901f0ba3b6f4228f11dcf069dd2e8f7392723bf#rd</t>
   </si>
   <si>
-    <t>觅源青志队部长团换届通知</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5RXNeQ7icPqEAeaG8jVkjicInqsxw39TslNB2B5aEsh7QJZQtgVZVicv9vaWXC8BC30jh4eaWZwJArmA/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzAwNTYxNzk3Mw==&amp;mid=2648011540&amp;idx=1&amp;sn=f1bd1d93df35cc1f5bd1a3b24d254904&amp;chksm=8338334eb44fba58f1b21c0608de25aaef4dcf110b9d74f410b867eeed2291e04851791f534f#rd</t>
+    <t>TA Workshop 2022 SU - 夏季学期助教分享会</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMgpVObYRaNXH7VxUvulxiaPG8xKdZ3sgD9WH5dQoXicaC8WmAKqaKNRyWUlxWFiamnhksxN7zEprUoAw/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484216&amp;idx=1&amp;sn=b338159a1ee1a6f4c224fcec3d3b21e3&amp;chksm=fbeb9485cc9c1d93aee62ad2eb0f654416f7f87e422aecd496dcf4941c4ac331972a55918444#rd</t>
   </si>
   <si>
     <t>2022-04-27</t>
@@ -278,6 +374,18 @@
   </si>
   <si>
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486093&amp;idx=1&amp;sn=d20cb7fbe6a7d64e0fd3c14c37a7a0ac&amp;chksm=fa3f1333cd489a25f1417672d98276aff3759c79a46685db68840edbb3d6237c898977f483a7#rd</t>
+  </si>
+  <si>
+    <t>2022-04-23</t>
+  </si>
+  <si>
+    <t>JI Science ｜Introduction to BCI</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWnGvm6FRmx8mdEgbdBIRK6TRtbaGib0s3NlhFnClKicibKCVszj8oIDRqwBk1fibTqHjgWXPCX070qaSw/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488169&amp;idx=1&amp;sn=1133f5b38631f2102db5049688e9d37c&amp;chksm=97d0fc1ea0a77508fde997f84c701122f97a363debb796eaaaf38406a22bd93a328df78491ba#rd</t>
   </si>
   <si>
     <t>2022-04-19</t>
@@ -357,12 +465,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,17 +485,9 @@
       <charset val="0"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -401,6 +501,14 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -408,9 +516,83 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -425,90 +607,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -521,9 +621,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -538,31 +638,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,13 +782,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,7 +806,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,121 +818,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,21 +829,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -771,37 +856,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -823,9 +882,50 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -834,157 +934,156 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1304,13 +1403,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="11.9765625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -1334,7 +1436,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>1652196254</v>
+        <v>1652423986</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1354,7 +1456,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>1652102252</v>
+        <v>1652196254</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -1363,207 +1465,207 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>1651989033</v>
+        <v>1652156920</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>1652004475</v>
+        <v>1652102252</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>1651902344</v>
+        <v>1652082724</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>1651923024</v>
+        <v>1652004475</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>1651834564</v>
+        <v>1651989033</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>1651827827</v>
+        <v>1651923024</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>1651730520</v>
+        <v>1651902344</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>1651646933</v>
+        <v>1651834916</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1">
-        <v>1651654866</v>
+        <v>1651834564</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1">
-        <v>1651644769</v>
+        <v>1651827827</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>51</v>
@@ -1574,329 +1676,565 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1">
-        <v>1651634414</v>
+        <v>1651827003</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1">
-        <v>1651499797</v>
+        <v>1651826605</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1">
-        <v>1651312543</v>
+        <v>1651820943</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>1651323746</v>
+        <v>1651730520</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>1651045196</v>
+        <v>1651659154</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>1651038505</v>
+        <v>1651654866</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>1651029491</v>
+        <v>1651646933</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>1650938536</v>
+        <v>1651644769</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>1650877867</v>
+        <v>1651634414</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>1650852390</v>
+        <v>1651633116</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
-        <v>1650355221</v>
+        <v>1651499797</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
-        <v>1650113970</v>
+        <v>1651487681</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>1649752200</v>
+        <v>1651323746</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>1649474737</v>
+        <v>1651312543</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>1648656738</v>
+        <v>1651295846</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
+        <v>1651045196</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
+        <v>1651038505</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1">
+        <v>1651029491</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1">
+        <v>1650938536</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1">
+        <v>1650877867</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1">
+        <v>1650852390</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1">
+        <v>1650701590</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1">
+        <v>1650355221</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
+        <v>1650113970</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1">
+        <v>1649752200</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1">
+        <v>1649474737</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1">
+        <v>1648656738</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1">
         <v>1648381501</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>111</v>
+      <c r="B41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" display="https://mmbiz.qlogo.cn/mmbiz_png/QfDapvG9u4DMj1WoP0ODbssa94NEKOS2uYX0CsZmdmjujUSYLMG1Ib0IotFv8A9IWGdpvuOGP8qOU9uPJmicKkw/0?wx_fmt=png"/>
-    <hyperlink ref="F9" r:id="rId2" display="http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486185&amp;idx=1&amp;sn=c64eeec3346165d5829cde1f61f4adca&amp;chksm=fa3f1357cd489a41ec0c01b809e0a927a2c0f5dada0dc88b1047f82f6f2fc35fc7f33bde445b#rd"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Site updated: 2022-05-14 19:47:33
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152">
   <si>
     <t>发布编号</t>
   </si>
@@ -34,6 +34,21 @@
     <t>公众号链接</t>
   </si>
   <si>
+    <t>2022-05-14</t>
+  </si>
+  <si>
+    <t>通知 | 关于组织开展“我的入团故事”主题征文活动的通知</t>
+  </si>
+  <si>
+    <t>JI青团</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4CdnRBr6OVoXeiaDIy2TKKHsll4IV7iaPX3tMPZpib0lD9kU80ndLq6erU5GUHnSp9JHYZdYM1NFc2SQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486232&amp;idx=1&amp;sn=11c57e492f04a420e99be69698e4f338&amp;chksm=fa3f12a6cd489bb034cf91791191f8298e6cffe04d1b2c5d969301a3f48b34a999451d2cf2c2#rd</t>
+  </si>
+  <si>
     <t>2022-05-13</t>
   </si>
   <si>
@@ -53,9 +68,6 @@
   </si>
   <si>
     <t>密西根学院青年热议习近平总书记在建团百年庆祝大会上的讲话</t>
-  </si>
-  <si>
-    <t>JI青团</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_png/QfDapvG9u4A3DpOJFqZjvyQSFw2O8xwZLTEQzwxxljD77o9lGlShLxbFRaKPmHwiatKDo3hTzzOj4mSw066tG5Q/0?wx_fmt=png</t>
@@ -465,9 +477,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -485,9 +497,41 @@
       <charset val="0"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -500,24 +544,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -531,15 +567,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -560,24 +596,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -591,39 +626,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -638,61 +650,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,121 +824,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -829,65 +841,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -909,8 +862,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -929,153 +912,182 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1403,16 +1415,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
-  <cols>
-    <col min="1" max="1" width="11.9765625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -1436,7 +1445,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>1652423986</v>
+        <v>1652502015</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1456,7 +1465,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>1652196254</v>
+        <v>1652423986</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -1476,30 +1485,30 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>1652156920</v>
+        <v>1652196254</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>1652102252</v>
+        <v>1652156920</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
@@ -1516,16 +1525,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>1652082724</v>
+        <v>1652102252</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>25</v>
@@ -1536,30 +1545,30 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>1652004475</v>
+        <v>1652082724</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>1651989033</v>
+        <v>1652004475</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1576,16 +1585,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>1651923024</v>
+        <v>1651989033</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>38</v>
@@ -1596,36 +1605,36 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>1651902344</v>
+        <v>1651923024</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>1651834916</v>
+        <v>1651902344</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>45</v>
@@ -1636,116 +1645,116 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1">
-        <v>1651834564</v>
+        <v>1651834916</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1">
-        <v>1651827827</v>
+        <v>1651834564</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1">
-        <v>1651827003</v>
+        <v>1651827827</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1">
-        <v>1651826605</v>
+        <v>1651827003</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1">
-        <v>1651820943</v>
+        <v>1651826605</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>1651730520</v>
+        <v>1651820943</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>60</v>
@@ -1756,7 +1765,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>1651659154</v>
+        <v>1651730520</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>62</v>
@@ -1765,7 +1774,7 @@
         <v>63</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>64</v>
@@ -1776,56 +1785,56 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>1651654866</v>
+        <v>1651659154</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>1651646933</v>
+        <v>1651654866</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>1651644769</v>
+        <v>1651646933</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>74</v>
@@ -1836,50 +1845,50 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>1651634414</v>
+        <v>1651644769</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>1651633116</v>
+        <v>1651634414</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
-        <v>1651499797</v>
+        <v>1651633116</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>83</v>
@@ -1896,36 +1905,36 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
-        <v>1651487681</v>
+        <v>1651499797</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>1651323746</v>
+        <v>1651487681</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>90</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>91</v>
@@ -1936,56 +1945,56 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>1651312543</v>
+        <v>1651323746</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>1651295846</v>
+        <v>1651312543</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>1651045196</v>
+        <v>1651295846</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>100</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>101</v>
@@ -1996,56 +2005,56 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1">
-        <v>1651038505</v>
+        <v>1651045196</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
-        <v>1651029491</v>
+        <v>1651038505</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1">
-        <v>1650938536</v>
+        <v>1651029491</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>110</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>111</v>
@@ -2056,7 +2065,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1">
-        <v>1650877867</v>
+        <v>1650938536</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>113</v>
@@ -2065,7 +2074,7 @@
         <v>114</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>115</v>
@@ -2076,36 +2085,36 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>1650852390</v>
+        <v>1650877867</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>1650701590</v>
+        <v>1650852390</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>121</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>122</v>
@@ -2116,7 +2125,7 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1">
-        <v>1650355221</v>
+        <v>1650701590</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>124</v>
@@ -2125,7 +2134,7 @@
         <v>125</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>126</v>
@@ -2136,7 +2145,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1">
-        <v>1650113970</v>
+        <v>1650355221</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>128</v>
@@ -2145,7 +2154,7 @@
         <v>129</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>130</v>
@@ -2156,7 +2165,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1">
-        <v>1649752200</v>
+        <v>1650113970</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>132</v>
@@ -2165,7 +2174,7 @@
         <v>133</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>134</v>
@@ -2176,7 +2185,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1">
-        <v>1649474737</v>
+        <v>1649752200</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>136</v>
@@ -2185,7 +2194,7 @@
         <v>137</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>138</v>
@@ -2196,7 +2205,7 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1">
-        <v>1648656738</v>
+        <v>1649474737</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>140</v>
@@ -2205,7 +2214,7 @@
         <v>141</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>142</v>
@@ -2216,7 +2225,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1">
-        <v>1648381501</v>
+        <v>1648656738</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>144</v>
@@ -2225,13 +2234,33 @@
         <v>145</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>146</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1">
+        <v>1648381501</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2022-05-15 21:54:05
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -493,13 +493,20 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
       <charset val="0"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -522,7 +529,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -530,24 +537,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -559,8 +552,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -575,7 +583,29 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -590,7 +620,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -602,44 +639,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -656,181 +655,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,6 +840,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -863,7 +873,31 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -879,21 +913,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -916,28 +935,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -946,142 +945,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">

</xml_diff>

<commit_message>
Site updated: 2022-05-15 22:04:08
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -34,7 +34,7 @@
     <t>公众号链接</t>
   </si>
   <si>
-    <t>2022-05-14</t>
+    <t>2022-05-15</t>
   </si>
   <si>
     <t>通知 | 关于组织开展“我的入团故事”主题征文活动的通知</t>
@@ -478,8 +478,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -498,13 +498,12 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -512,24 +511,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -537,7 +527,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -554,6 +544,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -561,14 +567,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -582,16 +581,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -604,21 +617,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -626,15 +624,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -649,25 +649,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -679,13 +787,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -697,67 +811,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -769,67 +829,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -845,10 +845,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -873,16 +871,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -902,17 +906,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -934,9 +932,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -945,118 +945,118 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1065,36 +1065,37 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1417,7 +1418,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F42"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1446,7 +1447,7 @@
       <c r="A2" s="1">
         <v>1652502015</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">

</xml_diff>

<commit_message>
Site updated: 2022-05-16 20:35:50
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156">
   <si>
     <t>发布编号</t>
   </si>
@@ -34,7 +34,22 @@
     <t>公众号链接</t>
   </si>
   <si>
-    <t>2022-05-15</t>
+    <t>2022-05-16</t>
+  </si>
+  <si>
+    <t>密西根学院学生会第十七届主席团候选人介绍</t>
+  </si>
+  <si>
+    <t>JIers</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNElgCAbsgr0A563icfX50g1XQZlITuIuaMTyianUCkxAm0zib4mHicAmEK1oiciaEnDfXv0DickKfUib6YhtA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185670&amp;idx=1&amp;sn=08acd02cf1fb3dfc6231d1892cf9fe79&amp;chksm=8bfc243ebc8bad28a1898210c6bdd7f34f16497df1ced5611ea2468f6e9c91300cd208c2b442#rd</t>
+  </si>
+  <si>
+    <t>2022-05-14</t>
   </si>
   <si>
     <t>通知 | 关于组织开展“我的入团故事”主题征文活动的通知</t>
@@ -125,9 +140,6 @@
   </si>
   <si>
     <t>上海交通大学密西根学院学生会第十七届主席团候选团队公示</t>
-  </si>
-  <si>
-    <t>JIers</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNGM1FaFYoiar2my7XBXG3m37zwL1hdu9Q5C6cGIAX6rKEr3aBYKfkZ8luyVibBicCnIkU5RgLtGQicibfw/0?wx_fmt=jpeg</t>
@@ -477,10 +489,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -493,12 +505,20 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="0"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -511,8 +531,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -544,7 +588,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -552,22 +603,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -582,36 +625,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -624,9 +638,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -649,37 +662,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -691,13 +776,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,19 +806,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -733,103 +842,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -840,15 +853,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -871,7 +875,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -887,6 +891,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -929,173 +953,161 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1415,10 +1427,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A1" sqref="A1:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1445,9 +1457,9 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>1652502015</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>1652633146</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1465,7 +1477,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>1652423986</v>
+        <v>1652502015</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -1485,7 +1497,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>1652196254</v>
+        <v>1652423986</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
@@ -1494,81 +1506,81 @@
         <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>1652156920</v>
+        <v>1652196254</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>1652102252</v>
+        <v>1652156920</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>1652082724</v>
+        <v>1652102252</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>1652004475</v>
+        <v>1652082724</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1585,36 +1597,36 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>1651989033</v>
+        <v>1652004475</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>1651923024</v>
+        <v>1651989033</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>42</v>
@@ -1625,36 +1637,36 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>1651902344</v>
+        <v>1651923024</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1">
-        <v>1651834916</v>
+        <v>1651902344</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>49</v>
@@ -1665,116 +1677,116 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1">
-        <v>1651834564</v>
+        <v>1651834916</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1">
-        <v>1651827827</v>
+        <v>1651834564</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1">
-        <v>1651827003</v>
+        <v>1651827827</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1">
-        <v>1651826605</v>
+        <v>1651827003</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>1651820943</v>
+        <v>1651826605</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>1651730520</v>
+        <v>1651820943</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>64</v>
@@ -1785,7 +1797,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>1651659154</v>
+        <v>1651730520</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>66</v>
@@ -1794,7 +1806,7 @@
         <v>67</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>68</v>
@@ -1805,56 +1817,56 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>1651654866</v>
+        <v>1651659154</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>1651646933</v>
+        <v>1651654866</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>1651644769</v>
+        <v>1651646933</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>78</v>
@@ -1865,56 +1877,56 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>1651634414</v>
+        <v>1651644769</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
-        <v>1651633116</v>
+        <v>1651634414</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
-        <v>1651499797</v>
+        <v>1651633116</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>88</v>
@@ -1925,36 +1937,36 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>1651487681</v>
+        <v>1651499797</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>1651323746</v>
+        <v>1651487681</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>95</v>
@@ -1965,56 +1977,56 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>1651312543</v>
+        <v>1651323746</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>1651295846</v>
+        <v>1651312543</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1">
-        <v>1651045196</v>
+        <v>1651295846</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>105</v>
@@ -2025,56 +2037,56 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
-        <v>1651038505</v>
+        <v>1651045196</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1">
-        <v>1651029491</v>
+        <v>1651038505</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1">
-        <v>1650938536</v>
+        <v>1651029491</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>115</v>
@@ -2085,7 +2097,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>1650877867</v>
+        <v>1650938536</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>117</v>
@@ -2094,7 +2106,7 @@
         <v>118</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>119</v>
@@ -2105,36 +2117,36 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>1650852390</v>
+        <v>1650877867</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1">
-        <v>1650701590</v>
+        <v>1650852390</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>125</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>126</v>
@@ -2145,7 +2157,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1">
-        <v>1650355221</v>
+        <v>1650701590</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>128</v>
@@ -2165,7 +2177,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1">
-        <v>1650113970</v>
+        <v>1650355221</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>132</v>
@@ -2174,7 +2186,7 @@
         <v>133</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>134</v>
@@ -2185,7 +2197,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1">
-        <v>1649752200</v>
+        <v>1650113970</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>136</v>
@@ -2194,7 +2206,7 @@
         <v>137</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>138</v>
@@ -2205,7 +2217,7 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1">
-        <v>1649474737</v>
+        <v>1649752200</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>140</v>
@@ -2214,7 +2226,7 @@
         <v>141</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>142</v>
@@ -2225,7 +2237,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1">
-        <v>1648656738</v>
+        <v>1649474737</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>144</v>
@@ -2234,7 +2246,7 @@
         <v>145</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>146</v>
@@ -2245,7 +2257,7 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1">
-        <v>1648381501</v>
+        <v>1648656738</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>148</v>
@@ -2254,13 +2266,33 @@
         <v>149</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>150</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="1">
+        <v>1648381501</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2022-05-17 16:37:31
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166">
   <si>
     <t>发布编号</t>
   </si>
@@ -482,6 +482,36 @@
   </si>
   <si>
     <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491470&amp;idx=1&amp;sn=9ae07a89758e30d73f6fe2868ff32be4&amp;chksm=ec0df69fdb7a7f89f3b898050fb3d9546846c42f58021e95e2ff02d40500b14c960e4b83bd7a#rd</t>
+  </si>
+  <si>
+    <t>2022-05-17</t>
+  </si>
+  <si>
+    <t>【招聘】Sophoton | 识光芯科在招岗位</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moSxJYWoqYh7Mcrp4pecJNeJiamkvhgNySd3PIVbsKgPZxBXo2tjcB9FibIF1XMvb6FoogQvdgCgDo2A/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491691&amp;idx=1&amp;sn=70aad1997dc0ba16c809ab3d1e53b883&amp;chksm=ec0e097adb79806cd753c4950d1309b9ad5f8e3c0a65d1a08e98030376caab819132b121ff3c#rd</t>
+  </si>
+  <si>
+    <t>【活动回顾】GDP×保研workshop圆满结束！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moSictu4icWQJwfw0Myibnt9xKLjlv13GbzAt9D2Vp7My36zeOH1cOQAYD4l68OZG638slxbzWuh4liczA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491681&amp;idx=1&amp;sn=9d27cb02f3aacbe6bfd5e8a4a3540e6a&amp;chksm=ec0e0970db798066032ba2bb809e8c29473206ce54164131221d23bbc2a7c1c8907e8f8ab307#rd</t>
+  </si>
+  <si>
+    <t>青年大学习：学习习近平总书记在庆祝中国共产主义青年团成立100周年大会上的重要讲话精神</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4Dib2WjxQn9Bgn5VticgfEfdKibYtX5BQA5zbt9gemyzTrFYp1oOzj1V6MyBUjqsV7mhqrKoCntc8ByQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486248&amp;idx=1&amp;sn=92d251a227a6a0190374ff5a283944af&amp;chksm=fa3f1296cd489b8003c01dfc403cce50dfd33c649544333390b6e15f72e1e3b738b7ef524719#rd</t>
   </si>
 </sst>
 </file>
@@ -489,10 +519,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -505,8 +535,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u/>
@@ -519,21 +548,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -555,8 +569,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -567,22 +589,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -601,6 +607,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,22 +639,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -639,7 +653,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -652,6 +666,21 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -662,25 +691,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,43 +847,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -740,109 +865,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -853,6 +882,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -873,8 +935,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -891,41 +955,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -958,61 +987,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1021,79 +1050,79 @@
     <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1427,10 +1456,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F43"/>
+      <selection activeCell="A1" sqref="A1:F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2295,6 +2324,66 @@
         <v>155</v>
       </c>
     </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="1">
+        <v>1652766746</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="1">
+        <v>1652708097</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="1">
+        <v>1652711615</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2022-05-21 23:30:22
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177">
   <si>
     <t>发布编号</t>
   </si>
@@ -34,15 +34,39 @@
     <t>公众号链接</t>
   </si>
   <si>
+    <t>2022-05-21</t>
+  </si>
+  <si>
+    <t>传媒部 | PPT Workshop 来啦！</t>
+  </si>
+  <si>
+    <t>JIers</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_png/sZvUJ5A0zNHTYUfqzx2ftWEXIwJzUMbfyM6ia03x3IBKrA9x5pj6VGIVQDdd4b2QDtVGgtHRXLwYibl1sX2LhQSA/0?wx_fmt=png</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185715&amp;idx=1&amp;sn=1da14bc3c3eff5415e4a74a75eec20e8&amp;chksm=8bfc240bbc8bad1d0dc99918068aa401798b07a58cc13334f9ac57ce872fb64edda0ae55553f#rd</t>
+  </si>
+  <si>
+    <t>研究生申请&amp;生涯发展经验分享会 | For DDers</t>
+  </si>
+  <si>
+    <t>JIAdvisingCenter</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMjp5FpuKh2hTVSicZnHxaiao3A7xRTBiceQMxoZUw2SICyL6Wt6D1SMeu6ic4CFecmtxkUrOUDZmlQDtQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484409&amp;idx=1&amp;sn=111ff93b1be572196741e31eb291a4e7&amp;chksm=fbeb9444cc9c1d5267e2fafd5a1864f6b9841c5d5205edd85182a9cd48344c9cd2aba1324849#rd</t>
+  </si>
+  <si>
     <t>2022-05-19</t>
   </si>
   <si>
     <t>服务月 |「JIers专属」一站式平台发布</t>
   </si>
   <si>
-    <t>JIers</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_png/sZvUJ5A0zNHRoV6nSVMPOzdC3f6xVmQF0B8OBLohsxx7g34l0M6sbr6y5ic9f0T6w66NoQxSqqo3PXBSUX8HjYw/0?wx_fmt=png</t>
   </si>
   <si>
@@ -113,9 +137,6 @@
   </si>
   <si>
     <t>Advising Center 2022夏季值班开始啦！</t>
-  </si>
-  <si>
-    <t>JIAdvisingCenter</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMjWgCnzBljYto7icrPEnHXQC4cy7rNjSd6GKiaD656icFHp9AnswEvkxLjQTNU8xvsYfm9dsCUI1AoeQ/0?wx_fmt=jpeg</t>
@@ -559,6 +580,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -566,46 +595,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -619,10 +626,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -641,9 +649,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -658,14 +695,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -679,21 +709,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -710,13 +731,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,163 +893,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -900,9 +921,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -912,21 +935,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -956,27 +964,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -995,147 +992,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1469,10 +1490,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F47"/>
+      <selection activeCell="A1" sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1499,7 +1520,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>1652946162</v>
+        <v>1653106699</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1519,56 +1540,56 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>1652766746</v>
+        <v>1653103833</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>1652711615</v>
+        <v>1652946162</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>1652633146</v>
+        <v>1652766746</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>22</v>
@@ -1579,96 +1600,96 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>1652708097</v>
+        <v>1652711615</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>1652502015</v>
+        <v>1652633146</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>1652423986</v>
+        <v>1652708097</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>1652196254</v>
+        <v>1652502015</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>1652156920</v>
+        <v>1652423986</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>41</v>
@@ -1679,7 +1700,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>1652102252</v>
+        <v>1652196254</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>43</v>
@@ -1688,7 +1709,7 @@
         <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>45</v>
@@ -1699,7 +1720,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1">
-        <v>1652082724</v>
+        <v>1652156920</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>43</v>
@@ -1708,47 +1729,47 @@
         <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1">
-        <v>1651989033</v>
+        <v>1652102252</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1">
-        <v>1652004475</v>
+        <v>1652082724</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>56</v>
@@ -1759,7 +1780,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1">
-        <v>1651923024</v>
+        <v>1651989033</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>58</v>
@@ -1768,7 +1789,7 @@
         <v>59</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>60</v>
@@ -1779,7 +1800,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1">
-        <v>1651902344</v>
+        <v>1652004475</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>58</v>
@@ -1788,7 +1809,7 @@
         <v>62</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>63</v>
@@ -1799,7 +1820,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>1651826605</v>
+        <v>1651923024</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>65</v>
@@ -1808,7 +1829,7 @@
         <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>67</v>
@@ -1819,116 +1840,116 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>1651827003</v>
+        <v>1651902344</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>1651827827</v>
+        <v>1651826605</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>1651834564</v>
+        <v>1651827003</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>1651820943</v>
+        <v>1651827827</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>1651834916</v>
+        <v>1651834564</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>1651730520</v>
+        <v>1651820943</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>82</v>
@@ -1939,36 +1960,36 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
-        <v>1651654866</v>
+        <v>1651834916</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
-        <v>1651634414</v>
+        <v>1651730520</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>89</v>
@@ -1979,56 +2000,56 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>1651646933</v>
+        <v>1651654866</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>1651633116</v>
+        <v>1651634414</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>1651644769</v>
+        <v>1651646933</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>99</v>
@@ -2039,16 +2060,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>1651659154</v>
+        <v>1651633116</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>101</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>102</v>
@@ -2059,16 +2080,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1">
-        <v>1651487681</v>
+        <v>1651644769</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>106</v>
@@ -2079,16 +2100,16 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
-        <v>1651499797</v>
+        <v>1651659154</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>108</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>109</v>
@@ -2099,7 +2120,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1">
-        <v>1651323746</v>
+        <v>1651487681</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>111</v>
@@ -2108,7 +2129,7 @@
         <v>112</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>113</v>
@@ -2119,7 +2140,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1">
-        <v>1651312543</v>
+        <v>1651499797</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>111</v>
@@ -2128,7 +2149,7 @@
         <v>115</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>116</v>
@@ -2139,36 +2160,36 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>1651295846</v>
+        <v>1651323746</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>1651029491</v>
+        <v>1651312543</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>123</v>
@@ -2179,16 +2200,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1">
-        <v>1651045196</v>
+        <v>1651295846</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>125</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>126</v>
@@ -2199,36 +2220,36 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1">
-        <v>1651038505</v>
+        <v>1651029491</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1">
-        <v>1650938536</v>
+        <v>1651045196</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>133</v>
@@ -2239,36 +2260,36 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1">
-        <v>1650852390</v>
+        <v>1651038505</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1">
-        <v>1650877867</v>
+        <v>1650938536</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>140</v>
@@ -2279,7 +2300,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1">
-        <v>1650701590</v>
+        <v>1650852390</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>142</v>
@@ -2288,7 +2309,7 @@
         <v>143</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>144</v>
@@ -2299,122 +2320,162 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1">
-        <v>1650355221</v>
+        <v>1650877867</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1">
-        <v>1650113970</v>
+        <v>1650701590</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="D43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1">
-        <v>1649752200</v>
+        <v>1650355221</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1">
-        <v>1649474737</v>
+        <v>1650113970</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1">
-        <v>1648656738</v>
+        <v>1649752200</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1">
+        <v>1649474737</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="1">
+        <v>1648656738</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="1">
         <v>1648381501</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>169</v>
+      <c r="B49" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2022-05-24 14:42:05
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192">
   <si>
     <t>发布编号</t>
   </si>
@@ -34,15 +34,66 @@
     <t>公众号链接</t>
   </si>
   <si>
+    <t>2022-05-24</t>
+  </si>
+  <si>
+    <t>换届通知 | 密院科协主席团及部长团换届通知</t>
+  </si>
+  <si>
+    <t>密院科协</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWlCKD9TF71qTBbDg7OpkibJWBc6qBD4a92JlJM3FfjxAVmSdvVASMI2evExEpVVGzI426fxiboiaIhng/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488285&amp;idx=1&amp;sn=fc1faa055cdbc5c872aa4943d5cfacbb&amp;chksm=97d0fdaaa0a774bc7f6cf9f307cfe6d50d9142b998ec0a0994609d63804731d70bfb41290562#rd</t>
+  </si>
+  <si>
+    <t>2022-05-23</t>
+  </si>
+  <si>
+    <t>青年大学习：在新时代谱写青年运动新篇章</t>
+  </si>
+  <si>
+    <t>JI青团</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4BpLzJpZx7aJSucg3tqNxdzDkEtBseX1MCwLp5ibaY3hcaD4kDnvkCe1cXt8NamrkJGcO8C0Cpe1eQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486280&amp;idx=1&amp;sn=65ed940286c4b33dca30d3c0dc51698d&amp;chksm=fa3f12f6cd489be0c11753c78fe3c958a5e6d81dadb60a0540ec5a4ff7fb22d2e57087fa3afa#rd</t>
+  </si>
+  <si>
+    <t>2022-05-22</t>
+  </si>
+  <si>
+    <t>服务月 | 夏季权益问卷·FOR BETTER SUMMER</t>
+  </si>
+  <si>
+    <t>JIers</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNGBibR9y9f9bXhWhzBGx1S8J2wy8wIfrPiaYOywsu47rm6rUfkfkP4Cl3AUqjLyNphMY7tlNJDYFia1g/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185743&amp;idx=1&amp;sn=4e7a32b232dddeac91fa925ca78dbb8b&amp;chksm=8bfc2477bc8bad6119958a7b429814d6566609876fe7c0fdadd76c0d5a600ea6e15354cd5b62#rd</t>
+  </si>
+  <si>
     <t>2022-05-21</t>
   </si>
   <si>
+    <t>回顾 | 春假BINGO活动回顾</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_png/sZvUJ5A0zNEE9ehUbp6PSwcd1icLh1UJnB7GuNz4PBl82BdZ2iarohOW3f2G80jicu50Syf3mo6IRjo4icjTBBiax2A/0?wx_fmt=png</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185716&amp;idx=1&amp;sn=123db9362c9f36bd74c775de1cb59253&amp;chksm=8bfc240cbc8bad1a195850bc17dd01b229ff089a3bb27ef358182aa504f0c7359a756832bfc2#rd</t>
+  </si>
+  <si>
     <t>传媒部 | PPT Workshop 来啦！</t>
   </si>
   <si>
-    <t>JIers</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_png/sZvUJ5A0zNHTYUfqzx2ftWEXIwJzUMbfyM6ia03x3IBKrA9x5pj6VGIVQDdd4b2QDtVGgtHRXLwYibl1sX2LhQSA/0?wx_fmt=png</t>
   </si>
   <si>
@@ -94,15 +145,21 @@
     <t>青年大学习：学习习近平总书记在庆祝中国共产主义青年团成立100周年大会上的重要讲话精神</t>
   </si>
   <si>
-    <t>JI青团</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4Dib2WjxQn9Bgn5VticgfEfdKibYtX5BQA5zbt9gemyzTrFYp1oOzj1V6MyBUjqsV7mhqrKoCntc8ByQ/0?wx_fmt=jpeg</t>
   </si>
   <si>
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486248&amp;idx=1&amp;sn=92d251a227a6a0190374ff5a283944af&amp;chksm=fa3f1296cd489b8003c01dfc403cce50dfd33c649544333390b6e15f72e1e3b738b7ef524719#rd</t>
   </si>
   <si>
+    <t>【活动回顾】GDP×保研workshop圆满结束！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moSictu4icWQJwfw0Myibnt9xKLjlv13GbzAt9D2Vp7My36zeOH1cOQAYD4l68OZG638slxbzWuh4liczA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491681&amp;idx=1&amp;sn=9d27cb02f3aacbe6bfd5e8a4a3540e6a&amp;chksm=ec0e0970db798066032ba2bb809e8c29473206ce54164131221d23bbc2a7c1c8907e8f8ab307#rd</t>
+  </si>
+  <si>
     <t>密西根学院学生会第十七届主席团候选人介绍</t>
   </si>
   <si>
@@ -112,15 +169,6 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185670&amp;idx=1&amp;sn=08acd02cf1fb3dfc6231d1892cf9fe79&amp;chksm=8bfc243ebc8bad28a1898210c6bdd7f34f16497df1ced5611ea2468f6e9c91300cd208c2b442#rd</t>
   </si>
   <si>
-    <t>【活动回顾】GDP×保研workshop圆满结束！</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moSictu4icWQJwfw0Myibnt9xKLjlv13GbzAt9D2Vp7My36zeOH1cOQAYD4l68OZG638slxbzWuh4liczA/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491681&amp;idx=1&amp;sn=9d27cb02f3aacbe6bfd5e8a4a3540e6a&amp;chksm=ec0e0970db798066032ba2bb809e8c29473206ce54164131221d23bbc2a7c1c8907e8f8ab307#rd</t>
-  </si>
-  <si>
     <t>2022-05-14</t>
   </si>
   <si>
@@ -181,9 +229,6 @@
     <t>JI Science｜浅谈卷积神经网络剪枝</t>
   </si>
   <si>
-    <t>密院科协</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWnZ7vX7YChza3GmCdIpXKj27x4O0woo44ib6icNmmn0mkDXTpUcAzlL1tuJibNF1mYJT1tQicVcaYRc9Q/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -193,6 +238,15 @@
     <t>2022-05-08</t>
   </si>
   <si>
+    <t>GDP × 保研workshop预告+预热系列之GDP项目专访</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moQ2PH5YeuJPgYpFv3BTia9hadiaicr4Vg38fj1lwKob4zuicY5qENleTMCiakoRaibvgl6UkN5yE9HOtbMA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491670&amp;idx=1&amp;sn=c1323727d8529c2e627a9130165052c3&amp;chksm=ec0e0947db7980518ce7fb1e26e3ac06f636d3cfe2e7997ef7abf032b47ea586f2b25dcca847#rd</t>
+  </si>
+  <si>
     <t>上海交通大学密西根学院学生会第十七届主席团候选团队公示</t>
   </si>
   <si>
@@ -202,15 +256,6 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185652&amp;idx=1&amp;sn=46e290b80311a189bf74761a80dd671f&amp;chksm=8bfc27ccbc8baedaeece4553f1e6c995cf9fb7dcbc51762dd9bb449091fe0ace68ba4e189cff#rd</t>
   </si>
   <si>
-    <t>GDP × 保研workshop预告+预热系列之GDP项目专访</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moQ2PH5YeuJPgYpFv3BTia9hadiaicr4Vg38fj1lwKob4zuicY5qENleTMCiakoRaibvgl6UkN5yE9HOtbMA/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491670&amp;idx=1&amp;sn=c1323727d8529c2e627a9130165052c3&amp;chksm=ec0e0947db7980518ce7fb1e26e3ac06f636d3cfe2e7997ef7abf032b47ea586f2b25dcca847#rd</t>
-  </si>
-  <si>
     <t>2022-05-07</t>
   </si>
   <si>
@@ -235,30 +280,39 @@
     <t>2022-05-06</t>
   </si>
   <si>
+    <t>2022 SU 夏季学期高阶课Workshop</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMiaOw0xZPvwT9sNvxmzSr6Pwv7HM5oGZM9hib0Dc5EuGzicIxfH6kKHxk5OQO0uNKY0D4aqQIkyNKzPw/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484343&amp;idx=1&amp;sn=5d6a9c8d05bd283af59317f9d51f450b&amp;chksm=fbeb940acc9c1d1cd6924f088a6b38cfed82ac1b7ac2cdc407c2a956fe33e65338f8ce26443f#rd</t>
+  </si>
+  <si>
+    <t>文艺部 | Echoism 线上歌会倒计时</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNEs74dkleoJ9mK3B9Tc6Ol7K7wLib13XG66krDialaNsSVJC5Xa0avEia7l2U2PwicIon4HltS9RuxqxA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185638&amp;idx=1&amp;sn=a435c5bf80dbbc801c8a2d103d7f8e50&amp;chksm=8bfc27debc8baec87ad109f1f309c90a8a757c817e118e23e3d458c9a0c21d29fe7ae8e79b30#rd</t>
+  </si>
+  <si>
     <t>优秀团员分享 | 百年共青团和我的故事</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_png/QfDapvG9u4DMj1WoP0ODbssa94NEKOS2uYX0CsZmdmjujUSYLMG1Ib0IotFv8A9IWGdpvuOGP8qOU9uPJmicKkw/0?wx_fmt=png</t>
   </si>
   <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486185&amp;idx=1&amp;sn=c64eeec3346165d5829cde1f61f4adca&amp;chksm=fa3f1357cd489a41ec0c01b809e0a927a2c0f5dada0dc88b1047f82f6f2fc35fc7f33bde445b#rd</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486182&amp;idx=1&amp;sn=72e51b4720009f9afef0c7d51fb692ff&amp;chksm=fa3f1358cd489a4e0a6f6e2aa1443c3a2be49eacb75df3bc656cafa6afc75bd79b1e2e236716#rd</t>
+  </si>
+  <si>
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486173&amp;idx=1&amp;sn=6ecdbacb97830fad0b757ce3b426e3c3&amp;chksm=fa3f1363cd489a7572205cb63ed1f80c34081f6fe7e49085756f9cd02555a09218933a6ad3b6#rd</t>
   </si>
   <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486182&amp;idx=1&amp;sn=72e51b4720009f9afef0c7d51fb692ff&amp;chksm=fa3f1358cd489a4e0a6f6e2aa1443c3a2be49eacb75df3bc656cafa6afc75bd79b1e2e236716#rd</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486185&amp;idx=1&amp;sn=c64eeec3346165d5829cde1f61f4adca&amp;chksm=fa3f1357cd489a41ec0c01b809e0a927a2c0f5dada0dc88b1047f82f6f2fc35fc7f33bde445b#rd</t>
-  </si>
-  <si>
-    <t>文艺部 | Echoism 线上歌会倒计时</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNEs74dkleoJ9mK3B9Tc6Ol7K7wLib13XG66krDialaNsSVJC5Xa0avEia7l2U2PwicIon4HltS9RuxqxA/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185638&amp;idx=1&amp;sn=a435c5bf80dbbc801c8a2d103d7f8e50&amp;chksm=8bfc27debc8baec87ad109f1f309c90a8a757c817e118e23e3d458c9a0c21d29fe7ae8e79b30#rd</t>
-  </si>
-  <si>
     <t>赛事相关 | E创 | 咱就是说，极客派对x创意工坊一整个爱住了</t>
   </si>
   <si>
@@ -268,15 +322,6 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488207&amp;idx=1&amp;sn=1953baf8cc4aad31e0d8a79a8105e3df&amp;chksm=97d0fc78a0a7756ee8e506311d88f0361953267b91db390e44655440abf5d2b5502cd4850ef6#rd</t>
   </si>
   <si>
-    <t>2022 SU 夏季学期高阶课Workshop</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMiaOw0xZPvwT9sNvxmzSr6Pwv7HM5oGZM9hib0Dc5EuGzicIxfH6kKHxk5OQO0uNKY0D4aqQIkyNKzPw/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484343&amp;idx=1&amp;sn=5d6a9c8d05bd283af59317f9d51f450b&amp;chksm=fbeb940acc9c1d1cd6924f088a6b38cfed82ac1b7ac2cdc407c2a956fe33e65338f8ce26443f#rd</t>
-  </si>
-  <si>
     <t>2022-05-05</t>
   </si>
   <si>
@@ -292,6 +337,15 @@
     <t>2022-05-04</t>
   </si>
   <si>
+    <t>百年风雨路，青春勇担当！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWnj8zwbJgnCyIS573w0WOreDvzkmrCOcHNZmDj9sFBVp5CyHyHJqjE8gNgCYYOAWIaDuMmxaZlB1Q/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488188&amp;idx=1&amp;sn=7bdb958cacbe58eef2a86d3951977b3c&amp;chksm=97d0fc0ba0a7751d5fb928108bea1a2b6a11a19112a12c582c04fb46e0c554034dce037efe1a#rd</t>
+  </si>
+  <si>
     <t>事业部Piazza | 期待你的加入！</t>
   </si>
   <si>
@@ -301,6 +355,27 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491595&amp;idx=1&amp;sn=f69986ee829561de050049d016718a05&amp;chksm=ec0e091adb79800c6376087fb6e78975c64c4c4bb7dca96d6adb9b7e1e5347ed959259424738#rd</t>
   </si>
   <si>
+    <t>庆祝中国共产主义青年团成立100周年！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNEYLIcBYQuf3VDK9ItGLYVZ41cLvWmERPxXt4C5c9nCl47XNs7r8rsBiaMefl6Bvbiak1AwAYCxqOfQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185625&amp;idx=1&amp;sn=d8383126344a73d70f669fdf402cc980&amp;chksm=8bfc27e1bc8baef7c57a15e9ce96a6dc6b19c1a6add98af6eb0d5c89ddefed115e1155e112e5#rd</t>
+  </si>
+  <si>
+    <t>分享图片</t>
+  </si>
+  <si>
+    <t>JI觅源</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5RB0Yiby9sB6Scf0yAHqes6AIg6AVOtiap9BYVlVAGGsYND2L6MDXlrjYRWpgpCRv6mzt5agpytq0hw/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzAwNTYxNzk3Mw==&amp;mid=2648011547&amp;idx=1&amp;sn=38b3042a6ebcce9a2af7631b30ff465d&amp;chksm=83383341b44fba57d607ed01069410c82785bab42763195c425b29d602c19b8274e74d49d882#rd</t>
+  </si>
+  <si>
     <t>热烈庆祝中国共产主义青年团成立100周年！</t>
   </si>
   <si>
@@ -310,15 +385,6 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486150&amp;idx=1&amp;sn=b3073dee8e7be246e703dd7d56e47d2f&amp;chksm=fa3f1378cd489a6ef3c9f4cbd1358175fe3cc881abb3b4855b78608d10fc786e927d4ef6fbba#rd</t>
   </si>
   <si>
-    <t>庆祝中国共产主义青年团成立100周年！</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNEYLIcBYQuf3VDK9ItGLYVZ41cLvWmERPxXt4C5c9nCl47XNs7r8rsBiaMefl6Bvbiak1AwAYCxqOfQ/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185625&amp;idx=1&amp;sn=d8383126344a73d70f669fdf402cc980&amp;chksm=8bfc27e1bc8baef7c57a15e9ce96a6dc6b19c1a6add98af6eb0d5c89ddefed115e1155e112e5#rd</t>
-  </si>
-  <si>
     <t>回顾 | 2022 SU TA Workshop</t>
   </si>
   <si>
@@ -328,30 +394,18 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484329&amp;idx=1&amp;sn=086b74915dd33d34ede2cef1f4adf534&amp;chksm=fbeb9414cc9c1d024b5cb0455b4ba3d568223d3de7ce1d6f7974c75e8ad0c32aebea745f33f3#rd</t>
   </si>
   <si>
-    <t>分享图片</t>
-  </si>
-  <si>
-    <t>JI觅源</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5RB0Yiby9sB6Scf0yAHqes6AIg6AVOtiap9BYVlVAGGsYND2L6MDXlrjYRWpgpCRv6mzt5agpytq0hw/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzAwNTYxNzk3Mw==&amp;mid=2648011547&amp;idx=1&amp;sn=38b3042a6ebcce9a2af7631b30ff465d&amp;chksm=83383341b44fba57d607ed01069410c82785bab42763195c425b29d602c19b8274e74d49d882#rd</t>
-  </si>
-  <si>
-    <t>百年风雨路，青春勇担当！</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWnj8zwbJgnCyIS573w0WOreDvzkmrCOcHNZmDj9sFBVp5CyHyHJqjE8gNgCYYOAWIaDuMmxaZlB1Q/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488188&amp;idx=1&amp;sn=7bdb958cacbe58eef2a86d3951977b3c&amp;chksm=97d0fc0ba0a7751d5fb928108bea1a2b6a11a19112a12c582c04fb46e0c554034dce037efe1a#rd</t>
-  </si>
-  <si>
     <t>2022-05-02</t>
   </si>
   <si>
+    <t>青年大学习：争做改革开放的“弄潮儿”</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4CxdYdsFEYgYoo7FYTIEibLFaM1Fg6xtvGy8n5mlm9B4yuTTcdJyIquWiaonicLPicqxvPJh2UUic9Bpgg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486142&amp;idx=1&amp;sn=ed082adade2cdf25de03ccae4b803cf1&amp;chksm=fa3f1300cd489a161734868acb63db53aee2a3f4eeb346a1ffd75423b4c82b5fa9dff2af3d97#rd</t>
+  </si>
+  <si>
     <t>赛事相关 | 2022年度上海交通大学“数学建模培训营”国赛招生通知</t>
   </si>
   <si>
@@ -361,15 +415,6 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488176&amp;idx=1&amp;sn=e5ac653e3bb798e01e7808af0c448c91&amp;chksm=97d0fc07a0a77511c146ac371336b4676e6f16c6004a5427da0629b64a131df9c82fd5dbddd7#rd</t>
   </si>
   <si>
-    <t>青年大学习：争做改革开放的“弄潮儿”</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4CxdYdsFEYgYoo7FYTIEibLFaM1Fg6xtvGy8n5mlm9B4yuTTcdJyIquWiaonicLPicqxvPJh2UUic9Bpgg/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486142&amp;idx=1&amp;sn=ed082adade2cdf25de03ccae4b803cf1&amp;chksm=fa3f1300cd489a161734868acb63db53aee2a3f4eeb346a1ffd75423b4c82b5fa9dff2af3d97#rd</t>
-  </si>
-  <si>
     <t>2022-04-30</t>
   </si>
   <si>
@@ -403,6 +448,24 @@
     <t>2022-04-27</t>
   </si>
   <si>
+    <t>文艺部 | Echoism歌手大赛 复赛反馈&amp;资格赛开启</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_png/sZvUJ5A0zNHxOO6BOrWicO1G7zIzzDOHJuC1PqcrQVSacE8fLJibF15PUYafOyyzfhMKEEWJ72RBUupVxic4JNERQ/0?wx_fmt=png</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185610&amp;idx=1&amp;sn=8bfeeda3b2e55aee59b0b8176bed0844&amp;chksm=8bfc27f2bc8baee4bdd644584a154ce39fb8ff15794982a30c4a03600fccea0635f3c5dabcea#rd</t>
+  </si>
+  <si>
+    <t>【招聘】富士康工业互联网2022校园招聘</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moSqoWKbGvU1nRtxjic9iahkKnaMic8QLcECVhJTXfukFTMV5jXkcFdAoic1iahSNAW05IhyI24GrUGgyrQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491525&amp;idx=1&amp;sn=6ab5a1f574fa632a2ad450880c0b2f53&amp;chksm=ec0df6d4db7a7fc2017063b6244913b002d4edfac1424d5ffd2ddbd9f256c6fe898466c3b83f#rd</t>
+  </si>
+  <si>
     <t>转载 | 习近平和大学生在一起</t>
   </si>
   <si>
@@ -412,24 +475,6 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486120&amp;idx=1&amp;sn=9335d6fd264eec3bcb9abc9ebeb1a3fb&amp;chksm=fa3f1316cd489a0038088066af34d7ac458e9067f496a8608779d580a1c440ca1aaabaa0453d#rd</t>
   </si>
   <si>
-    <t>文艺部 | Echoism歌手大赛 复赛反馈&amp;资格赛开启</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_png/sZvUJ5A0zNHxOO6BOrWicO1G7zIzzDOHJuC1PqcrQVSacE8fLJibF15PUYafOyyzfhMKEEWJ72RBUupVxic4JNERQ/0?wx_fmt=png</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185610&amp;idx=1&amp;sn=8bfeeda3b2e55aee59b0b8176bed0844&amp;chksm=8bfc27f2bc8baee4bdd644584a154ce39fb8ff15794982a30c4a03600fccea0635f3c5dabcea#rd</t>
-  </si>
-  <si>
-    <t>【招聘】富士康工业互联网2022校园招聘</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moSqoWKbGvU1nRtxjic9iahkKnaMic8QLcECVhJTXfukFTMV5jXkcFdAoic1iahSNAW05IhyI24GrUGgyrQ/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491525&amp;idx=1&amp;sn=6ab5a1f574fa632a2ad450880c0b2f53&amp;chksm=ec0df6d4db7a7fc2017063b6244913b002d4edfac1424d5ffd2ddbd9f256c6fe898466c3b83f#rd</t>
-  </si>
-  <si>
     <t>2022-04-26</t>
   </si>
   <si>
@@ -445,6 +490,15 @@
     <t>2022-04-25</t>
   </si>
   <si>
+    <t>快来查收你的春假Bingo召集令！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNHZy4vBcYSKXbo5B49nwqNZbvKjRsC651mfAYib5M7aClTQ3QBmclSyQIAYDrRMqx6wCNEB3klJHXg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185604&amp;idx=1&amp;sn=2037bed613387e5dcb2ebb7c8e21cde4&amp;chksm=8bfc27fcbc8baeea3638463edc150c2884c774617f7dca9c763ee757dc507c104f5facad1c64#rd</t>
+  </si>
+  <si>
     <t>转载 | 新时代加强和改进共青团思想政治引领工作实施纲要</t>
   </si>
   <si>
@@ -452,15 +506,6 @@
   </si>
   <si>
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486093&amp;idx=1&amp;sn=d20cb7fbe6a7d64e0fd3c14c37a7a0ac&amp;chksm=fa3f1333cd489a25f1417672d98276aff3759c79a46685db68840edbb3d6237c898977f483a7#rd</t>
-  </si>
-  <si>
-    <t>快来查收你的春假Bingo召集令！</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNHZy4vBcYSKXbo5B49nwqNZbvKjRsC651mfAYib5M7aClTQ3QBmclSyQIAYDrRMqx6wCNEB3klJHXg/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185604&amp;idx=1&amp;sn=2037bed613387e5dcb2ebb7c8e21cde4&amp;chksm=8bfc27fcbc8baeea3638463edc150c2884c774617f7dca9c763ee757dc507c104f5facad1c64#rd</t>
   </si>
   <si>
     <t>2022-04-23</t>
@@ -553,8 +598,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -580,7 +625,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -589,22 +640,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -620,6 +656,82 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -635,17 +747,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -655,66 +760,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -731,181 +776,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -916,35 +961,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -959,6 +975,36 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -978,17 +1024,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1002,17 +1053,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1021,142 +1066,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1490,10 +1535,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F49"/>
+      <selection activeCell="A1" sqref="A1:F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1520,7 +1565,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>1653106699</v>
+        <v>1653358054</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1540,96 +1585,96 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>1653103833</v>
+        <v>1653310453</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>1652946162</v>
+        <v>1653206327</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>1652766746</v>
+        <v>1653112956</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>1652711615</v>
+        <v>1653106699</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>1652633146</v>
+        <v>1653103833</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>30</v>
@@ -1640,716 +1685,716 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>1652708097</v>
+        <v>1652946162</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>1652502015</v>
+        <v>1652766746</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>1652423986</v>
+        <v>1652711615</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>1652196254</v>
+        <v>1652708097</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1">
-        <v>1652156920</v>
+        <v>1652633146</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1">
-        <v>1652102252</v>
+        <v>1652502015</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1">
-        <v>1652082724</v>
+        <v>1652423986</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1">
-        <v>1651989033</v>
+        <v>1652196254</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1">
-        <v>1652004475</v>
+        <v>1652156920</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>1651923024</v>
+        <v>1652102252</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>1651902344</v>
+        <v>1652082724</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>1651826605</v>
+        <v>1652004475</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>1651827003</v>
+        <v>1651989033</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>1651827827</v>
+        <v>1651923024</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>1651834564</v>
+        <v>1651902344</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>1651820943</v>
+        <v>1651834916</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
-        <v>1651834916</v>
+        <v>1651834564</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
-        <v>1651730520</v>
+        <v>1651827827</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>1651654866</v>
+        <v>1651827003</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>1651634414</v>
+        <v>1651826605</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="F27" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>1651646933</v>
+        <v>1651820943</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>1651633116</v>
+        <v>1651730520</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1">
-        <v>1651644769</v>
+        <v>1651659154</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
-        <v>1651659154</v>
+        <v>1651654866</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1">
-        <v>1651487681</v>
+        <v>1651646933</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1">
-        <v>1651499797</v>
+        <v>1651644769</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>1651323746</v>
+        <v>1651634414</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>1651312543</v>
+        <v>1651633116</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1">
-        <v>1651295846</v>
+        <v>1651499797</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1">
-        <v>1651029491</v>
+        <v>1651487681</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1">
-        <v>1651045196</v>
+        <v>1651323746</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1">
-        <v>1651038505</v>
+        <v>1651312543</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1">
-        <v>1650938536</v>
+        <v>1651295846</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1">
-        <v>1650852390</v>
+        <v>1651045196</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1">
-        <v>1650877867</v>
+        <v>1651038505</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1">
-        <v>1650701590</v>
+        <v>1651029491</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>150</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>151</v>
@@ -2360,7 +2405,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1">
-        <v>1650355221</v>
+        <v>1650938536</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>153</v>
@@ -2369,7 +2414,7 @@
         <v>154</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>155</v>
@@ -2380,7 +2425,7 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1">
-        <v>1650113970</v>
+        <v>1650877867</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>157</v>
@@ -2389,7 +2434,7 @@
         <v>158</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>159</v>
@@ -2400,82 +2445,162 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1">
-        <v>1649752200</v>
+        <v>1650852390</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1">
-        <v>1649474737</v>
+        <v>1650701590</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="D47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1">
-        <v>1648656738</v>
+        <v>1650355221</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1">
+        <v>1650113970</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="1">
+        <v>1649752200</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="1">
+        <v>1649474737</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="1">
+        <v>1648656738</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="1">
         <v>1648381501</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>176</v>
+      <c r="B53" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2022-05-25 22:05:26
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205">
   <si>
     <t>发布编号</t>
   </si>
@@ -34,6 +34,33 @@
     <t>公众号链接</t>
   </si>
   <si>
+    <t>2022-05-25</t>
+  </si>
+  <si>
+    <t>2022年毕业学生团员组织关系转接指引和问答，请查收！</t>
+  </si>
+  <si>
+    <t>JI青团</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4Akqks8JI1u5vfREuf7qHxQ31mPyOia2ic8oklruf5dicxYAmOTge3UUNmVKmfoE2hl0kcQfrL8V1IicA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486292&amp;idx=1&amp;sn=e58d83d7d2be4d9857458ffce5bb4828&amp;chksm=fa3f12eacd489bfcd40d5a35729467cbe84fb2c2faa67ad3e4280946e4fae4938551b3528b42#rd</t>
+  </si>
+  <si>
+    <t>回顾｜研究生申请workshop for DDers</t>
+  </si>
+  <si>
+    <t>JIAdvisingCenter</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMia2Qwiatd5dibItBUFVSeuQqwqp1vyia856ficIbNguV9FrDoRLKNbs5cGWXtwUQCaMu7GBng1YRib6c3A/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484415&amp;idx=1&amp;sn=871a6907a654ed93473a2b1e7ac3a19d&amp;chksm=fbeb9442cc9c1d544d442d36b2ef242e51fe30af501dfa88b7d2ad2f87383eb7b86a97137644#rd</t>
+  </si>
+  <si>
     <t>2022-05-24</t>
   </si>
   <si>
@@ -49,15 +76,33 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488285&amp;idx=1&amp;sn=fc1faa055cdbc5c872aa4943d5cfacbb&amp;chksm=97d0fdaaa0a774bc7f6cf9f307cfe6d50d9142b998ec0a0994609d63804731d70bfb41290562#rd</t>
   </si>
   <si>
+    <t>服务月 | 学生会活动策划体验小程序发布·舞会专场</t>
+  </si>
+  <si>
+    <t>JIers</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNF8oSW3NkPmUIUVnuj1eslVrp1gKNdXsicCsXZgwNc4OE4WqHbc815nGyCqXLM9wchR8t8FhHib6oZA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185750&amp;idx=1&amp;sn=aef0ae274678e64323612345555d502e&amp;chksm=8bfc246ebc8bad78e7f3b89409b106f6fc7afb97cdbb9d1275f5ee0a24588c8576c6d8ff58b9#rd</t>
+  </si>
+  <si>
+    <t>人民日报评论部：理想远大、信念坚定——把青春播撒在民族复兴的征程上①</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4BZcibEN1k9RxoEN0XLnO4ov0u4Za4fFpgyCMHJ2nib6gUGl4s0e5DPQDJWzttcfvBXibvicyHdPEz8wA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486285&amp;idx=1&amp;sn=087e843ea5d9de4425b5eb981628854a&amp;chksm=fa3f12f3cd489be5f3d39f074ba02b13485ed3c61cbcae13b6dde4d016ac85a36208888e1e7b#rd</t>
+  </si>
+  <si>
     <t>2022-05-23</t>
   </si>
   <si>
     <t>青年大学习：在新时代谱写青年运动新篇章</t>
   </si>
   <si>
-    <t>JI青团</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4BpLzJpZx7aJSucg3tqNxdzDkEtBseX1MCwLp5ibaY3hcaD4kDnvkCe1cXt8NamrkJGcO8C0Cpe1eQ/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -70,9 +115,6 @@
     <t>服务月 | 夏季权益问卷·FOR BETTER SUMMER</t>
   </si>
   <si>
-    <t>JIers</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNGBibR9y9f9bXhWhzBGx1S8J2wy8wIfrPiaYOywsu47rm6rUfkfkP4Cl3AUqjLyNphMY7tlNJDYFia1g/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -101,9 +143,6 @@
   </si>
   <si>
     <t>研究生申请&amp;生涯发展经验分享会 | For DDers</t>
-  </si>
-  <si>
-    <t>JIAdvisingCenter</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMjp5FpuKh2hTVSicZnHxaiao3A7xRTBiceQMxoZUw2SICyL6Wt6D1SMeu6ic4CFecmtxkUrOUDZmlQDtQ/0?wx_fmt=jpeg</t>
@@ -625,6 +664,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -632,8 +679,99 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -656,106 +794,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -770,187 +809,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -961,21 +1000,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -994,17 +1018,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1053,11 +1086,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1066,142 +1105,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1535,10 +1574,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F53"/>
+      <selection activeCell="A1" sqref="A1:F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1565,7 +1604,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>1653358054</v>
+        <v>1653455486</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1585,456 +1624,456 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>1653310453</v>
+        <v>1653457678</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>1653206327</v>
+        <v>1653358054</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>1653112956</v>
+        <v>1653381370</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>1653106699</v>
+        <v>1653400076</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>1653103833</v>
+        <v>1653310453</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>1652946162</v>
+        <v>1653206327</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>1652766746</v>
+        <v>1653112956</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>1652711615</v>
+        <v>1653106699</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>1652708097</v>
+        <v>1653103833</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1">
-        <v>1652633146</v>
+        <v>1652946162</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1">
-        <v>1652502015</v>
+        <v>1652766746</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1">
-        <v>1652423986</v>
+        <v>1652711615</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1">
-        <v>1652196254</v>
+        <v>1652708097</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1">
-        <v>1652156920</v>
+        <v>1652633146</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>1652102252</v>
+        <v>1652502015</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>1652082724</v>
+        <v>1652423986</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>1652004475</v>
+        <v>1652196254</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>1651989033</v>
+        <v>1652156920</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>1651923024</v>
+        <v>1652102252</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>1651902344</v>
+        <v>1652082724</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>1651834916</v>
+        <v>1652004475</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
-        <v>1651834564</v>
+        <v>1651989033</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
-        <v>1651827827</v>
+        <v>1651923024</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>95</v>
@@ -2045,90 +2084,90 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>1651827003</v>
+        <v>1651902344</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>1651826605</v>
+        <v>1651834916</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>1651820943</v>
+        <v>1651834564</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>1651730520</v>
+        <v>1651827827</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1">
-        <v>1651659154</v>
+        <v>1651827003</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>107</v>
@@ -2140,81 +2179,81 @@
         <v>108</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
-        <v>1651654866</v>
+        <v>1651826605</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1">
-        <v>1651646933</v>
+        <v>1651820943</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1">
-        <v>1651644769</v>
+        <v>1651730520</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>116</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>1651634414</v>
+        <v>1651659154</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>120</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>121</v>
@@ -2225,16 +2264,16 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>1651633116</v>
+        <v>1651654866</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>123</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>124</v>
@@ -2245,36 +2284,36 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1">
-        <v>1651499797</v>
+        <v>1651646933</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1">
-        <v>1651487681</v>
+        <v>1651644769</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>131</v>
@@ -2285,56 +2324,56 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1">
-        <v>1651323746</v>
+        <v>1651634414</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1">
-        <v>1651312543</v>
+        <v>1651633116</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1">
-        <v>1651295846</v>
+        <v>1651499797</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>140</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>141</v>
@@ -2345,36 +2384,36 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1">
-        <v>1651045196</v>
+        <v>1651487681</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1">
-        <v>1651038505</v>
+        <v>1651323746</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>147</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>148</v>
@@ -2385,16 +2424,16 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1">
-        <v>1651029491</v>
+        <v>1651312543</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>150</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>151</v>
@@ -2405,202 +2444,282 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1">
-        <v>1650938536</v>
+        <v>1651295846</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1">
-        <v>1650877867</v>
+        <v>1651045196</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1">
-        <v>1650852390</v>
+        <v>1651038505</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1">
-        <v>1650701590</v>
+        <v>1651029491</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1">
-        <v>1650355221</v>
+        <v>1650938536</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1">
-        <v>1650113970</v>
+        <v>1650877867</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="1">
-        <v>1649752200</v>
+        <v>1650852390</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="1">
-        <v>1649474737</v>
+        <v>1650701590</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="1">
-        <v>1648656738</v>
+        <v>1650355221</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="1">
+        <v>1650113970</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="1">
+        <v>1649752200</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="1">
+        <v>1649474737</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="1">
+        <v>1648656738</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="1">
         <v>1648381501</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>191</v>
+      <c r="B57" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2022-05-28 22:36:58
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223">
   <si>
     <t>发布编号</t>
   </si>
@@ -34,15 +34,69 @@
     <t>公众号链接</t>
   </si>
   <si>
+    <t>2022-05-28</t>
+  </si>
+  <si>
+    <t>人民日报评论部：崇德向善、严守纪律——把青春播撒在民族复兴的征程上⑤</t>
+  </si>
+  <si>
+    <t>JI青团</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4BZcibEN1k9RxoEN0XLnO4ov0u4Za4fFpgyCMHJ2nib6gUGl4s0e5DPQDJWzttcfvBXibvicyHdPEz8wA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486301&amp;idx=1&amp;sn=2fa7e5ccab9f282fa61b91f8c513ff77&amp;chksm=fa3f12e3cd489bf58d4bc50da91bd1cc00592253bb7645dcb42195333f466429271c80abbbcb#rd</t>
+  </si>
+  <si>
+    <t>2022-05-27</t>
+  </si>
+  <si>
+    <t>Announcement | 觅源青志队部长团名单</t>
+  </si>
+  <si>
+    <t>JI觅源</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5TRhB2Fy8Bxht2NOVicqtM6ONplETHrVyGeMicbJOZ1cVudXBcEzZCa20pT9xFzaMSkPxM9QdX7v9oQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzAwNTYxNzk3Mw==&amp;mid=2648011583&amp;idx=1&amp;sn=c08e640d1c0debfdcb0d21f3e90a25b7&amp;chksm=83383365b44fba737163412305df6146a878945364c028a00c9eecc10f535a440995f8b9292e#rd</t>
+  </si>
+  <si>
+    <t>人民日报评论部：艰苦奋斗、无私奉献——把青春播撒在民族复兴的征程上④</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486298&amp;idx=1&amp;sn=e10bac10a7f30f9387ac16ae0e84de95&amp;chksm=fa3f12e4cd489bf20f6a08598636cb5580d5f18fbd3e10087630f529707848911f030e7c40b0#rd</t>
+  </si>
+  <si>
+    <t>2022-05-26</t>
+  </si>
+  <si>
+    <t>服务月｜密院12345：全新的权益反馈体验！</t>
+  </si>
+  <si>
+    <t>JIers</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNENeh0X1llR0s9joO2LI6E3e1U6I5IulEHuBtGf4ZrJ81YU3ia4xYbDsxuEZCvpria8Q1RLSdiclao9g/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185769&amp;idx=1&amp;sn=5b295c9a0f58b3af1dfa26dbfc2bb96e&amp;chksm=8bfc2451bc8bad4713a5663ff2713d51264add07d4b3ee37ca23ef1c928cb14edf8154193688#rd</t>
+  </si>
+  <si>
+    <t>人民日报评论部：敢于斗争、善于斗争——把青春播撒在民族复兴的征程上③</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486295&amp;idx=1&amp;sn=f14ac378113a19fd357d4e22f749d11e&amp;chksm=fa3f12e9cd489bff2aef57e2d0480760ac704825021a2f28d43c09f32fd6294efff46609bcbc#rd</t>
+  </si>
+  <si>
     <t>2022-05-25</t>
   </si>
   <si>
     <t>2022年毕业学生团员组织关系转接指引和问答，请查收！</t>
   </si>
   <si>
-    <t>JI青团</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4Akqks8JI1u5vfREuf7qHxQ31mPyOia2ic8oklruf5dicxYAmOTge3UUNmVKmfoE2hl0kcQfrL8V1IicA/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -61,6 +115,18 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484415&amp;idx=1&amp;sn=871a6907a654ed93473a2b1e7ac3a19d&amp;chksm=fbeb9442cc9c1d544d442d36b2ef242e51fe30af501dfa88b7d2ad2f87383eb7b86a97137644#rd</t>
   </si>
   <si>
+    <t>【活动】密院“工转商”升学分享会预告</t>
+  </si>
+  <si>
+    <t>JIcareer</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moSNQpVcLYNa57WN3ufOeuCxzKbaO9RG8LEDw2CMnyPskCSe9l7D0atcDqdFwo19d8ibJQqiccG6VEHg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491710&amp;idx=1&amp;sn=6ef79f4599404bf731dc226397fd15cb&amp;chksm=ec0e096fdb7980791670c3ed17b9db99ea954ada8dd84baf686847744cf326207bff0c8ec3a0#rd</t>
+  </si>
+  <si>
     <t>2022-05-24</t>
   </si>
   <si>
@@ -79,9 +145,6 @@
     <t>服务月 | 学生会活动策划体验小程序发布·舞会专场</t>
   </si>
   <si>
-    <t>JIers</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNF8oSW3NkPmUIUVnuj1eslVrp1gKNdXsicCsXZgwNc4OE4WqHbc815nGyCqXLM9wchR8t8FhHib6oZA/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -91,9 +154,6 @@
     <t>人民日报评论部：理想远大、信念坚定——把青春播撒在民族复兴的征程上①</t>
   </si>
   <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4BZcibEN1k9RxoEN0XLnO4ov0u4Za4fFpgyCMHJ2nib6gUGl4s0e5DPQDJWzttcfvBXibvicyHdPEz8wA/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486285&amp;idx=1&amp;sn=087e843ea5d9de4425b5eb981628854a&amp;chksm=fa3f12f3cd489be5f3d39f074ba02b13485ed3c61cbcae13b6dde4d016ac85a36208888e1e7b#rd</t>
   </si>
   <si>
@@ -169,9 +229,6 @@
     <t>【招聘】Sophoton | 识光芯科在招岗位</t>
   </si>
   <si>
-    <t>JIcareer</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moSxJYWoqYh7Mcrp4pecJNeJiamkvhgNySd3PIVbsKgPZxBXo2tjcB9FibIF1XMvb6FoogQvdgCgDo2A/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -404,9 +461,6 @@
   </si>
   <si>
     <t>分享图片</t>
-  </si>
-  <si>
-    <t>JI觅源</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5RB0Yiby9sB6Scf0yAHqes6AIg6AVOtiap9BYVlVAGGsYND2L6MDXlrjYRWpgpCRv6mzt5agpytq0hw/0?wx_fmt=jpeg</t>
@@ -636,9 +690,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -659,14 +713,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -694,16 +740,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -717,11 +771,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -733,8 +802,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -763,10 +833,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -778,23 +848,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -809,13 +863,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -827,13 +1007,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -845,151 +1037,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1003,17 +1057,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1022,7 +1070,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1043,16 +1091,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1071,32 +1119,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1105,142 +1159,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1574,10 +1628,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F57"/>
+      <selection activeCell="A1" sqref="A1:F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1604,7 +1658,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>1653455486</v>
+        <v>1653734498</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1624,156 +1678,156 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>1653457678</v>
+        <v>1653661410</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>1653358054</v>
+        <v>1653655336</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>1653381370</v>
+        <v>1653560174</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>1653400076</v>
+        <v>1653566952</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>1653310453</v>
+        <v>1653455486</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>1653206327</v>
+        <v>1653457678</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>1653112956</v>
+        <v>1653488445</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>1653106699</v>
+        <v>1653358054</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>40</v>
@@ -1784,16 +1838,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>1653103833</v>
+        <v>1653381370</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>43</v>
@@ -1804,487 +1858,487 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1">
-        <v>1652946162</v>
+        <v>1653400076</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1">
-        <v>1652766746</v>
+        <v>1653310453</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1">
-        <v>1652711615</v>
+        <v>1653206327</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1">
-        <v>1652708097</v>
+        <v>1653112956</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1">
-        <v>1652633146</v>
+        <v>1653106699</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>1652502015</v>
+        <v>1653103833</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>1652423986</v>
+        <v>1652946162</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>1652196254</v>
+        <v>1652766746</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>1652156920</v>
+        <v>1652711615</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>1652102252</v>
+        <v>1652708097</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>1652082724</v>
+        <v>1652633146</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>1652004475</v>
+        <v>1652502015</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
-        <v>1651989033</v>
+        <v>1652423986</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
-        <v>1651923024</v>
+        <v>1652196254</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>1651902344</v>
+        <v>1652156920</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>1651834916</v>
+        <v>1652102252</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>1651834564</v>
+        <v>1652082724</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>1651827827</v>
+        <v>1652004475</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1">
-        <v>1651827003</v>
+        <v>1651989033</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
-        <v>1651826605</v>
+        <v>1651923024</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1">
-        <v>1651820943</v>
+        <v>1651902344</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1">
-        <v>1651730520</v>
+        <v>1651834916</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>1651659154</v>
+        <v>1651834564</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>1651654866</v>
+        <v>1651827827</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1">
-        <v>1651646933</v>
+        <v>1651827003</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>119</v>
@@ -2293,433 +2347,553 @@
         <v>126</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>127</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1">
-        <v>1651644769</v>
+        <v>1651826605</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1">
-        <v>1651634414</v>
+        <v>1651820943</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1">
-        <v>1651633116</v>
+        <v>1651730520</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1">
-        <v>1651499797</v>
+        <v>1651659154</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1">
-        <v>1651487681</v>
+        <v>1651654866</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1">
-        <v>1651323746</v>
+        <v>1651646933</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1">
-        <v>1651312543</v>
+        <v>1651644769</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1">
-        <v>1651295846</v>
+        <v>1651634414</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1">
-        <v>1651045196</v>
+        <v>1651633116</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1">
-        <v>1651038505</v>
+        <v>1651499797</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1">
-        <v>1651029491</v>
+        <v>1651487681</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1">
-        <v>1650938536</v>
+        <v>1651323746</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1">
-        <v>1650877867</v>
+        <v>1651312543</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="1">
-        <v>1650852390</v>
+        <v>1651295846</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="1">
-        <v>1650701590</v>
+        <v>1651045196</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="1">
-        <v>1650355221</v>
+        <v>1651038505</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="1">
-        <v>1650113970</v>
+        <v>1651029491</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="1">
-        <v>1649752200</v>
+        <v>1650938536</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="1">
-        <v>1649474737</v>
+        <v>1650877867</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="1">
-        <v>1648656738</v>
+        <v>1650852390</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="1">
+        <v>1650701590</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="1">
+        <v>1650355221</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="1">
+        <v>1650113970</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="1">
+        <v>1649752200</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="1">
+        <v>1649474737</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="1">
+        <v>1648656738</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="1">
         <v>1648381501</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>204</v>
+      <c r="B63" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2022-05-29 16:12:24
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233">
   <si>
     <t>发布编号</t>
   </si>
@@ -34,6 +34,33 @@
     <t>公众号链接</t>
   </si>
   <si>
+    <t>2022-05-29</t>
+  </si>
+  <si>
+    <t>Sign Up | Female Leadership Forum 2022</t>
+  </si>
+  <si>
+    <t>JIcareer</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moQ4AibkvlTuk6ptJxszs7BJKDibzniaTjNt2ZNDo4hibtrwZ6KMPL6ln282pKO4KT9TFfaFR1ssMxPccg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491725&amp;idx=1&amp;sn=41c4c275965a0b2ee76d681a3e83e73f&amp;chksm=ec0e099cdb79808a4e0daadf14c17a3120b0782d7c2a7ab619660205686eed9f1b35851126b5#rd</t>
+  </si>
+  <si>
+    <t>研究生申请&amp;生涯发展经验分享会 | For DDers (CE/EE/IOE专场)</t>
+  </si>
+  <si>
+    <t>JIAdvisingCenter</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMiaqQz5WPAGMHUvEZ9SNcyN4QXXC1jtEkNFc1fUXoiczUlicT3B1YjfuM5Pz5fUdtsB9BPLWLVvHUhqQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484425&amp;idx=1&amp;sn=aa9ce6b447305c994aaca1fbe733a074&amp;chksm=fbeb93b4cc9c1aa2153c9c421ad4c8c56ab5e3dc2c4ed4ac5128c371db1d166c211b6442293a#rd</t>
+  </si>
+  <si>
     <t>2022-05-28</t>
   </si>
   <si>
@@ -49,6 +76,18 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486301&amp;idx=1&amp;sn=2fa7e5ccab9f282fa61b91f8c513ff77&amp;chksm=fa3f12e3cd489bf58d4bc50da91bd1cc00592253bb7645dcb42195333f466429271c80abbbcb#rd</t>
   </si>
   <si>
+    <t>【推广】EECS专场 | 耶鲁、西北、UIUC！当前形势下，我该如何申请EECS？</t>
+  </si>
+  <si>
+    <t>JIers</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNHKYBDGQ7oiauy1QOLia0EBCwicY8aXmdHvHeibUO1JdqQ5MVLo0TXLrVj5o0n3blmg4WsZsB00h0yZZQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185782&amp;idx=2&amp;sn=2bf72405fd4782c9dbd20a5ea80058ff&amp;chksm=8bfc244ebc8bad5875cfbad7136894091e9fa26380609c8a5fd82e0519cfca4b16d3f4182925#rd</t>
+  </si>
+  <si>
     <t>2022-05-27</t>
   </si>
   <si>
@@ -76,9 +115,6 @@
     <t>服务月｜密院12345：全新的权益反馈体验！</t>
   </si>
   <si>
-    <t>JIers</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNENeh0X1llR0s9joO2LI6E3e1U6I5IulEHuBtGf4ZrJ81YU3ia4xYbDsxuEZCvpria8Q1RLSdiclao9g/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -106,9 +142,6 @@
     <t>回顾｜研究生申请workshop for DDers</t>
   </si>
   <si>
-    <t>JIAdvisingCenter</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMia2Qwiatd5dibItBUFVSeuQqwqp1vyia856ficIbNguV9FrDoRLKNbs5cGWXtwUQCaMu7GBng1YRib6c3A/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -116,9 +149,6 @@
   </si>
   <si>
     <t>【活动】密院“工转商”升学分享会预告</t>
-  </si>
-  <si>
-    <t>JIcareer</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moSNQpVcLYNa57WN3ufOeuCxzKbaO9RG8LEDw2CMnyPskCSe9l7D0atcDqdFwo19d8ibJQqiccG6VEHg/0?wx_fmt=jpeg</t>
@@ -691,9 +721,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -718,8 +748,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -733,10 +771,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -772,33 +833,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -825,13 +862,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -848,7 +878,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -863,181 +893,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1091,6 +1121,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1116,15 +1161,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1140,17 +1176,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1159,142 +1189,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1628,10 +1658,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F63"/>
+      <selection activeCell="A1" sqref="A1:F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1658,7 +1688,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>1653734498</v>
+        <v>1653809321</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1678,139 +1708,139 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>1653661410</v>
+        <v>1653756447</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>1653655336</v>
+        <v>1653734498</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>1653560174</v>
+        <v>1653752093</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>1653566952</v>
+        <v>1653661410</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>1653455486</v>
+        <v>1653655336</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>1653457678</v>
+        <v>1653560174</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>1653488445</v>
+        <v>1653566952</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>36</v>
@@ -1818,7 +1848,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>1653358054</v>
+        <v>1653455486</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>37</v>
@@ -1827,50 +1857,50 @@
         <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>1653381370</v>
+        <v>1653457678</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1">
-        <v>1653400076</v>
+        <v>1653488445</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>46</v>
@@ -1878,7 +1908,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1">
-        <v>1653310453</v>
+        <v>1653358054</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>47</v>
@@ -1887,27 +1917,27 @@
         <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1">
-        <v>1653206327</v>
+        <v>1653381370</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>53</v>
@@ -1918,56 +1948,56 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1">
-        <v>1653112956</v>
+        <v>1653400076</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1">
-        <v>1653106699</v>
+        <v>1653310453</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>1653103833</v>
+        <v>1653206327</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>63</v>
@@ -1978,7 +2008,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>1652946162</v>
+        <v>1653112956</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>65</v>
@@ -1987,7 +2017,7 @@
         <v>66</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>67</v>
@@ -1998,76 +2028,76 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>1652766746</v>
+        <v>1653106699</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>1652711615</v>
+        <v>1653103833</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>1652708097</v>
+        <v>1652946162</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>1652633146</v>
+        <v>1652766746</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>81</v>
@@ -2078,7 +2108,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>1652502015</v>
+        <v>1652711615</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>83</v>
@@ -2087,7 +2117,7 @@
         <v>84</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>85</v>
@@ -2098,96 +2128,96 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
-        <v>1652423986</v>
+        <v>1652708097</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
-        <v>1652196254</v>
+        <v>1652633146</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>1652156920</v>
+        <v>1652502015</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>1652102252</v>
+        <v>1652423986</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>1652082724</v>
+        <v>1652196254</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>103</v>
@@ -2198,36 +2228,36 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>1652004475</v>
+        <v>1652156920</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1">
-        <v>1651989033</v>
+        <v>1652102252</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>109</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>110</v>
@@ -2238,36 +2268,36 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
-        <v>1651923024</v>
+        <v>1652082724</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1">
-        <v>1651902344</v>
+        <v>1652004475</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>116</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>117</v>
@@ -2278,36 +2308,36 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1">
-        <v>1651834916</v>
+        <v>1651989033</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>1651834564</v>
+        <v>1651923024</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>123</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>124</v>
@@ -2318,16 +2348,16 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>1651827827</v>
+        <v>1651902344</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>127</v>
@@ -2338,136 +2368,136 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1">
-        <v>1651827003</v>
+        <v>1651834916</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1">
-        <v>1651826605</v>
+        <v>1651834564</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1">
-        <v>1651820943</v>
+        <v>1651827827</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1">
-        <v>1651730520</v>
+        <v>1651827003</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1">
-        <v>1651659154</v>
+        <v>1651826605</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1">
-        <v>1651654866</v>
+        <v>1651820943</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1">
-        <v>1651646933</v>
+        <v>1651730520</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>145</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>146</v>
@@ -2478,76 +2508,76 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1">
-        <v>1651644769</v>
+        <v>1651659154</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1">
-        <v>1651634414</v>
+        <v>1651654866</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1">
-        <v>1651633116</v>
+        <v>1651646933</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1">
-        <v>1651499797</v>
+        <v>1651644769</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>158</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>159</v>
@@ -2558,16 +2588,16 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1">
-        <v>1651487681</v>
+        <v>1651634414</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>161</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>162</v>
@@ -2578,36 +2608,36 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1">
-        <v>1651323746</v>
+        <v>1651633116</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1">
-        <v>1651312543</v>
+        <v>1651499797</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>168</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>169</v>
@@ -2618,16 +2648,16 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="1">
-        <v>1651295846</v>
+        <v>1651487681</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>171</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>172</v>
@@ -2638,7 +2668,7 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="1">
-        <v>1651045196</v>
+        <v>1651323746</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>174</v>
@@ -2647,7 +2677,7 @@
         <v>175</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>176</v>
@@ -2658,7 +2688,7 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="1">
-        <v>1651038505</v>
+        <v>1651312543</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>174</v>
@@ -2667,7 +2697,7 @@
         <v>178</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>179</v>
@@ -2678,7 +2708,7 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="1">
-        <v>1651029491</v>
+        <v>1651295846</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>174</v>
@@ -2687,7 +2717,7 @@
         <v>181</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>182</v>
@@ -2698,7 +2728,7 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="1">
-        <v>1650938536</v>
+        <v>1651045196</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>184</v>
@@ -2707,7 +2737,7 @@
         <v>185</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>186</v>
@@ -2718,182 +2748,242 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="1">
-        <v>1650877867</v>
+        <v>1651038505</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="1">
-        <v>1650852390</v>
+        <v>1651029491</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="1">
-        <v>1650701590</v>
+        <v>1650938536</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="1">
-        <v>1650355221</v>
+        <v>1650877867</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="1">
-        <v>1650113970</v>
+        <v>1650852390</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="1">
-        <v>1649752200</v>
+        <v>1650701590</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="1">
-        <v>1649474737</v>
+        <v>1650355221</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="F61" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="1">
-        <v>1648656738</v>
+        <v>1650113970</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="F62" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="1">
+        <v>1649752200</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="1">
+        <v>1649474737</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="1">
+        <v>1648656738</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="1">
         <v>1648381501</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>222</v>
+      <c r="B66" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2022-05-31 18:26:41
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233">
-  <si>
-    <t>发布编号</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242">
   <si>
     <t>发布日期</t>
   </si>
@@ -34,6 +31,45 @@
     <t>公众号链接</t>
   </si>
   <si>
+    <t>2022-05-30</t>
+  </si>
+  <si>
+    <t>Back to life | “灵感在线” 夏季周边设计大赛</t>
+  </si>
+  <si>
+    <t>JIers</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNHFqfJMycO2dibic9hpLxOafiaqce34xYdW6ZFfibKZibLvaXQAaCCEWAR28ficRztFiaveJGC1qXNGe6QUQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185797&amp;idx=1&amp;sn=583df7fa1bad87585e0a1a36444e4872&amp;chksm=8bfc24bdbc8badab8c057799cc9b3c1604c644c1d7a4e1beac7025987c64f250db5481633072#rd</t>
+  </si>
+  <si>
+    <t>青年大学习：学习习近平总书记给“国际青年领袖对话”项目外籍青年代表回信精神</t>
+  </si>
+  <si>
+    <t>JI青团</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4AS174Tw821oTqcznMB6yI1syMxezhQibgHE5icl07ekALXRCgJYLGN94FsLCLCl3MDJEdfvUVreomg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486319&amp;idx=1&amp;sn=6e951565810d42f521d6dae9eb330934&amp;chksm=fa3f12d1cd489bc74904fe9c7bedd465ed897121eb57adb284035315f21eda756d1990e73a36#rd</t>
+  </si>
+  <si>
+    <t>赛事相关 | 第八届中国国际“互联网+”大学生创新创业大赛</t>
+  </si>
+  <si>
+    <t>密院科协</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWkEKyssWic5OIwVtuvw7HQibibQuKWXVE83U1BMGabBicSgiabRobY2S75F7vMt0Opiapxth8HIRdXYT8Pw/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488296&amp;idx=1&amp;sn=ee28dcb53c3710abec89e6089f70f0f0&amp;chksm=97d0fd9fa0a77489d53393357853b655e107777a6f54d514dceb08164d198e9ff4cbd338525e#rd</t>
+  </si>
+  <si>
     <t>2022-05-29</t>
   </si>
   <si>
@@ -67,9 +103,6 @@
     <t>人民日报评论部：崇德向善、严守纪律——把青春播撒在民族复兴的征程上⑤</t>
   </si>
   <si>
-    <t>JI青团</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4BZcibEN1k9RxoEN0XLnO4ov0u4Za4fFpgyCMHJ2nib6gUGl4s0e5DPQDJWzttcfvBXibvicyHdPEz8wA/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -79,9 +112,6 @@
     <t>【推广】EECS专场 | 耶鲁、西北、UIUC！当前形势下，我该如何申请EECS？</t>
   </si>
   <si>
-    <t>JIers</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNHKYBDGQ7oiauy1QOLia0EBCwicY8aXmdHvHeibUO1JdqQ5MVLo0TXLrVj5o0n3blmg4WsZsB00h0yZZQ/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -161,9 +191,6 @@
   </si>
   <si>
     <t>换届通知 | 密院科协主席团及部长团换届通知</t>
-  </si>
-  <si>
-    <t>密院科协</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWlCKD9TF71qTBbDg7OpkibJWBc6qBD4a92JlJM3FfjxAVmSdvVASMI2evExEpVVGzI426fxiboiaIhng/0?wx_fmt=jpeg</t>
@@ -720,10 +747,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -748,16 +775,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -771,69 +790,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -849,7 +808,82 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -863,10 +897,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -876,13 +910,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -890,6 +917,48 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -899,7 +968,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -911,79 +1070,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -995,67 +1082,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1067,13 +1094,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1096,11 +1123,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1116,47 +1149,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1178,153 +1170,188 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1658,149 +1685,147 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F66"/>
+      <selection activeCell="A1" sqref="A1:F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>1653809321</v>
+        <v>1653893676</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>1653756447</v>
+        <v>1653918467</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>1653734498</v>
+        <v>1653915004</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>1653752093</v>
+        <v>1653809321</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>1653661410</v>
+        <v>1653756447</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>1653655336</v>
+        <v>1653734498</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>30</v>
@@ -1808,59 +1833,59 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>1653560174</v>
+        <v>1653752093</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>1653566952</v>
+        <v>1653661410</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>1653455486</v>
+        <v>1653655336</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>40</v>
@@ -1868,39 +1893,39 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>1653457678</v>
+        <v>1653560174</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1">
-        <v>1653488445</v>
+        <v>1653566952</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>46</v>
@@ -1908,7 +1933,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1">
-        <v>1653358054</v>
+        <v>1653455486</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>47</v>
@@ -1917,50 +1942,50 @@
         <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1">
-        <v>1653381370</v>
+        <v>1653457678</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1">
-        <v>1653400076</v>
+        <v>1653488445</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>56</v>
@@ -1968,7 +1993,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1">
-        <v>1653310453</v>
+        <v>1653358054</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>57</v>
@@ -1977,7 +2002,7 @@
         <v>58</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>59</v>
@@ -1988,596 +2013,596 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>1653206327</v>
+        <v>1653381370</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>1653112956</v>
+        <v>1653400076</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>1653106699</v>
+        <v>1653310453</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>1653103833</v>
+        <v>1653206327</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>1652946162</v>
+        <v>1653112956</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>1652766746</v>
+        <v>1653106699</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>1652711615</v>
+        <v>1653103833</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
-        <v>1652708097</v>
+        <v>1652946162</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
-        <v>1652633146</v>
+        <v>1652766746</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>1652502015</v>
+        <v>1652711615</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>1652423986</v>
+        <v>1652708097</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>1652196254</v>
+        <v>1652633146</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>1652156920</v>
+        <v>1652502015</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1">
-        <v>1652102252</v>
+        <v>1652423986</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
-        <v>1652082724</v>
+        <v>1652196254</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1">
-        <v>1652004475</v>
+        <v>1652156920</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1">
-        <v>1651989033</v>
+        <v>1652102252</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>1651923024</v>
+        <v>1652082724</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>1651902344</v>
+        <v>1652004475</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1">
-        <v>1651834916</v>
+        <v>1651989033</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1">
-        <v>1651834564</v>
+        <v>1651923024</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1">
-        <v>1651827827</v>
+        <v>1651902344</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1">
-        <v>1651827003</v>
+        <v>1651834916</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1">
-        <v>1651826605</v>
+        <v>1651834564</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1">
-        <v>1651820943</v>
+        <v>1651827827</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1">
-        <v>1651730520</v>
+        <v>1651827003</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>145</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>146</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1">
-        <v>1651659154</v>
+        <v>1651826605</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1">
-        <v>1651654866</v>
+        <v>1651820943</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1">
-        <v>1651646933</v>
+        <v>1651730520</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1">
-        <v>1651644769</v>
+        <v>1651659154</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>158</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>159</v>
@@ -2588,16 +2613,16 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1">
-        <v>1651634414</v>
+        <v>1651654866</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>161</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>162</v>
@@ -2608,16 +2633,16 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1">
-        <v>1651633116</v>
+        <v>1651646933</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>164</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>165</v>
@@ -2628,362 +2653,422 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1">
-        <v>1651499797</v>
+        <v>1651644769</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="1">
-        <v>1651487681</v>
+        <v>1651634414</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="1">
-        <v>1651323746</v>
+        <v>1651633116</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="1">
-        <v>1651312543</v>
+        <v>1651499797</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E52" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="1">
-        <v>1651295846</v>
+        <v>1651487681</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="1">
-        <v>1651045196</v>
+        <v>1651323746</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="1">
-        <v>1651038505</v>
+        <v>1651312543</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="1">
-        <v>1651029491</v>
+        <v>1651295846</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E56" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="1">
-        <v>1650938536</v>
+        <v>1651045196</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="1">
-        <v>1650877867</v>
+        <v>1651038505</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="1">
-        <v>1650852390</v>
+        <v>1651029491</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="1">
-        <v>1650701590</v>
+        <v>1650938536</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="1">
-        <v>1650355221</v>
+        <v>1650877867</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="F61" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="1">
-        <v>1650113970</v>
+        <v>1650852390</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="1">
-        <v>1649752200</v>
+        <v>1650701590</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="1">
-        <v>1649474737</v>
+        <v>1650355221</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="1">
-        <v>1648656738</v>
+        <v>1650113970</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="1">
+        <v>1649752200</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="1">
+        <v>1649474737</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="1">
+        <v>1648656738</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="1">
         <v>1648381501</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>232</v>
+      <c r="B69" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2022-06-08 19:00:41
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269">
   <si>
     <t>发布日期</t>
   </si>
@@ -797,6 +797,30 @@
   </si>
   <si>
     <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491470&amp;idx=1&amp;sn=9ae07a89758e30d73f6fe2868ff32be4&amp;chksm=ec0df69fdb7a7f89f3b898050fb3d9546846c42f58021e95e2ff02d40500b14c960e4b83bd7a#rd</t>
+  </si>
+  <si>
+    <t>2022-06-07</t>
+  </si>
+  <si>
+    <t>通知 | 关于开展2022年上海交通大学暑期社会实践的通知</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_png/QfDapvG9u4AmJ3iaZRWu8ZlB7ficzAEoXM0o3NLYG53goB7nr1kuOwvEicibDXWdD9Btq7Fwkj92KUMQDsjYsnd6qA/0?wx_fmt=png</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486349&amp;idx=1&amp;sn=4be0b005228f81c99e38b5610c9aa769&amp;chksm=fa3f1233cd489b25f15a87cdaf3173ffef923601b0096c30b2e20bc6157e14f730649f861680#rd</t>
+  </si>
+  <si>
+    <t>2022-06-06</t>
+  </si>
+  <si>
+    <t>新一期青年大学习来啦！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4DqIu8iccicyWEOzLmgsEGDsWKx0brvl21p54pndW57KibsUmWbgRYcibIRWa8b2xBmg6e6HRZx9rNaicA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486337&amp;idx=1&amp;sn=37f520d21e21fc4cfa82a1056a7f9690&amp;chksm=fa3f123fcd489b298963676544f00da8e408bfabdd7dedff9d7975ba67606f045fd0ee727048#rd</t>
   </si>
 </sst>
 </file>
@@ -805,9 +829,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -820,12 +844,49 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -840,38 +901,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -886,8 +923,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -895,14 +941,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -917,36 +971,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -954,15 +978,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -977,7 +1000,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -989,19 +1090,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1013,31 +1114,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1055,109 +1174,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1168,24 +1191,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1219,17 +1224,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1258,6 +1257,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1268,153 +1282,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1422,7 +1445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1745,10 +1768,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F74"/>
+      <selection activeCell="A1" sqref="A1:F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3231,6 +3254,46 @@
         <v>260</v>
       </c>
     </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="2">
+        <v>1654615201</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="2">
+        <v>1654524315</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2022-06-09 20:35:39
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280">
   <si>
     <t>发布日期</t>
   </si>
@@ -31,6 +31,69 @@
     <t>公众号链接</t>
   </si>
   <si>
+    <t>2022-06-09</t>
+  </si>
+  <si>
+    <t>服务月 | 当你一早醒来，蓝虎变成了.....</t>
+  </si>
+  <si>
+    <t>JIers</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNGhlic3CvsC1EDD26IYENNtj92PWZYqdMXcO0cCh4j217nMKiaEEneEn0pqWjic54dibAPOrqicfltqeFg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185867&amp;idx=1&amp;sn=2d4e3bfb8e4efeb4de9f3158763f3648&amp;chksm=8bfc24f3bc8bade52e450b1adeb5f1f398718ef7f79fc3f759811df8ce80408e4ac25e780ea1#rd</t>
+  </si>
+  <si>
+    <t>2022-06-08</t>
+  </si>
+  <si>
+    <t>服务月 | 手机版canvas app x 信息整合平台 x 密院12345 联合发布</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNHjckU4uv3EycF3IaT10icDKGOIKiacicKZD8oByicAClUdhXgsgOKVtnmpBb5dRZR51VRliapvNdrNic9w/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185851&amp;idx=1&amp;sn=99cff554bfa2ff09f2a36342c5348803&amp;chksm=8bfc2483bc8bad95849cb5775bc946e78b747fbbc5d67be7e035f4dc568b4d1b3556e8e76a10#rd</t>
+  </si>
+  <si>
+    <t>交大密西根学院夏季学期云端自习室上线啦！</t>
+  </si>
+  <si>
+    <t>JI青团</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4D7vGvOvz0xzibptAbpN8v2VFwuwzxwx4P3pR43gSue5mZficTH0InT3P953WTag8xylxAvnqkUk6icg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486353&amp;idx=1&amp;sn=9c58a974da912ea5870364c627677120&amp;chksm=fa3f122fcd489b39049f8b8c397945a354ec67a3677c0c7522d2370cc321ac7d585528d416d3#rd</t>
+  </si>
+  <si>
+    <t>2022-06-07</t>
+  </si>
+  <si>
+    <t>通知 | 关于开展2022年上海交通大学暑期社会实践的通知</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_png/QfDapvG9u4AmJ3iaZRWu8ZlB7ficzAEoXM0o3NLYG53goB7nr1kuOwvEicibDXWdD9Btq7Fwkj92KUMQDsjYsnd6qA/0?wx_fmt=png</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486349&amp;idx=1&amp;sn=4be0b005228f81c99e38b5610c9aa769&amp;chksm=fa3f1233cd489b25f15a87cdaf3173ffef923601b0096c30b2e20bc6157e14f730649f861680#rd</t>
+  </si>
+  <si>
+    <t>2022-06-06</t>
+  </si>
+  <si>
+    <t>新一期青年大学习来啦！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4DqIu8iccicyWEOzLmgsEGDsWKx0brvl21p54pndW57KibsUmWbgRYcibIRWa8b2xBmg6e6HRZx9rNaicA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486337&amp;idx=1&amp;sn=37f520d21e21fc4cfa82a1056a7f9690&amp;chksm=fa3f123fcd489b298963676544f00da8e408bfabdd7dedff9d7975ba67606f045fd0ee727048#rd</t>
+  </si>
+  <si>
     <t>2022-06-04</t>
   </si>
   <si>
@@ -64,9 +127,6 @@
     <t>服务月 | 夏季权益问题反馈 · 重点问题定点调研 · FOR BETTER SUMMER</t>
   </si>
   <si>
-    <t>JIers</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNEYOf3xlHvztPduN27SkoQkviaKQibDQR35QzSa6L1zuz1kk9mhVy8svicQyrD4wCQibLSgxoMasbFwrA/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -112,9 +172,6 @@
     <t>青年大学习：学习习近平总书记给“国际青年领袖对话”项目外籍青年代表回信精神</t>
   </si>
   <si>
-    <t>JI青团</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4AS174Tw821oTqcznMB6yI1syMxezhQibgHE5icl07ekALXRCgJYLGN94FsLCLCl3MDJEdfvUVreomg/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -797,30 +854,6 @@
   </si>
   <si>
     <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491470&amp;idx=1&amp;sn=9ae07a89758e30d73f6fe2868ff32be4&amp;chksm=ec0df69fdb7a7f89f3b898050fb3d9546846c42f58021e95e2ff02d40500b14c960e4b83bd7a#rd</t>
-  </si>
-  <si>
-    <t>2022-06-07</t>
-  </si>
-  <si>
-    <t>通知 | 关于开展2022年上海交通大学暑期社会实践的通知</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_png/QfDapvG9u4AmJ3iaZRWu8ZlB7ficzAEoXM0o3NLYG53goB7nr1kuOwvEicibDXWdD9Btq7Fwkj92KUMQDsjYsnd6qA/0?wx_fmt=png</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486349&amp;idx=1&amp;sn=4be0b005228f81c99e38b5610c9aa769&amp;chksm=fa3f1233cd489b25f15a87cdaf3173ffef923601b0096c30b2e20bc6157e14f730649f861680#rd</t>
-  </si>
-  <si>
-    <t>2022-06-06</t>
-  </si>
-  <si>
-    <t>新一期青年大学习来啦！</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4DqIu8iccicyWEOzLmgsEGDsWKx0brvl21p54pndW57KibsUmWbgRYcibIRWa8b2xBmg6e6HRZx9rNaicA/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486337&amp;idx=1&amp;sn=37f520d21e21fc4cfa82a1056a7f9690&amp;chksm=fa3f123fcd489b298963676544f00da8e408bfabdd7dedff9d7975ba67606f045fd0ee727048#rd</t>
   </si>
 </sst>
 </file>
@@ -828,10 +861,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -844,12 +877,20 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="0"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -864,24 +905,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -892,39 +918,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -940,6 +935,45 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -947,16 +981,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -976,20 +1024,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1000,7 +1034,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1012,31 +1082,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1048,91 +1112,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1144,25 +1130,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1180,7 +1148,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1209,6 +1243,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1220,24 +1278,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1257,17 +1297,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1296,142 +1330,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1768,10 +1802,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F76"/>
+      <selection activeCell="A1" sqref="A1:F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1796,7 +1830,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>1654337062</v>
+        <v>1654746363</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1816,16 +1850,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>1654328621</v>
+        <v>1654683827</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
@@ -1836,76 +1870,76 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>1654228442</v>
+        <v>1654696237</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>1654153902</v>
+        <v>1654615201</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>1654091999</v>
+        <v>1654524315</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>1653893676</v>
+        <v>1654337062</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>29</v>
@@ -1916,10 +1950,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>1653918467</v>
+        <v>1654328621</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>31</v>
@@ -1936,16 +1970,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>1653915004</v>
+        <v>1654228442</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>37</v>
@@ -1956,7 +1990,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>1653809321</v>
+        <v>1654153902</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>39</v>
@@ -1976,16 +2010,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
-        <v>1653756447</v>
+        <v>1654091999</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>45</v>
@@ -1996,7 +2030,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2">
-        <v>1653734498</v>
+        <v>1653893676</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>47</v>
@@ -2005,7 +2039,7 @@
         <v>48</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>49</v>
@@ -2016,7 +2050,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2">
-        <v>1653752093</v>
+        <v>1653918467</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>47</v>
@@ -2025,7 +2059,7 @@
         <v>51</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>52</v>
@@ -2036,16 +2070,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2">
-        <v>1653661410</v>
+        <v>1653915004</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>56</v>
@@ -2056,476 +2090,476 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2">
-        <v>1653655336</v>
+        <v>1653809321</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>1653560174</v>
+        <v>1653756447</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>1653566952</v>
+        <v>1653734498</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>1653455486</v>
+        <v>1653752093</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>1653457678</v>
+        <v>1653661410</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>1653488445</v>
+        <v>1653655336</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>1653358054</v>
+        <v>1653560174</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>1653381370</v>
+        <v>1653566952</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>1653400076</v>
+        <v>1653455486</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>1653310453</v>
+        <v>1653457678</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>1653206327</v>
+        <v>1653488445</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>1653112956</v>
+        <v>1653358054</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>1653106699</v>
+        <v>1653381370</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>1653103833</v>
+        <v>1653400076</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>1652946162</v>
+        <v>1653310453</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>1652766746</v>
+        <v>1653206327</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2">
-        <v>1652711615</v>
+        <v>1653112956</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>1652708097</v>
+        <v>1653106699</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2">
-        <v>1652633146</v>
+        <v>1653103833</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2">
-        <v>1652502015</v>
+        <v>1652946162</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2">
-        <v>1652423986</v>
+        <v>1652766746</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2">
-        <v>1652196254</v>
+        <v>1652711615</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2">
-        <v>1652156920</v>
+        <v>1652708097</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2">
-        <v>1652102252</v>
+        <v>1652633146</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>137</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>138</v>
@@ -2536,287 +2570,287 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2">
-        <v>1652082724</v>
+        <v>1652502015</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2">
-        <v>1652004475</v>
+        <v>1652423986</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2">
-        <v>1651989033</v>
+        <v>1652196254</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2">
-        <v>1651923024</v>
+        <v>1652156920</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2">
-        <v>1651902344</v>
+        <v>1652102252</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2">
-        <v>1651834916</v>
+        <v>1652082724</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2">
-        <v>1651834564</v>
+        <v>1652004475</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2">
-        <v>1651827827</v>
+        <v>1651989033</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2">
-        <v>1651827003</v>
+        <v>1651923024</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2">
-        <v>1651826605</v>
+        <v>1651902344</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2">
-        <v>1651820943</v>
+        <v>1651834916</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2">
-        <v>1651730520</v>
+        <v>1651834564</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2">
-        <v>1651659154</v>
+        <v>1651827827</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>176</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2">
-        <v>1651654866</v>
+        <v>1651827003</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>176</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2">
-        <v>1651646933</v>
+        <v>1651826605</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>176</v>
@@ -2825,327 +2859,327 @@
         <v>183</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>184</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2">
-        <v>1651644769</v>
+        <v>1651820943</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>176</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2">
-        <v>1651634414</v>
+        <v>1651730520</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2">
-        <v>1651633116</v>
+        <v>1651659154</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2">
-        <v>1651499797</v>
+        <v>1651654866</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>195</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>1651487681</v>
+        <v>1651646933</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>195</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2">
-        <v>1651323746</v>
+        <v>1651644769</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2">
-        <v>1651312543</v>
+        <v>1651634414</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2">
-        <v>1651295846</v>
+        <v>1651633116</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2">
-        <v>1651045196</v>
+        <v>1651499797</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2">
-        <v>1651038505</v>
+        <v>1651487681</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2">
-        <v>1651029491</v>
+        <v>1651323746</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2">
-        <v>1650938536</v>
+        <v>1651312543</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2">
-        <v>1650877867</v>
+        <v>1651295846</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2">
-        <v>1650852390</v>
+        <v>1651045196</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2">
-        <v>1650701590</v>
+        <v>1651038505</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2">
-        <v>1650355221</v>
+        <v>1651029491</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>238</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>239</v>
@@ -3156,7 +3190,7 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2">
-        <v>1650113970</v>
+        <v>1650938536</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>241</v>
@@ -3165,7 +3199,7 @@
         <v>242</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>243</v>
@@ -3176,7 +3210,7 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2">
-        <v>1649752200</v>
+        <v>1650877867</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>245</v>
@@ -3196,102 +3230,162 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2">
-        <v>1649474737</v>
+        <v>1650852390</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="D72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E72" s="2" t="s">
+      <c r="F72" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2">
-        <v>1648656738</v>
+        <v>1650701590</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="D73" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2">
-        <v>1648381501</v>
+        <v>1650355221</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="D74" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E74" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2">
-        <v>1654615201</v>
+        <v>1650113970</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E75" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2">
-        <v>1654524315</v>
+        <v>1649752200</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="F76" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="2">
+        <v>1649474737</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E76" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>268</v>
+      <c r="E77" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="2">
+        <v>1648656738</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="2">
+        <v>1648381501</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2022-06-11 15:14:44
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283">
   <si>
     <t>发布日期</t>
   </si>
@@ -46,6 +46,18 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185867&amp;idx=1&amp;sn=2d4e3bfb8e4efeb4de9f3158763f3648&amp;chksm=8bfc24f3bc8bade52e450b1adeb5f1f398718ef7f79fc3f759811df8ce80408e4ac25e780ea1#rd</t>
   </si>
   <si>
+    <t>回顾｜研究生申请workshop for DDers (CE/EE/IOE专场)</t>
+  </si>
+  <si>
+    <t>JIAdvisingCenter</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMhfgY8NzZpoBjzaTTmvibAAlBuAOdoHrabH3E2nL8Y2HO6TErbticAprk0wqLLJtjjJZv4YlVDClAFA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484441&amp;idx=1&amp;sn=3d0a7f98a3bd02976b0e45220c438a38&amp;chksm=fbeb93a4cc9c1ab25d4347f51790d03ba7bf3d78a5ddeed62ba5dfebfd04f08fecc109855bda#rd</t>
+  </si>
+  <si>
     <t>2022-06-08</t>
   </si>
   <si>
@@ -203,9 +215,6 @@
   </si>
   <si>
     <t>研究生申请&amp;生涯发展经验分享会 | For DDers (CE/EE/IOE专场)</t>
-  </si>
-  <si>
-    <t>JIAdvisingCenter</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMiaqQz5WPAGMHUvEZ9SNcyN4QXXC1jtEkNFc1fUXoiczUlicT3B1YjfuM5Pz5fUdtsB9BPLWLVvHUhqQ/0?wx_fmt=jpeg</t>
@@ -862,9 +871,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -890,7 +899,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -898,44 +923,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -950,16 +937,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -975,36 +954,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1019,7 +969,66 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1034,7 +1043,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1046,7 +1085,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1058,31 +1115,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1094,13 +1139,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1118,7 +1157,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1130,25 +1175,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1160,61 +1205,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1228,17 +1237,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1282,6 +1285,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1293,15 +1311,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1330,142 +1339,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1802,15 +1811,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F79"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:G80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1827,8 +1836,9 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1654746363</v>
       </c>
@@ -1847,19 +1857,20 @@
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
-        <v>1654683827</v>
+        <v>1654784264</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
@@ -1867,19 +1878,20 @@
       <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
-        <v>1654696237</v>
+        <v>1654683827</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -1887,19 +1899,20 @@
       <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
-        <v>1654615201</v>
+        <v>1654696237</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>20</v>
@@ -1907,10 +1920,11 @@
       <c r="F5" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
-        <v>1654524315</v>
+        <v>1654615201</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -1919,7 +1933,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>24</v>
@@ -1927,10 +1941,11 @@
       <c r="F6" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
-        <v>1654337062</v>
+        <v>1654524315</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>26</v>
@@ -1939,21 +1954,22 @@
         <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2">
+        <v>1654337062</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2">
-        <v>1654328621</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>31</v>
@@ -1967,19 +1983,20 @@
       <c r="F8" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
-        <v>1654228442</v>
+        <v>1654328621</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>37</v>
@@ -1987,10 +2004,11 @@
       <c r="F9" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
-        <v>1654153902</v>
+        <v>1654228442</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>39</v>
@@ -2007,10 +2025,11 @@
       <c r="F10" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
-        <v>1654091999</v>
+        <v>1654153902</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>43</v>
@@ -2019,7 +2038,7 @@
         <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>45</v>
@@ -2027,10 +2046,11 @@
       <c r="F11" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
-        <v>1653893676</v>
+        <v>1654091999</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>47</v>
@@ -2039,7 +2059,7 @@
         <v>48</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>49</v>
@@ -2047,39 +2067,41 @@
       <c r="F12" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
+        <v>1653893676</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2">
         <v>1653918467</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2">
-        <v>1653915004</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>56</v>
@@ -2087,19 +2109,20 @@
       <c r="F14" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
-        <v>1653809321</v>
+        <v>1653915004</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>60</v>
@@ -2107,19 +2130,20 @@
       <c r="F15" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2">
-        <v>1653756447</v>
+        <v>1653809321</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>64</v>
@@ -2127,39 +2151,41 @@
       <c r="F16" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
+        <v>1653756447</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2">
         <v>1653734498</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2">
-        <v>1653752093</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>71</v>
@@ -2167,119 +2193,125 @@
       <c r="F18" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
+        <v>1653752093</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2">
         <v>1653661410</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="2">
-        <v>1653655336</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>77</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>79</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
-        <v>1653560174</v>
+        <v>1653655336</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="2">
+        <v>1653560174</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="2">
-        <v>1653566952</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>83</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>85</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="2">
-        <v>1653455486</v>
+        <v>1653566952</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2">
+        <v>1653455486</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="2">
-        <v>1653457678</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>90</v>
@@ -2287,19 +2319,20 @@
       <c r="F24" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="2">
-        <v>1653488445</v>
+        <v>1653457678</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>93</v>
@@ -2307,39 +2340,41 @@
       <c r="F25" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="2">
+        <v>1653488445</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2">
         <v>1653358054</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="2">
-        <v>1653381370</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>100</v>
@@ -2347,93 +2382,98 @@
       <c r="F27" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="2">
-        <v>1653400076</v>
+        <v>1653381370</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>102</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>104</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="2">
-        <v>1653310453</v>
+        <v>1653400076</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>105</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="2">
+        <v>1653310453</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="2">
+      <c r="C30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="2">
         <v>1653206327</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="2">
-        <v>1653112956</v>
-      </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="2">
+        <v>1653112956</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="2">
-        <v>1653106699</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>116</v>
@@ -2447,19 +2487,20 @@
       <c r="F32" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="2">
-        <v>1653103833</v>
+        <v>1653106699</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>119</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>120</v>
@@ -2467,79 +2508,83 @@
       <c r="F33" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="2">
+        <v>1653103833</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="2">
         <v>1652946162</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="B35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="2">
+      <c r="E35" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2">
         <v>1652766746</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="2">
+      <c r="C36" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2">
         <v>1652711615</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="2">
-        <v>1652708097</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>134</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>135</v>
@@ -2547,19 +2592,20 @@
       <c r="F37" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="2">
-        <v>1652633146</v>
+        <v>1652708097</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>137</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>138</v>
@@ -2567,79 +2613,83 @@
       <c r="F38" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="2">
+        <v>1652633146</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2">
         <v>1652502015</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="2">
+      <c r="C40" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2">
         <v>1652423986</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="2">
+      <c r="C41" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="2">
         <v>1652196254</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="2">
-        <v>1652156920</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>152</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>153</v>
@@ -2647,39 +2697,41 @@
       <c r="F42" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="2">
+        <v>1652156920</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="2">
         <v>1652102252</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="2">
-        <v>1652082724</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>159</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>160</v>
@@ -2687,39 +2739,41 @@
       <c r="F44" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="2">
+        <v>1652082724</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="2">
         <v>1652004475</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="2">
-        <v>1651989033</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>166</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>167</v>
@@ -2727,39 +2781,41 @@
       <c r="F46" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="2">
+        <v>1651989033</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="2">
         <v>1651923024</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="2">
-        <v>1651902344</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>173</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>174</v>
@@ -2767,39 +2823,41 @@
       <c r="F48" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="2">
+        <v>1651902344</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="2">
         <v>1651834916</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="2">
-        <v>1651834564</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>181</v>
@@ -2807,19 +2865,20 @@
       <c r="F50" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="2">
-        <v>1651827827</v>
+        <v>1651834564</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>183</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>184</v>
@@ -2827,119 +2886,125 @@
       <c r="F51" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="2">
+        <v>1651827827</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="2">
         <v>1651827003</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F52" s="2" t="s">
+      <c r="B53" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="2">
+      <c r="D53" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="2">
         <v>1651826605</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F53" s="2" t="s">
+      <c r="B54" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="2">
-        <v>1651820943</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="2">
+        <v>1651820943</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="2">
         <v>1651730520</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D55" s="2" t="s">
+      <c r="B56" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="2">
+      <c r="E56" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="2">
         <v>1651659154</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="2">
-        <v>1651654866</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>199</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>200</v>
@@ -2947,19 +3012,20 @@
       <c r="F57" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="2">
-        <v>1651646933</v>
+        <v>1651654866</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>202</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>203</v>
@@ -2967,19 +3033,20 @@
       <c r="F58" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="2">
-        <v>1651644769</v>
+        <v>1651646933</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>205</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>206</v>
@@ -2987,19 +3054,20 @@
       <c r="F59" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="2">
-        <v>1651634414</v>
+        <v>1651644769</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>208</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>209</v>
@@ -3007,19 +3075,20 @@
       <c r="F60" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="2">
-        <v>1651633116</v>
+        <v>1651634414</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>211</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>212</v>
@@ -3027,39 +3096,41 @@
       <c r="F61" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="2">
+        <v>1651633116</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="2">
         <v>1651499797</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="F62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="2">
-        <v>1651487681</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>219</v>
@@ -3067,39 +3138,41 @@
       <c r="F63" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="2">
+        <v>1651487681</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="2">
         <v>1651323746</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="F64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="2">
-        <v>1651312543</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>225</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>226</v>
@@ -3107,19 +3180,20 @@
       <c r="F65" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="2">
-        <v>1651295846</v>
+        <v>1651312543</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>228</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>229</v>
@@ -3127,39 +3201,41 @@
       <c r="F66" s="2" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="2">
+        <v>1651295846</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="2">
         <v>1651045196</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="F67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="2">
-        <v>1651038505</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>235</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>236</v>
@@ -3167,19 +3243,20 @@
       <c r="F68" s="2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="2">
-        <v>1651029491</v>
+        <v>1651038505</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>238</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>239</v>
@@ -3187,59 +3264,62 @@
       <c r="F69" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="2">
+        <v>1651029491</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="2">
         <v>1650938536</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="2">
+      <c r="C71" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="2">
         <v>1650877867</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="F71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="2">
-        <v>1650852390</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>249</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>250</v>
@@ -3247,146 +3327,175 @@
       <c r="F72" s="2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="2">
+        <v>1650852390</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="2">
         <v>1650701590</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="F73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="2">
+      <c r="C74" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="2">
         <v>1650355221</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="F74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="2">
-        <v>1650113970</v>
-      </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E75" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="2">
+        <v>1650113970</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="2">
+      <c r="C76" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="2">
         <v>1649752200</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="F76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="2">
-        <v>1649474737</v>
-      </c>
-      <c r="B77" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E77" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="2">
+        <v>1649474737</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="2">
+      <c r="C78" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="2">
         <v>1648656738</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="D78" s="2" t="s">
+      <c r="B79" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="2">
+        <v>1648381501</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E78" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="2">
-        <v>1648381501</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>279</v>
-      </c>
+      <c r="E80" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G80" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Site updated: 2022-06-16 23:35:19
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332">
   <si>
     <t>发布日期</t>
   </si>
@@ -31,9 +31,112 @@
     <t>公众号链接</t>
   </si>
   <si>
+    <t>2022-06-16</t>
+  </si>
+  <si>
+    <t>招募令|“交阳似火”暑期社会实践报名</t>
+  </si>
+  <si>
+    <t>JI觅源</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5RCBmHib6ooicpibUDm0Rbzp895WrfaWe7Bc2eZTwia4PsWVawcGTrm2xgqumGyFDoSGg5d1mSklH9FXQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzAwNTYxNzk3Mw==&amp;mid=2648011717&amp;idx=1&amp;sn=3ae100b85ad81c236cbfd2a35595607a&amp;chksm=8338339fb44fba89bcdd1118c15cee0e851cd4dc375c110cb72eaf4933cff317e610a6c30aa0#rd</t>
+  </si>
+  <si>
+    <t>6.16天气预报</t>
+  </si>
+  <si>
+    <t>密院气象</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/ic56fiaeKmYMA2iaA6K6ACfOFuoIvDicia2TdQxFCiazAibeGpAwwzDr4B1ugWvsictfflBdZTodl3SQg7rtLpDdPkaQFQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483736&amp;idx=1&amp;sn=b1137ffd0cfd68e5794ca845d56c0e5f&amp;chksm=c02ab842f75d315459af6ed12611115b00580012cdf78a8f2c73126447577d53e7417dc70176#rd</t>
+  </si>
+  <si>
+    <t>2022-06-15</t>
+  </si>
+  <si>
+    <t>万般玩趣 | 召集令成果反馈！</t>
+  </si>
+  <si>
+    <t>JIers</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNGnOqjX9BBzhbkylTfN0TkGwLTianyqaCayPdYN8Rb89Re7CYTrMLeL7VicOBiafs9sibJafwTKQ1YOgA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185926&amp;idx=1&amp;sn=3ec6849e7a2fc5a8e6bcab4364c3be6b&amp;chksm=8bfc253ebc8bac28dfc3d39839076d707eac5ff567bb5c86f5f807211ab7f555ca2d1aa6b70e#rd</t>
+  </si>
+  <si>
+    <t>6.15天气预报</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483734&amp;idx=1&amp;sn=4c08fe25912365143a20fb6a82388812&amp;chksm=c02ab84cf75d315acdbfda65826c84a91fd380530b4fca4d10405e83f88c75e3e25bf04da81b#rd</t>
+  </si>
+  <si>
+    <t>2022-06-14</t>
+  </si>
+  <si>
+    <t>志愿者群像 | 线上陪伴，用心呵“沪”</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/LYfalg5ibn0BagfEbvGBJYTw2PQqWp6R0Phuan37RjjzF57vpqztNrsHxgLQEIibzdLwq0fNibdd9iaYOPUoNPeApg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzAwNTYxNzk3Mw==&amp;mid=2648011595&amp;idx=1&amp;sn=3a175647577957414ade8d54eaf3453d&amp;chksm=83383311b44fba079a2c419b42092ea09a31c7edf33db981044dc6b045e7f9fc7c777c0a3d5a#rd</t>
+  </si>
+  <si>
+    <t>6.14天气预报</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/ic56fiaeKmYMDmFxRMibEFTK9hAyfUlcgdNwR0CjvvVjffnc0VhQyNgJbVO4OcsgYye26d3J9pNuxgibdIhqTD1sgA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483730&amp;idx=1&amp;sn=90bdf740a179109ffdb14f79c4510e0f&amp;chksm=c02ab848f75d315e622dd3cb40624454509725995e2e9344c870b9a64b1a70c498e6a6ea7978#rd</t>
+  </si>
+  <si>
+    <t>2022-06-13</t>
+  </si>
+  <si>
+    <t>叮咚，青年大学习来啦</t>
+  </si>
+  <si>
+    <t>JI青团</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4CuQBibeZ4MPQtYrgXu0ldplEmibzan1rd5XDULibnKfVueAuwL8C0oUXxPofibr8IWsiamvgeSyGFciaQw/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486369&amp;idx=1&amp;sn=41ebde5e85d4236ab08716c6c8a6555f&amp;chksm=fa3f121fcd489b097af59157db93f5e3c599c9b2fc95a97232c728e420d1ff019ce8c4efb2d2#rd</t>
+  </si>
+  <si>
+    <t>【入梅第二天，今明依然是以小雨为主午后有雷雨的配置，17日后主雨带北抬，本市降水过程增多，本市常年梅雨长达25天，平均降水量250mm】
+密院气象2022/6/13 7时发布6月13/14日天气预报：
+13日，中雨转小雨，东到东南风3-4级，21-25度，相对湿度65%-95%，空气质量优。
+14日，阴，午后有雷阵雨，东南风4-5级，22-28度，相对湿度75%-100%，空气质量优。
+安娜堡天气预报：
+【预计15、16两日天气晴朗，最高气温可达34度以上，气温变化剧烈且多阵雨天气】
+13日：阴有阵雨，14-25度，降水概率中，东南风3级
+14日：雷阵雨转多云，17-30度，降水概率中，静风</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483726&amp;idx=1&amp;sn=e0fccdab4564269f6bc8b7043ac0f86a&amp;chksm=c02ab854f75d31423168e274ec76c40bf7c2eb78bdedfb66b303202d6dc5ef182e732393817d#rd</t>
+  </si>
+  <si>
     <t>2022-06-12</t>
   </si>
   <si>
+    <t>测试：即日起，每天早晨的校园气象预报信息将同步由公众号发布</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483724&amp;idx=1&amp;sn=4d1c80549340988ddef7d1579c78e076&amp;chksm=c02ab856f75d3140a7c5c873d08e110d76aec0ec8033e24926291eb85652e700ff5696993047#rd</t>
+  </si>
+  <si>
     <t>赛事相关 | 2022年度上海交通大学“数学建模培训营”研赛招生通知</t>
   </si>
   <si>
@@ -49,33 +152,39 @@
     <t>2022-06-09</t>
   </si>
   <si>
+    <t>回顾｜研究生申请workshop for DDers (CE/EE/IOE专场)</t>
+  </si>
+  <si>
+    <t>JIAdvisingCenter</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMhfgY8NzZpoBjzaTTmvibAAlBuAOdoHrabH3E2nL8Y2HO6TErbticAprk0wqLLJtjjJZv4YlVDClAFA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484441&amp;idx=1&amp;sn=3d0a7f98a3bd02976b0e45220c438a38&amp;chksm=fbeb93a4cc9c1ab25d4347f51790d03ba7bf3d78a5ddeed62ba5dfebfd04f08fecc109855bda#rd</t>
+  </si>
+  <si>
     <t>服务月 | 当你一早醒来，蓝虎变成了.....</t>
   </si>
   <si>
-    <t>JIers</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNGhlic3CvsC1EDD26IYENNtj92PWZYqdMXcO0cCh4j217nMKiaEEneEn0pqWjic54dibAPOrqicfltqeFg/0?wx_fmt=jpeg</t>
   </si>
   <si>
     <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185867&amp;idx=1&amp;sn=2d4e3bfb8e4efeb4de9f3158763f3648&amp;chksm=8bfc24f3bc8bade52e450b1adeb5f1f398718ef7f79fc3f759811df8ce80408e4ac25e780ea1#rd</t>
   </si>
   <si>
-    <t>回顾｜研究生申请workshop for DDers (CE/EE/IOE专场)</t>
-  </si>
-  <si>
-    <t>JIAdvisingCenter</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMhfgY8NzZpoBjzaTTmvibAAlBuAOdoHrabH3E2nL8Y2HO6TErbticAprk0wqLLJtjjJZv4YlVDClAFA/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484441&amp;idx=1&amp;sn=3d0a7f98a3bd02976b0e45220c438a38&amp;chksm=fbeb93a4cc9c1ab25d4347f51790d03ba7bf3d78a5ddeed62ba5dfebfd04f08fecc109855bda#rd</t>
-  </si>
-  <si>
     <t>2022-06-08</t>
   </si>
   <si>
+    <t>交大密西根学院夏季学期云端自习室上线啦！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4D7vGvOvz0xzibptAbpN8v2VFwuwzxwx4P3pR43gSue5mZficTH0InT3P953WTag8xylxAvnqkUk6icg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486353&amp;idx=1&amp;sn=9c58a974da912ea5870364c627677120&amp;chksm=fa3f122fcd489b39049f8b8c397945a354ec67a3677c0c7522d2370cc321ac7d585528d416d3#rd</t>
+  </si>
+  <si>
     <t>服务月 | 手机版canvas app x 信息整合平台 x 密院12345 联合发布</t>
   </si>
   <si>
@@ -85,18 +194,6 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185851&amp;idx=1&amp;sn=99cff554bfa2ff09f2a36342c5348803&amp;chksm=8bfc2483bc8bad95849cb5775bc946e78b747fbbc5d67be7e035f4dc568b4d1b3556e8e76a10#rd</t>
   </si>
   <si>
-    <t>交大密西根学院夏季学期云端自习室上线啦！</t>
-  </si>
-  <si>
-    <t>JI青团</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4D7vGvOvz0xzibptAbpN8v2VFwuwzxwx4P3pR43gSue5mZficTH0InT3P953WTag8xylxAvnqkUk6icg/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486353&amp;idx=1&amp;sn=9c58a974da912ea5870364c627677120&amp;chksm=fa3f122fcd489b39049f8b8c397945a354ec67a3677c0c7522d2370cc321ac7d585528d416d3#rd</t>
-  </si>
-  <si>
     <t>2022-06-07</t>
   </si>
   <si>
@@ -139,9 +236,6 @@
     <t>云托班志愿者信息统计</t>
   </si>
   <si>
-    <t>JI觅源</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5QqpMZ45ribYngdYEC1qJAnvqDiciaia79e09wlH2tjyd0JDQacf52vic8wO2AlNH0zKtoqibCpCkCibyLcg/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -187,6 +281,24 @@
     <t>2022-05-30</t>
   </si>
   <si>
+    <t>青年大学习：学习习近平总书记给“国际青年领袖对话”项目外籍青年代表回信精神</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4AS174Tw821oTqcznMB6yI1syMxezhQibgHE5icl07ekALXRCgJYLGN94FsLCLCl3MDJEdfvUVreomg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486319&amp;idx=1&amp;sn=6e951565810d42f521d6dae9eb330934&amp;chksm=fa3f12d1cd489bc74904fe9c7bedd465ed897121eb57adb284035315f21eda756d1990e73a36#rd</t>
+  </si>
+  <si>
+    <t>赛事相关 | 第八届中国国际“互联网+”大学生创新创业大赛</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWkEKyssWic5OIwVtuvw7HQibibQuKWXVE83U1BMGabBicSgiabRobY2S75F7vMt0Opiapxth8HIRdXYT8Pw/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488296&amp;idx=1&amp;sn=ee28dcb53c3710abec89e6089f70f0f0&amp;chksm=97d0fd9fa0a77489d53393357853b655e107777a6f54d514dceb08164d198e9ff4cbd338525e#rd</t>
+  </si>
+  <si>
     <t>Back to life | “灵感在线” 夏季周边设计大赛</t>
   </si>
   <si>
@@ -196,24 +308,6 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185797&amp;idx=1&amp;sn=583df7fa1bad87585e0a1a36444e4872&amp;chksm=8bfc24bdbc8badab8c057799cc9b3c1604c644c1d7a4e1beac7025987c64f250db5481633072#rd</t>
   </si>
   <si>
-    <t>青年大学习：学习习近平总书记给“国际青年领袖对话”项目外籍青年代表回信精神</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4AS174Tw821oTqcznMB6yI1syMxezhQibgHE5icl07ekALXRCgJYLGN94FsLCLCl3MDJEdfvUVreomg/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486319&amp;idx=1&amp;sn=6e951565810d42f521d6dae9eb330934&amp;chksm=fa3f12d1cd489bc74904fe9c7bedd465ed897121eb57adb284035315f21eda756d1990e73a36#rd</t>
-  </si>
-  <si>
-    <t>赛事相关 | 第八届中国国际“互联网+”大学生创新创业大赛</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/jcRlSfwIXWkEKyssWic5OIwVtuvw7HQibibQuKWXVE83U1BMGabBicSgiabRobY2S75F7vMt0Opiapxth8HIRdXYT8Pw/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488296&amp;idx=1&amp;sn=ee28dcb53c3710abec89e6089f70f0f0&amp;chksm=97d0fd9fa0a77489d53393357853b655e107777a6f54d514dceb08164d198e9ff4cbd338525e#rd</t>
-  </si>
-  <si>
     <t>2022-05-29</t>
   </si>
   <si>
@@ -238,6 +332,15 @@
     <t>2022-05-28</t>
   </si>
   <si>
+    <t>【推广】EECS专场 | 耶鲁、西北、UIUC！当前形势下，我该如何申请EECS？</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNHKYBDGQ7oiauy1QOLia0EBCwicY8aXmdHvHeibUO1JdqQ5MVLo0TXLrVj5o0n3blmg4WsZsB00h0yZZQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185782&amp;idx=2&amp;sn=2bf72405fd4782c9dbd20a5ea80058ff&amp;chksm=8bfc244ebc8bad5875cfbad7136894091e9fa26380609c8a5fd82e0519cfca4b16d3f4182925#rd</t>
+  </si>
+  <si>
     <t>人民日报评论部：崇德向善、严守纪律——把青春播撒在民族复兴的征程上⑤</t>
   </si>
   <si>
@@ -247,15 +350,6 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486301&amp;idx=1&amp;sn=2fa7e5ccab9f282fa61b91f8c513ff77&amp;chksm=fa3f12e3cd489bf58d4bc50da91bd1cc00592253bb7645dcb42195333f466429271c80abbbcb#rd</t>
   </si>
   <si>
-    <t>【推广】EECS专场 | 耶鲁、西北、UIUC！当前形势下，我该如何申请EECS？</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNHKYBDGQ7oiauy1QOLia0EBCwicY8aXmdHvHeibUO1JdqQ5MVLo0TXLrVj5o0n3blmg4WsZsB00h0yZZQ/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185782&amp;idx=2&amp;sn=2bf72405fd4782c9dbd20a5ea80058ff&amp;chksm=8bfc244ebc8bad5875cfbad7136894091e9fa26380609c8a5fd82e0519cfca4b16d3f4182925#rd</t>
-  </si>
-  <si>
     <t>2022-05-27</t>
   </si>
   <si>
@@ -277,6 +371,12 @@
     <t>2022-05-26</t>
   </si>
   <si>
+    <t>人民日报评论部：敢于斗争、善于斗争——把青春播撒在民族复兴的征程上③</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486295&amp;idx=1&amp;sn=f14ac378113a19fd357d4e22f749d11e&amp;chksm=fa3f12e9cd489bff2aef57e2d0480760ac704825021a2f28d43c09f32fd6294efff46609bcbc#rd</t>
+  </si>
+  <si>
     <t>服务月｜密院12345：全新的权益反馈体验！</t>
   </si>
   <si>
@@ -286,15 +386,27 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185769&amp;idx=1&amp;sn=5b295c9a0f58b3af1dfa26dbfc2bb96e&amp;chksm=8bfc2451bc8bad4713a5663ff2713d51264add07d4b3ee37ca23ef1c928cb14edf8154193688#rd</t>
   </si>
   <si>
-    <t>人民日报评论部：敢于斗争、善于斗争——把青春播撒在民族复兴的征程上③</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486295&amp;idx=1&amp;sn=f14ac378113a19fd357d4e22f749d11e&amp;chksm=fa3f12e9cd489bff2aef57e2d0480760ac704825021a2f28d43c09f32fd6294efff46609bcbc#rd</t>
-  </si>
-  <si>
     <t>2022-05-25</t>
   </si>
   <si>
+    <t>【活动】密院“工转商”升学分享会预告</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moSNQpVcLYNa57WN3ufOeuCxzKbaO9RG8LEDw2CMnyPskCSe9l7D0atcDqdFwo19d8ibJQqiccG6VEHg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491710&amp;idx=1&amp;sn=6ef79f4599404bf731dc226397fd15cb&amp;chksm=ec0e096fdb7980791670c3ed17b9db99ea954ada8dd84baf686847744cf326207bff0c8ec3a0#rd</t>
+  </si>
+  <si>
+    <t>回顾｜研究生申请workshop for DDers</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMia2Qwiatd5dibItBUFVSeuQqwqp1vyia856ficIbNguV9FrDoRLKNbs5cGWXtwUQCaMu7GBng1YRib6c3A/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484415&amp;idx=1&amp;sn=871a6907a654ed93473a2b1e7ac3a19d&amp;chksm=fbeb9442cc9c1d544d442d36b2ef242e51fe30af501dfa88b7d2ad2f87383eb7b86a97137644#rd</t>
+  </si>
+  <si>
     <t>2022年毕业学生团员组织关系转接指引和问答，请查收！</t>
   </si>
   <si>
@@ -304,27 +416,24 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486292&amp;idx=1&amp;sn=e58d83d7d2be4d9857458ffce5bb4828&amp;chksm=fa3f12eacd489bfcd40d5a35729467cbe84fb2c2faa67ad3e4280946e4fae4938551b3528b42#rd</t>
   </si>
   <si>
-    <t>回顾｜研究生申请workshop for DDers</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMia2Qwiatd5dibItBUFVSeuQqwqp1vyia856ficIbNguV9FrDoRLKNbs5cGWXtwUQCaMu7GBng1YRib6c3A/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484415&amp;idx=1&amp;sn=871a6907a654ed93473a2b1e7ac3a19d&amp;chksm=fbeb9442cc9c1d544d442d36b2ef242e51fe30af501dfa88b7d2ad2f87383eb7b86a97137644#rd</t>
-  </si>
-  <si>
-    <t>【活动】密院“工转商”升学分享会预告</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moSNQpVcLYNa57WN3ufOeuCxzKbaO9RG8LEDw2CMnyPskCSe9l7D0atcDqdFwo19d8ibJQqiccG6VEHg/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491710&amp;idx=1&amp;sn=6ef79f4599404bf731dc226397fd15cb&amp;chksm=ec0e096fdb7980791670c3ed17b9db99ea954ada8dd84baf686847744cf326207bff0c8ec3a0#rd</t>
-  </si>
-  <si>
     <t>2022-05-24</t>
   </si>
   <si>
+    <t>人民日报评论部：理想远大、信念坚定——把青春播撒在民族复兴的征程上①</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486285&amp;idx=1&amp;sn=087e843ea5d9de4425b5eb981628854a&amp;chksm=fa3f12f3cd489be5f3d39f074ba02b13485ed3c61cbcae13b6dde4d016ac85a36208888e1e7b#rd</t>
+  </si>
+  <si>
+    <t>服务月 | 学生会活动策划体验小程序发布·舞会专场</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNF8oSW3NkPmUIUVnuj1eslVrp1gKNdXsicCsXZgwNc4OE4WqHbc815nGyCqXLM9wchR8t8FhHib6oZA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185750&amp;idx=1&amp;sn=aef0ae274678e64323612345555d502e&amp;chksm=8bfc246ebc8bad78e7f3b89409b106f6fc7afb97cdbb9d1275f5ee0a24588c8576c6d8ff58b9#rd</t>
+  </si>
+  <si>
     <t>换届通知 | 密院科协主席团及部长团换届通知</t>
   </si>
   <si>
@@ -334,21 +443,6 @@
     <t>http://mp.weixin.qq.com/s?__biz=MzIyMDA2ODgyNA==&amp;mid=2247488285&amp;idx=1&amp;sn=fc1faa055cdbc5c872aa4943d5cfacbb&amp;chksm=97d0fdaaa0a774bc7f6cf9f307cfe6d50d9142b998ec0a0994609d63804731d70bfb41290562#rd</t>
   </si>
   <si>
-    <t>服务月 | 学生会活动策划体验小程序发布·舞会专场</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNF8oSW3NkPmUIUVnuj1eslVrp1gKNdXsicCsXZgwNc4OE4WqHbc815nGyCqXLM9wchR8t8FhHib6oZA/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185750&amp;idx=1&amp;sn=aef0ae274678e64323612345555d502e&amp;chksm=8bfc246ebc8bad78e7f3b89409b106f6fc7afb97cdbb9d1275f5ee0a24588c8576c6d8ff58b9#rd</t>
-  </si>
-  <si>
-    <t>人民日报评论部：理想远大、信念坚定——把青春播撒在民族复兴的征程上①</t>
-  </si>
-  <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486285&amp;idx=1&amp;sn=087e843ea5d9de4425b5eb981628854a&amp;chksm=fa3f12f3cd489be5f3d39f074ba02b13485ed3c61cbcae13b6dde4d016ac85a36208888e1e7b#rd</t>
-  </si>
-  <si>
     <t>2022-05-23</t>
   </si>
   <si>
@@ -881,9 +975,6 @@
   </si>
   <si>
     <t>2021秋季招新|密院气象</t>
-  </si>
-  <si>
-    <t>密院气象</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/ic56fiaeKmYMAt8UlgIribsQqScjaR2tf2RLYdx8oEHliaNtJZBjGb94TjhRHk07CIAIXkQmNTOs4UticUgpdFuPtfg/0?wx_fmt=jpeg</t>
@@ -933,9 +1024,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -954,7 +1045,30 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -970,7 +1084,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -984,20 +1098,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1006,17 +1106,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1030,38 +1122,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1076,15 +1137,23 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1096,6 +1165,28 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1103,42 +1194,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1154,7 +1209,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1166,37 +1317,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1214,13 +1353,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1232,25 +1365,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1262,31 +1377,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1297,30 +1388,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1339,15 +1406,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1359,6 +1417,24 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1397,153 +1473,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1874,19 +1965,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A$1:F$1048576"/>
+      <selection activeCell="A1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
-  <cols>
-    <col min="1" max="1" width="10.3046875" style="1"/>
-    <col min="2" max="6" width="7.7734375" style="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1905,7 +1993,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>1655012637</v>
+        <v>1655373138</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1925,30 +2013,30 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>1654746363</v>
+        <v>1655340412</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>1654784264</v>
+        <v>1655258539</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>15</v>
@@ -1965,399 +2053,395 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>1654683827</v>
+        <v>1655254575</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>1654696237</v>
+        <v>1655174263</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>1654615201</v>
+        <v>1655168550</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>1654524315</v>
+        <v>1655130382</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>1654337062</v>
+        <v>1655082511</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>1654328621</v>
+        <v>1655043434</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
-        <v>1654228442</v>
+        <v>1655012637</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2">
-        <v>1654153902</v>
+        <v>1654784264</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2">
-        <v>1654091999</v>
+        <v>1654746363</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2">
-        <v>1653893676</v>
+        <v>1654696237</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2">
-        <v>1653918467</v>
+        <v>1654683827</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>1653915004</v>
+        <v>1654615201</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>1653809321</v>
+        <v>1654524315</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>1653756447</v>
+        <v>1654337062</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>1653734498</v>
+        <v>1654328621</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>1653752093</v>
+        <v>1654228442</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>1653661410</v>
+        <v>1654153902</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>1653655336</v>
+        <v>1654091999</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>1653560174</v>
+        <v>1653918467</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>1653566952</v>
+        <v>1653915004</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>91</v>
@@ -2365,36 +2449,36 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>1653455486</v>
+        <v>1653893676</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>1653457678</v>
+        <v>1653809321</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>96</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>97</v>
@@ -2405,16 +2489,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>1653488445</v>
+        <v>1653756447</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>100</v>
@@ -2425,7 +2509,7 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>1653358054</v>
+        <v>1653752093</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>102</v>
@@ -2434,7 +2518,7 @@
         <v>103</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>104</v>
@@ -2445,7 +2529,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>1653381370</v>
+        <v>1653734498</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>102</v>
@@ -2454,7 +2538,7 @@
         <v>106</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>107</v>
@@ -2465,39 +2549,39 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>1653400076</v>
+        <v>1653661410</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2">
-        <v>1653310453</v>
+        <v>1653655336</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>114</v>
@@ -2505,7 +2589,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>1653206327</v>
+        <v>1653566952</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>115</v>
@@ -2514,707 +2598,707 @@
         <v>116</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2">
-        <v>1653112956</v>
+        <v>1653560174</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2">
-        <v>1653106699</v>
+        <v>1653488445</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2">
-        <v>1653103833</v>
+        <v>1653457678</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2">
-        <v>1652946162</v>
+        <v>1653455486</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2">
-        <v>1652766746</v>
+        <v>1653400076</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2">
-        <v>1652711615</v>
+        <v>1653381370</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2">
-        <v>1652708097</v>
+        <v>1653358054</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2">
-        <v>1652633146</v>
+        <v>1653310453</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2">
-        <v>1652502015</v>
+        <v>1653206327</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2">
-        <v>1652423986</v>
+        <v>1653112956</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2">
-        <v>1652196254</v>
+        <v>1653106699</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2">
-        <v>1652156920</v>
+        <v>1653103833</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2">
-        <v>1652102252</v>
+        <v>1652946162</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2">
-        <v>1652082724</v>
+        <v>1652766746</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>162</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2">
-        <v>1652004475</v>
+        <v>1652711615</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2">
-        <v>1651989033</v>
+        <v>1652708097</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2">
-        <v>1651923024</v>
+        <v>1652633146</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2">
-        <v>1651902344</v>
+        <v>1652502015</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>176</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2">
-        <v>1651834916</v>
+        <v>1652423986</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2">
-        <v>1651834564</v>
+        <v>1652196254</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2">
-        <v>1651827827</v>
+        <v>1652156920</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2">
-        <v>1651827003</v>
+        <v>1652102252</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2">
-        <v>1651826605</v>
+        <v>1652082724</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2">
-        <v>1651820943</v>
+        <v>1652004475</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2">
-        <v>1651730520</v>
+        <v>1651989033</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>198</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>1651659154</v>
+        <v>1651923024</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2">
-        <v>1651654866</v>
+        <v>1651902344</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2">
-        <v>1651646933</v>
+        <v>1651834916</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2">
-        <v>1651644769</v>
+        <v>1651834564</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2">
-        <v>1651634414</v>
+        <v>1651827827</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2">
-        <v>1651633116</v>
+        <v>1651827003</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2">
-        <v>1651499797</v>
+        <v>1651826605</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E64" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F64" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2">
-        <v>1651487681</v>
+        <v>1651820943</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C65" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E65" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2">
-        <v>1651323746</v>
+        <v>1651730520</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="D66" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E66" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2">
-        <v>1651312543</v>
+        <v>1651659154</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>232</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>233</v>
@@ -3225,16 +3309,16 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2">
-        <v>1651295846</v>
+        <v>1651654866</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>235</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>236</v>
@@ -3245,342 +3329,522 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2">
-        <v>1651045196</v>
+        <v>1651646933</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E69" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2">
-        <v>1651038505</v>
+        <v>1651644769</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C70" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E70" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2">
-        <v>1651029491</v>
+        <v>1651634414</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C71" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E71" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2">
-        <v>1650938536</v>
+        <v>1651633116</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="F72" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2">
-        <v>1650877867</v>
+        <v>1651499797</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2">
-        <v>1650852390</v>
+        <v>1651487681</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C74" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2">
-        <v>1650701590</v>
+        <v>1651323746</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2">
-        <v>1650355221</v>
+        <v>1651312543</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F76" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2">
-        <v>1650113970</v>
+        <v>1651295846</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2">
-        <v>1649752200</v>
+        <v>1651045196</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="2">
-        <v>1649474737</v>
+        <v>1651038505</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2">
-        <v>1648656738</v>
+        <v>1651029491</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2">
-        <v>1648381501</v>
+        <v>1650938536</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2">
-        <v>1631875901</v>
+        <v>1650877867</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>289</v>
+        <v>16</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2">
-        <v>1626011329</v>
+        <v>1650852390</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>289</v>
+        <v>30</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2">
-        <v>1623555180</v>
+        <v>1650701590</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>289</v>
+        <v>39</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="2">
+        <v>1650355221</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="2">
+        <v>1650113970</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="2">
+        <v>1649752200</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="2">
+        <v>1649474737</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="2">
+        <v>1648656738</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="2">
+        <v>1648381501</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="2">
+        <v>1631875901</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="2">
+        <v>1626011329</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="2">
+        <v>1623555180</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="2">
         <v>1622215014</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>303</v>
+      <c r="B94" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2022-06-27 17:06:46
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397">
   <si>
     <t>发布日期</t>
   </si>
@@ -31,15 +31,228 @@
     <t>公众号链接</t>
   </si>
   <si>
+    <t>2022-06-27</t>
+  </si>
+  <si>
+    <t>6.27天气预报</t>
+  </si>
+  <si>
+    <t>密院气象</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/ic56fiaeKmYMA2iaA6K6ACfOFuoIvDicia2TdQxFCiazAibeGpAwwzDr4B1ugWvsictfflBdZTodl3SQg7rtLpDdPkaQFQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483759&amp;idx=1&amp;sn=59c119cfd995903f26bebeeaf6afec09&amp;chksm=c02ab875f75d3163d10f373df7948ca9272083b005f63f283734a7f8c7cb612c55491c8ded6c#rd</t>
+  </si>
+  <si>
+    <t>2022-06-26</t>
+  </si>
+  <si>
+    <t>服务月 | 你有3条来自professors的未读信息~</t>
+  </si>
+  <si>
+    <t>JIers</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNEBf8wgIofDAb1zVgncv1USjzbG9Ro4IC6bxxFFvnrhGNYm9fvwbibwKpXntMTT8NZ92iameJF80McA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651186001&amp;idx=1&amp;sn=a14f45ec76060c9fa10a70e82b17e2d2&amp;chksm=8bfc2569bc8bac7f8bde190472b37f14bc75d8ffd4686a19c2797fa74a9d75b628b6a8865fa0#rd</t>
+  </si>
+  <si>
+    <t>6.26天气预报</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483757&amp;idx=1&amp;sn=45664e41f99e08be3d5fc32b52520a1b&amp;chksm=c02ab877f75d3161c6645d4893a675b96551c2b5efef07e11cbff10396606e46bbde1aa30c77#rd</t>
+  </si>
+  <si>
+    <t>2022-06-25</t>
+  </si>
+  <si>
+    <t>回顾| “小班”一年 我的“关键词”</t>
+  </si>
+  <si>
+    <t>JI觅源</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5RjsOq84FtPg2NA4c4iaM3ZXrzzo8Oe4V6ShXYaCY04Sq9Zgkdw4uCNWQfeUtb1rAt0Ma87AFKJclg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzAwNTYxNzk3Mw==&amp;mid=2648011946&amp;idx=1&amp;sn=d6dcecce26443fd44136c1a5f4cc098a&amp;chksm=833834f0b44fbde6dff5a3f82c200ffafc40f2433f3ef83086a7786aa6d1c4a944a7f8fdb68b#rd</t>
+  </si>
+  <si>
+    <t>6.25天气预报</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483755&amp;idx=1&amp;sn=5e614c0aabaa4621a5efa623901d1d87&amp;chksm=c02ab871f75d316704d0868d3a8622b9b303c6a11b7532899595e5510609d0050abe631fc7c0#rd</t>
+  </si>
+  <si>
+    <t>2022-06-24</t>
+  </si>
+  <si>
+    <t>习近平同志《论党的青年工作》主要篇目介绍（一）</t>
+  </si>
+  <si>
+    <t>JI青团</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4DRAnrv3NOo57nTbRnjEel2BnM2iaf9eicv8GRAcDo34SXJUq04Cib8O1gx70dOA5wF2iam1XwPfo1gibg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486396&amp;idx=1&amp;sn=eecb131e6b41762ba8f3f33dc391fc8d&amp;chksm=fa3f1202cd489b1499acff193604d256f0dbd6d6ca92547effe8a8b30827c1620ca7e880a19e#rd</t>
+  </si>
+  <si>
+    <t>研究生申请&amp;生涯发展经验分享会 (3)</t>
+  </si>
+  <si>
+    <t>JIAdvisingCenter</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMiaQCneOUx6aF6qKqoRSHCF0Y8eQbiaWiczs0qwDFVb2w5WGFwBKrLPDuLjJJe5bfzAck7wTjEK9n0ow/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484465&amp;idx=1&amp;sn=af4876dcf59ef55c019643c5b0c2bbe2&amp;chksm=fbeb938ccc9c1a9a1019dda986ab6d5e9f3c0101980a73ff28f4ba8428dad20fe573b8511be3#rd</t>
+  </si>
+  <si>
+    <t>6.24天气预报</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483753&amp;idx=1&amp;sn=76a43909754e5dd4e407639764a0df22&amp;chksm=c02ab873f75d31659229700244b8745d96ce2c4dd77609b0b706bfc01c8dbc152a322ddc2684#rd</t>
+  </si>
+  <si>
+    <t>2022-06-23</t>
+  </si>
+  <si>
+    <t>6.23天气预报</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483751&amp;idx=1&amp;sn=bb072cfeb28f5018a12901de9c1a0912&amp;chksm=c02ab87df75d316ba8e36465ae076bcd2e9d06e079d67d9c66a1d1a4f22f7c3095c372d5301a#rd</t>
+  </si>
+  <si>
+    <t>2022-06-22</t>
+  </si>
+  <si>
+    <t>快来查收蓝虎新版动态表情包吧！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNFvLKo7nj6eia8qyWWalicu0k6SRmx17Nje8ibefYb3nfJicD4icohiaoUbCf1QyraRTRiaalIRDGJKCichaw/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185980&amp;idx=1&amp;sn=68795d12ca5df99a3f3fdab6b05f2982&amp;chksm=8bfc2504bc8bac12cdba5cdd5f77f21f541e145d5a464cbba780d338d119e721ed827539942e#rd</t>
+  </si>
+  <si>
+    <t>招募|小班招募</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5QqmYSZAibUyfFfPteIYPLdr3ibrCx0aPd2W5z5e1O3J2GMpBYH6ibz8HiaqvRskLJ93JwnLd3ia5o5SHg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzAwNTYxNzk3Mw==&amp;mid=2648011899&amp;idx=1&amp;sn=f520c5a26d769065839abf69fa934412&amp;chksm=83383421b44fbd3796c726453f0e91ed87c810bd3b4e6d1550b781cf3299274191787cfaf199#rd</t>
+  </si>
+  <si>
+    <t>2022-06-21</t>
+  </si>
+  <si>
+    <t>公示|“交阳似火”暑期社会实践团正式名单公示</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5S6IWXF61M3N8ibsuwYcibxbpiapLqRNca8Wibib836JficVpSQPul2Joficyrib0Em71fVXJPdxfnH7GV1Cg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzAwNTYxNzk3Mw==&amp;mid=2648011810&amp;idx=1&amp;sn=8f4e97069323eb968966c7184ad88519&amp;chksm=83383478b44fbd6eb57b2026b023199eb683d875b9bc2b49508ab0cb8b544a4ce5dbcebe202f#rd</t>
+  </si>
+  <si>
+    <t>2022-06-20</t>
+  </si>
+  <si>
+    <t>公示|“交阳似火”暑期社会实践团名单</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5R7fgSqrJpoQplicmpxOwSMNznmg6CQpW0bbUich5nK0O7UII4sNwccmIsiceJLjB6tSIB8RPtxiaddqg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzAwNTYxNzk3Mw==&amp;mid=2648011794&amp;idx=1&amp;sn=d0c71635512d2029050ce2d5b54cd3c8&amp;chksm=83383448b44fbd5e99e27efe0c07da5d0881ddcac3dbc5fbe1ede755268e7b15278fd9c096ac#rd</t>
+  </si>
+  <si>
+    <t>坚持做一件事是件很酷的事情，让我们一起做一个酷酷的仔~</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4BTa8hyibReYyHZ1UicS7dQ2J908lIuKhdRVQmYibMvboTaf6SLiax29klwqVPasrvO92Ye43nouFGkNg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486384&amp;idx=1&amp;sn=6f7486c21d04268e4e492e55dff63310&amp;chksm=fa3f120ecd489b189d96c3a30ebe4225a639335f33da36a82254614b83d73d1e5bd0b450eae6#rd</t>
+  </si>
+  <si>
+    <t>2022-06-19</t>
+  </si>
+  <si>
+    <t>服务月 | JIer的蓝虎live2D它来了！！！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNGPfh4fwEPUHkKcfkaQrp0fvhLxg6aiaAEsbUyoq6LFdwfPDH9MXKrMPLt9EvPFxvBkvINA1Dw70rw/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185975&amp;idx=1&amp;sn=d57927381e66db52f1e7ad2ba2e9b895&amp;chksm=8bfc250fbc8bac19eb73e4fd2c0db3739f2217e10715bbc9556abfd0966bdf90495a4e4b3748#rd</t>
+  </si>
+  <si>
+    <t>密西根学院毕尤一教授课题组招募“互联网+”大学生创新创业大赛项目成员</t>
+  </si>
+  <si>
+    <t>JIcareer</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moS1GGwCtJTMNWvica4cSxB456uEHV4jyJIuAnOGsuQaxtk4qj1TWrVQadfoBbRN9AsHmZRmOmmgRYQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491845&amp;idx=1&amp;sn=8f1a14a70249cf4b9d5ae5a9d9c6e840&amp;chksm=ec0e0814db7981029ac7f286c6b99f23f5035d2083ebee30337e15dd2d46bf45338c2b2fdee9#rd</t>
+  </si>
+  <si>
+    <t>服务月 | F.B.S. x Advising Center 让我们瞧瞧，是哪位JIer又emo了？</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMhNctykibiaibjhYyevuSiaGENA8twBic0YFIWSgIynwrzmzEnq8KMYVTqWm8aEWkgiaCtmsPMjgcibeLolA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484461&amp;idx=1&amp;sn=f6c4a45c0eb585e00d37c4f3fedd6ebf&amp;chksm=fbeb9390cc9c1a86d9de59446dd77d93e829b71c20326bda571de9c3e84bfd0c70c89454c760#rd</t>
+  </si>
+  <si>
+    <t>2022-06-18</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNHUiaTicwoVNXYiaIJnDByzJGib5K8mMonseLsLGibORJJzfTfRz4cVwIwS5a5zq6y4ia9Dic1RSEiax723XA/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185953&amp;idx=1&amp;sn=e9acf2d17cfde1ec64a09d291f2da0b5&amp;chksm=8bfc2519bc8bac0fc7a9d25ffa5901910722f085b9a292b35c4c623dabff4abe6a3e399acad2#rd</t>
+  </si>
+  <si>
+    <t>职场分享| 新能源车企体验经理&amp;互联网公司商业分析师</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moQp0xEL3BbQGSCKhKZxj4ib0eWacuaIJKWXcoMEazE21M98I9q62HOzsMUsgUhgGFsKv2TSyjgR68Q/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzI5MTcwMDg2Mg==&amp;mid=2247491837&amp;idx=1&amp;sn=ceae55436333a0146e8c711b0ed7498f&amp;chksm=ec0e09ecdb7980fa741034f09d0a112e063c2f701ab50208225cbb6f051767ef5e01c341cdea#rd</t>
+  </si>
+  <si>
+    <t>2022-06-17</t>
+  </si>
+  <si>
+    <t>服务月 | 盘点：如何避免提案咕咕？！</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNE1fVflw5icBTgZokiaIXBP1tC4XfjcY2oxa0hVnP0zBAyQp63ceKLv2wfFluRYY9LgXUSEU3LkVERg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651185936&amp;idx=1&amp;sn=b24837bf70080ad03e38711c664bd1c1&amp;chksm=8bfc2528bc8bac3ebe92b1ed0e3ea907e88458e87027eb605ba9aa34c73485c1a3fc7649d075#rd</t>
+  </si>
+  <si>
     <t>2022-06-16</t>
   </si>
   <si>
     <t>招募令|“交阳似火”暑期社会实践报名</t>
   </si>
   <si>
-    <t>JI觅源</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/5Y86fOG9o5RCBmHib6ooicpibUDm0Rbzp895WrfaWe7Bc2eZTwia4PsWVawcGTrm2xgqumGyFDoSGg5d1mSklH9FXQ/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -49,12 +262,6 @@
     <t>6.16天气预报</t>
   </si>
   <si>
-    <t>密院气象</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/ic56fiaeKmYMA2iaA6K6ACfOFuoIvDicia2TdQxFCiazAibeGpAwwzDr4B1ugWvsictfflBdZTodl3SQg7rtLpDdPkaQFQ/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
     <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483736&amp;idx=1&amp;sn=b1137ffd0cfd68e5794ca845d56c0e5f&amp;chksm=c02ab842f75d315459af6ed12611115b00580012cdf78a8f2c73126447577d53e7417dc70176#rd</t>
   </si>
   <si>
@@ -64,9 +271,6 @@
     <t>万般玩趣 | 召集令成果反馈！</t>
   </si>
   <si>
-    <t>JIers</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNGnOqjX9BBzhbkylTfN0TkGwLTianyqaCayPdYN8Rb89Re7CYTrMLeL7VicOBiafs9sibJafwTKQ1YOgA/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -104,9 +308,6 @@
   </si>
   <si>
     <t>叮咚，青年大学习来啦</t>
-  </si>
-  <si>
-    <t>JI青团</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4CuQBibeZ4MPQtYrgXu0ldplEmibzan1rd5XDULibnKfVueAuwL8C0oUXxPofibr8IWsiamvgeSyGFciaQw/0?wx_fmt=jpeg</t>
@@ -155,9 +356,6 @@
     <t>回顾｜研究生申请workshop for DDers (CE/EE/IOE专场)</t>
   </si>
   <si>
-    <t>JIAdvisingCenter</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMhfgY8NzZpoBjzaTTmvibAAlBuAOdoHrabH3E2nL8Y2HO6TErbticAprk0wqLLJtjjJZv4YlVDClAFA/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -222,9 +420,6 @@
   </si>
   <si>
     <t>职场分享| 新能源车企资深工程师&amp;半导体芯片公司架构师</t>
-  </si>
-  <si>
-    <t>JIcareer</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/PB5L45ia5moQp0xEL3BbQGSCKhKZxj4ib0victafib9wExzbQsicniaezM6XjanaFOjgHianDrO8kQzp1ezB8nhCb6KVw/0?wx_fmt=jpeg</t>
@@ -1024,10 +1219,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1044,37 +1239,6 @@
       <charset val="0"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -1084,7 +1248,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1098,8 +1262,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1115,14 +1294,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1131,6 +1303,21 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1153,7 +1340,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1167,7 +1354,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1181,8 +1368,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1197,7 +1392,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1209,7 +1500,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1221,163 +1566,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1388,6 +1583,50 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1421,59 +1660,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1488,153 +1674,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1965,10 +2160,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F1"/>
+      <selection activeCell="A1" sqref="A1:F114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1993,7 +2188,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>1655373138</v>
+        <v>1656291679</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -2013,70 +2208,70 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>1655340412</v>
+        <v>1656234516</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>1655258539</v>
+        <v>1656209902</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>1655254575</v>
+        <v>1656167460</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>1655174263</v>
+        <v>1656119323</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -2085,38 +2280,38 @@
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>1655168550</v>
+        <v>1656054385</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>1655130382</v>
+        <v>1656074997</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>29</v>
@@ -2133,25 +2328,27 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>1655082511</v>
+        <v>1656031420</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>1655043434</v>
+        <v>1655950244</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
@@ -2160,25 +2357,27 @@
         <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
-        <v>1655012637</v>
+        <v>1655870443</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>40</v>
@@ -2189,1076 +2388,1072 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2">
-        <v>1654784264</v>
+        <v>1655890058</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2">
-        <v>1654746363</v>
+        <v>1655793054</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2">
-        <v>1654696237</v>
+        <v>1655687671</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2">
-        <v>1654683827</v>
+        <v>1655734146</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>1654615201</v>
+        <v>1655648822</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>1654524315</v>
+        <v>1655602200</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>1654337062</v>
+        <v>1655627833</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>1654328621</v>
+        <v>1655543700</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>1654228442</v>
+        <v>1655546531</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>1654153902</v>
+        <v>1655440790</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>1654091999</v>
+        <v>1655373138</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>1653918467</v>
+        <v>1655340412</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>87</v>
+        <v>8</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>1653915004</v>
+        <v>1655258539</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>1653893676</v>
+        <v>1655254575</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>1653809321</v>
+        <v>1655174263</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>1653756447</v>
+        <v>1655168550</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>1653752093</v>
+        <v>1655130382</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>1653734498</v>
+        <v>1655082511</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>107</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E29" s="1"/>
       <c r="F29" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>1653661410</v>
+        <v>1655043434</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>111</v>
-      </c>
+      <c r="E30" s="1"/>
       <c r="F30" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2">
-        <v>1653655336</v>
+        <v>1655012637</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>1653566952</v>
+        <v>1654784264</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2">
-        <v>1653560174</v>
+        <v>1654746363</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2">
-        <v>1653488445</v>
+        <v>1654696237</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2">
-        <v>1653457678</v>
+        <v>1654683827</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="F35" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2">
-        <v>1653455486</v>
+        <v>1654615201</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2">
-        <v>1653400076</v>
+        <v>1654524315</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2">
-        <v>1653381370</v>
+        <v>1654337062</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>131</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2">
-        <v>1653358054</v>
+        <v>1654328621</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>131</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2">
-        <v>1653310453</v>
+        <v>1654228442</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2">
-        <v>1653206327</v>
+        <v>1654153902</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2">
-        <v>1653112956</v>
+        <v>1654091999</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2">
-        <v>1653106699</v>
+        <v>1653918467</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2">
-        <v>1653103833</v>
+        <v>1653915004</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2">
-        <v>1652946162</v>
+        <v>1653893676</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2">
-        <v>1652766746</v>
+        <v>1653809321</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2">
-        <v>1652711615</v>
+        <v>1653756447</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2">
-        <v>1652708097</v>
+        <v>1653752093</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2">
-        <v>1652633146</v>
+        <v>1653734498</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2">
-        <v>1652502015</v>
+        <v>1653661410</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2">
-        <v>1652423986</v>
+        <v>1653655336</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2">
-        <v>1652196254</v>
+        <v>1653566952</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2">
-        <v>1652156920</v>
+        <v>1653560174</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="F53" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2">
-        <v>1652102252</v>
+        <v>1653488445</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2">
-        <v>1652082724</v>
+        <v>1653457678</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F55" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2">
-        <v>1652004475</v>
+        <v>1653455486</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2">
-        <v>1651989033</v>
+        <v>1653400076</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>1651923024</v>
+        <v>1653381370</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2">
-        <v>1651902344</v>
+        <v>1653358054</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2">
-        <v>1651834916</v>
+        <v>1653310453</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2">
-        <v>1651834564</v>
+        <v>1653206327</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2">
-        <v>1651827827</v>
+        <v>1653112956</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2">
-        <v>1651827003</v>
+        <v>1653106699</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C63" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2">
-        <v>1651826605</v>
+        <v>1653103833</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2">
-        <v>1651820943</v>
+        <v>1652946162</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>224</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>225</v>
@@ -3269,7 +3464,7 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2">
-        <v>1651730520</v>
+        <v>1652766746</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>227</v>
@@ -3278,7 +3473,7 @@
         <v>228</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>229</v>
@@ -3289,7 +3484,7 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2">
-        <v>1651659154</v>
+        <v>1652711615</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>231</v>
@@ -3298,7 +3493,7 @@
         <v>232</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>233</v>
@@ -3309,7 +3504,7 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2">
-        <v>1651654866</v>
+        <v>1652708097</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>231</v>
@@ -3318,7 +3513,7 @@
         <v>235</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>236</v>
@@ -3329,7 +3524,7 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2">
-        <v>1651646933</v>
+        <v>1652633146</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>231</v>
@@ -3338,7 +3533,7 @@
         <v>238</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>239</v>
@@ -3349,279 +3544,279 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2">
-        <v>1651644769</v>
+        <v>1652502015</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2">
-        <v>1651634414</v>
+        <v>1652423986</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2">
-        <v>1651633116</v>
+        <v>1652196254</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2">
-        <v>1651499797</v>
+        <v>1652156920</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2">
-        <v>1651487681</v>
+        <v>1652102252</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2">
-        <v>1651323746</v>
+        <v>1652082724</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2">
-        <v>1651312543</v>
+        <v>1652004475</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2">
-        <v>1651295846</v>
+        <v>1651989033</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2">
-        <v>1651045196</v>
+        <v>1651923024</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="2">
-        <v>1651038505</v>
+        <v>1651902344</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2">
-        <v>1651029491</v>
+        <v>1651834916</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2">
-        <v>1650938536</v>
+        <v>1651834564</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>277</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2">
-        <v>1650877867</v>
+        <v>1651827827</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2">
-        <v>1650852390</v>
+        <v>1651827003</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C83" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>287</v>
@@ -3629,222 +3824,622 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2">
-        <v>1650701590</v>
+        <v>1651826605</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F84" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="2">
-        <v>1650355221</v>
+        <v>1651820943</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="2">
-        <v>1650113970</v>
+        <v>1651730520</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="2">
-        <v>1649752200</v>
+        <v>1651659154</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2">
-        <v>1649474737</v>
+        <v>1651654866</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="2">
-        <v>1648656738</v>
+        <v>1651646933</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="2">
-        <v>1648381501</v>
+        <v>1651644769</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2">
-        <v>1631875901</v>
+        <v>1651634414</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2">
-        <v>1626011329</v>
+        <v>1651633116</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="2">
-        <v>1623555180</v>
+        <v>1651499797</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="2">
+        <v>1651487681</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="2">
+        <v>1651323746</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="2">
+        <v>1651312543</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="2">
+        <v>1651295846</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="2">
+        <v>1651045196</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="2">
+        <v>1651038505</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="2">
+        <v>1651029491</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="2">
+        <v>1650938536</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="2">
+        <v>1650877867</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="2">
+        <v>1650852390</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="2">
+        <v>1650701590</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="2">
+        <v>1650355221</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="2">
+        <v>1650113970</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="2">
+        <v>1649752200</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="2">
+        <v>1649474737</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="2">
+        <v>1648656738</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="2">
+        <v>1648381501</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="2">
+        <v>1631875901</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="2">
+        <v>1626011329</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="2">
+        <v>1623555180</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="2">
         <v>1622215014</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>331</v>
+      <c r="B114" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2022-06-28 18:04:51
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11840"/>
+    <workbookView windowWidth="21080" windowHeight="11840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409">
   <si>
     <t>发布日期</t>
   </si>
@@ -31,30 +31,72 @@
     <t>公众号链接</t>
   </si>
   <si>
+    <t>2022-06-28</t>
+  </si>
+  <si>
+    <t>服务月 | 学生会活动策划体验小程序更新啦·院长见面会专场</t>
+  </si>
+  <si>
+    <t>JIers</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNEibycYfZHhibXBUXGxUeialpfh46oibNnrA0K7O38v25UECibWUHHKOEgVZUyuMDKENthBcIlyB2khbtg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA5MDMyMTc1MQ==&amp;mid=2651186043&amp;idx=1&amp;sn=dc918e179e545dfcf2e48b4c896e39d3&amp;chksm=8bfc2543bc8bac55eb4e03ee715ab47ac4dd200f90d051759fb2c664f5d8ad0b32928c1c5a6c#rd</t>
+  </si>
+  <si>
+    <t>6.28天气预报</t>
+  </si>
+  <si>
+    <t>密院气象</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/ic56fiaeKmYMA2iaA6K6ACfOFuoIvDicia2TdQxFCiazAibeGpAwwzDr4B1ugWvsictfflBdZTodl3SQg7rtLpDdPkaQFQ/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483761&amp;idx=1&amp;sn=18ee54a6776700870b55c018a4cfc428&amp;chksm=c02ab86bf75d317dee4df488e2fecedcfd4a088d4d6557fa7667b93f770b646e62a3f1f36af3#rd</t>
+  </si>
+  <si>
     <t>2022-06-27</t>
   </si>
   <si>
     <t>6.27天气预报</t>
   </si>
   <si>
-    <t>密院气象</t>
-  </si>
-  <si>
-    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/ic56fiaeKmYMA2iaA6K6ACfOFuoIvDicia2TdQxFCiazAibeGpAwwzDr4B1ugWvsictfflBdZTodl3SQg7rtLpDdPkaQFQ/0?wx_fmt=jpeg</t>
-  </si>
-  <si>
     <t>http://mp.weixin.qq.com/s?__biz=Mzg5MzYyODUzMw==&amp;mid=2247483759&amp;idx=1&amp;sn=59c119cfd995903f26bebeeaf6afec09&amp;chksm=c02ab875f75d3163d10f373df7948ca9272083b005f63f283734a7f8c7cb612c55491c8ded6c#rd</t>
   </si>
   <si>
+    <t>上周错过咖啡的快乐，这次奶茶给你补上！大学习放暑假啦~</t>
+  </si>
+  <si>
+    <t>JI青团</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4Da27cicUSFryFebTa1N8icqniaaEhQHfiadicv6nFWDiclvForrDw68ccu8ewAO5bdR5nBRGPicrWicEdo0Q/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzUyMzMyNTY0OQ==&amp;mid=2247486438&amp;idx=1&amp;sn=2abf9efb94fbc91153cb4d95c3fa7f87&amp;chksm=fa3f1258cd489b4e238b7409850dd6a4c8e8a92f6bd0cae92aa0f894e3ee519915d948ccfdb0#rd</t>
+  </si>
+  <si>
+    <t>服务月 | F.B.S. x Advising Center·请查收JIer的抗emo干货宝典</t>
+  </si>
+  <si>
+    <t>JIAdvisingCenter</t>
+  </si>
+  <si>
+    <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMjmDvpmnp9R25ia5CjaKibPy2HV43sVor0GYwrlicbyc10JDjLnIzyQ1GKHF891LGEzVKCFuAeviapuxg/0?wx_fmt=jpeg</t>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzU1Mzk2MDE0Ng==&amp;mid=2247484489&amp;idx=1&amp;sn=c1b067bdeaf8c928cfceb49e3a992110&amp;chksm=fbeb93f4cc9c1ae2ea89d0a4a36ffa86a80339489601292f10683a02fe1ea881950a7e8c4537#rd</t>
+  </si>
+  <si>
     <t>2022-06-26</t>
   </si>
   <si>
     <t>服务月 | 你有3条来自professors的未读信息~</t>
   </si>
   <si>
-    <t>JIers</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/sZvUJ5A0zNEBf8wgIofDAb1zVgncv1USjzbG9Ro4IC6bxxFFvnrhGNYm9fvwbibwKpXntMTT8NZ92iameJF80McA/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -94,9 +136,6 @@
     <t>习近平同志《论党的青年工作》主要篇目介绍（一）</t>
   </si>
   <si>
-    <t>JI青团</t>
-  </si>
-  <si>
     <t>https://mmbiz.qlogo.cn/mmbiz_jpg/QfDapvG9u4DRAnrv3NOo57nTbRnjEel2BnM2iaf9eicv8GRAcDo34SXJUq04Cib8O1gx70dOA5wF2iam1XwPfo1gibg/0?wx_fmt=jpeg</t>
   </si>
   <si>
@@ -104,9 +143,6 @@
   </si>
   <si>
     <t>研究生申请&amp;生涯发展经验分享会 (3)</t>
-  </si>
-  <si>
-    <t>JIAdvisingCenter</t>
   </si>
   <si>
     <t>https://mmbiz.qlogo.cn/sz_mmbiz_jpg/vibN6sMP6fMiaQCneOUx6aF6qKqoRSHCF0Y8eQbiaWiczs0qwDFVb2w5WGFwBKrLPDuLjJJe5bfzAck7wTjEK9n0ow/0?wx_fmt=jpeg</t>
@@ -1219,10 +1255,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1241,52 +1277,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1300,47 +1290,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1360,9 +1311,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1370,7 +1328,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1382,6 +1347,77 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1389,6 +1425,126 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1404,7 +1560,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1416,25 +1572,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1446,73 +1596,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1524,55 +1608,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1589,17 +1625,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1621,6 +1678,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1630,17 +1696,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1659,177 +1719,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2160,10 +2196,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F114"/>
+      <selection activeCell="A1" sqref="A1:F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2188,7 +2224,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>1656291679</v>
+        <v>1656348218</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -2208,39 +2244,39 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>1656234516</v>
+        <v>1656377807</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>1656209902</v>
+        <v>1656291679</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>16</v>
@@ -2248,56 +2284,56 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>1656167460</v>
+        <v>1656341354</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>1656119323</v>
+        <v>1656330921</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>1656054385</v>
+        <v>1656234516</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>27</v>
@@ -2308,59 +2344,59 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>1656074997</v>
+        <v>1656209902</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>1656031420</v>
+        <v>1656167460</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>1655950244</v>
+        <v>1656119323</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>37</v>
@@ -2368,7 +2404,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
-        <v>1655870443</v>
+        <v>1656054385</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>38</v>
@@ -2377,7 +2413,7 @@
         <v>39</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>40</v>
@@ -2388,7 +2424,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2">
-        <v>1655890058</v>
+        <v>1656074997</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>38</v>
@@ -2397,7 +2433,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>43</v>
@@ -2408,259 +2444,259 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2">
-        <v>1655793054</v>
+        <v>1656031420</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2">
-        <v>1655687671</v>
+        <v>1655950244</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2">
-        <v>1655734146</v>
+        <v>1655870443</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>1655648822</v>
+        <v>1655890058</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>1655602200</v>
+        <v>1655793054</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>1655627833</v>
+        <v>1655687671</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>1655543700</v>
+        <v>1655734146</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>1655546531</v>
+        <v>1655648822</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>1655440790</v>
+        <v>1655602200</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>1655373138</v>
+        <v>1655627833</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>1655340412</v>
+        <v>1655543700</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>1655258539</v>
+        <v>1655546531</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>1655254575</v>
+        <v>1655440790</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>88</v>
@@ -2668,7 +2704,7 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>1655174263</v>
+        <v>1655373138</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>89</v>
@@ -2677,7 +2713,7 @@
         <v>90</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>91</v>
@@ -2688,7 +2724,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>1655168550</v>
+        <v>1655340412</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>89</v>
@@ -2697,506 +2733,506 @@
         <v>93</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>1655130382</v>
+        <v>1655258539</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>1655082511</v>
+        <v>1655254575</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>1655043434</v>
+        <v>1655174263</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="1"/>
       <c r="F30" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2">
-        <v>1655012637</v>
+        <v>1655168550</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>105</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>1654784264</v>
+        <v>1655130382</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2">
-        <v>1654746363</v>
+        <v>1655082511</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2">
-        <v>1654696237</v>
+        <v>1655043434</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2">
-        <v>1654683827</v>
+        <v>1655012637</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2">
-        <v>1654615201</v>
+        <v>1654784264</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2">
-        <v>1654524315</v>
+        <v>1654746363</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2">
-        <v>1654337062</v>
+        <v>1654696237</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2">
-        <v>1654328621</v>
+        <v>1654683827</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2">
-        <v>1654228442</v>
+        <v>1654615201</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2">
-        <v>1654153902</v>
+        <v>1654524315</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2">
-        <v>1654091999</v>
+        <v>1654337062</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2">
-        <v>1653918467</v>
+        <v>1654328621</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2">
-        <v>1653915004</v>
+        <v>1654228442</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2">
-        <v>1653893676</v>
+        <v>1654153902</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2">
-        <v>1653809321</v>
+        <v>1654091999</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2">
-        <v>1653756447</v>
+        <v>1653918467</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E47" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2">
-        <v>1653752093</v>
+        <v>1653915004</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2">
-        <v>1653734498</v>
+        <v>1653893676</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2">
-        <v>1653661410</v>
+        <v>1653809321</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2">
-        <v>1653655336</v>
+        <v>1653756447</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2">
-        <v>1653566952</v>
+        <v>1653752093</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>182</v>
@@ -3204,16 +3240,16 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2">
-        <v>1653560174</v>
+        <v>1653734498</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>183</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>184</v>
@@ -3224,7 +3260,7 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2">
-        <v>1653488445</v>
+        <v>1653661410</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>186</v>
@@ -3233,7 +3269,7 @@
         <v>187</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>188</v>
@@ -3244,7 +3280,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2">
-        <v>1653457678</v>
+        <v>1653655336</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>186</v>
@@ -3253,67 +3289,67 @@
         <v>190</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E55" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2">
-        <v>1653455486</v>
+        <v>1653566952</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>193</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E56" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2">
-        <v>1653400076</v>
+        <v>1653560174</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>1653381370</v>
+        <v>1653488445</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>199</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>200</v>
@@ -3324,16 +3360,16 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2">
-        <v>1653358054</v>
+        <v>1653457678</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>202</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>106</v>
+        <v>22</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>203</v>
@@ -3344,559 +3380,559 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2">
-        <v>1653310453</v>
+        <v>1653455486</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E60" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2">
-        <v>1653206327</v>
+        <v>1653400076</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2">
-        <v>1653112956</v>
+        <v>1653381370</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2">
-        <v>1653106699</v>
+        <v>1653358054</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2">
-        <v>1653103833</v>
+        <v>1653310453</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C64" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F64" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2">
-        <v>1652946162</v>
+        <v>1653206327</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2">
-        <v>1652766746</v>
+        <v>1653112956</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2">
-        <v>1652711615</v>
+        <v>1653106699</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2">
-        <v>1652708097</v>
+        <v>1653103833</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2">
-        <v>1652633146</v>
+        <v>1652946162</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C69" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2">
-        <v>1652502015</v>
+        <v>1652766746</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2">
-        <v>1652423986</v>
+        <v>1652711615</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2">
-        <v>1652196254</v>
+        <v>1652708097</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2">
-        <v>1652156920</v>
+        <v>1652633146</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2">
-        <v>1652102252</v>
+        <v>1652502015</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2">
-        <v>1652082724</v>
+        <v>1652423986</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2">
-        <v>1652004475</v>
+        <v>1652196254</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2">
-        <v>1651989033</v>
+        <v>1652156920</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2">
-        <v>1651923024</v>
+        <v>1652102252</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="2">
-        <v>1651902344</v>
+        <v>1652082724</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F79" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2">
-        <v>1651834916</v>
+        <v>1652004475</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2">
-        <v>1651834564</v>
+        <v>1651989033</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C81" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2">
-        <v>1651827827</v>
+        <v>1651923024</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="C82" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E82" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E82" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2">
-        <v>1651827003</v>
+        <v>1651902344</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2">
-        <v>1651826605</v>
+        <v>1651834916</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="2">
-        <v>1651820943</v>
+        <v>1651834564</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="2">
-        <v>1651730520</v>
+        <v>1651827827</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="2">
-        <v>1651659154</v>
+        <v>1651827003</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="D87" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>298</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>299</v>
@@ -3904,76 +3940,76 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2">
-        <v>1651654866</v>
+        <v>1651826605</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="D88" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="2">
-        <v>1651646933</v>
+        <v>1651820943</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C89" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F89" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="2">
-        <v>1651644769</v>
+        <v>1651730520</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="C90" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E90" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>307</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2">
-        <v>1651634414</v>
+        <v>1651659154</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>309</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>310</v>
@@ -3984,16 +4020,16 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2">
-        <v>1651633116</v>
+        <v>1651654866</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>312</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>313</v>
@@ -4004,442 +4040,522 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="2">
-        <v>1651499797</v>
+        <v>1651646933</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="D93" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E93" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="2">
-        <v>1651487681</v>
+        <v>1651644769</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C94" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E94" s="2" t="s">
+      <c r="F94" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="2">
-        <v>1651323746</v>
+        <v>1651634414</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E95" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="F95" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="2">
-        <v>1651312543</v>
+        <v>1651633116</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="C96" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F96" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="2">
-        <v>1651295846</v>
+        <v>1651499797</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="C97" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E97" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D97" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E97" s="2" t="s">
+      <c r="F97" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="2">
-        <v>1651045196</v>
+        <v>1651487681</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E98" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="F98" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="2">
-        <v>1651038505</v>
+        <v>1651323746</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C99" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E99" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E99" s="2" t="s">
+      <c r="F99" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="2">
-        <v>1651029491</v>
+        <v>1651312543</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C100" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="D100" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E100" s="2" t="s">
+      <c r="F100" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="2">
-        <v>1650938536</v>
+        <v>1651295846</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E101" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="F101" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="2">
-        <v>1650877867</v>
+        <v>1651045196</v>
       </c>
       <c r="B102" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="F102" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="2">
-        <v>1650852390</v>
+        <v>1651038505</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C103" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="F103" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="2">
-        <v>1650701590</v>
+        <v>1651029491</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="F104" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="2">
-        <v>1650355221</v>
+        <v>1650938536</v>
       </c>
       <c r="B105" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="2">
-        <v>1650113970</v>
+        <v>1650877867</v>
       </c>
       <c r="B106" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="F106" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="2">
-        <v>1649752200</v>
+        <v>1650852390</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="2">
-        <v>1649474737</v>
+        <v>1650701590</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="2">
-        <v>1648656738</v>
+        <v>1650355221</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="2">
-        <v>1648381501</v>
+        <v>1650113970</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="2">
-        <v>1631875901</v>
+        <v>1649752200</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="2">
-        <v>1626011329</v>
+        <v>1649474737</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" s="2">
-        <v>1623555180</v>
+        <v>1648656738</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" s="2">
+        <v>1648381501</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="2">
+        <v>1631875901</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="2">
+        <v>1626011329</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="2">
+        <v>1623555180</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="2">
         <v>1622215014</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>396</v>
+      <c r="B118" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>